<commit_message>
Completed sections 7 & 8
</commit_message>
<xml_diff>
--- a/Unity Certification Course (Udemy) - Video Listing.xlsx
+++ b/Unity Certification Course (Udemy) - Video Listing.xlsx
@@ -4804,8 +4804,8 @@
   <dimension ref="A1:J246"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>
+      <pane ySplit="3" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G107" sqref="G107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -4833,15 +4833,15 @@
       </c>
       <c r="F1" s="34">
         <f>SUMIF(G4:G244, "&gt;0", C4:C244)</f>
-        <v>409</v>
+        <v>566</v>
       </c>
       <c r="G1" s="35">
         <f>+C245</f>
-        <v>1336</v>
+        <v>1304</v>
       </c>
       <c r="H1" s="36">
         <f>+F1/G1</f>
-        <v>0.30613772455089822</v>
+        <v>0.43404907975460122</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -4852,7 +4852,7 @@
       <c r="C2" s="4"/>
       <c r="G2" s="38">
         <f>+G1/60</f>
-        <v>22.266666666666666</v>
+        <v>21.733333333333334</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="45.75" thickBot="1">
@@ -4912,7 +4912,7 @@
       </c>
       <c r="F5" s="15">
         <f>F4+(C5/$C$245)</f>
-        <v>1.4970059880239522E-3</v>
+        <v>1.5337423312883436E-3</v>
       </c>
       <c r="G5" s="30">
         <v>42789</v>
@@ -4943,7 +4943,7 @@
       </c>
       <c r="F6" s="15">
         <f t="shared" ref="F6:F69" si="2">F5+(C6/$C$245)</f>
-        <v>2.9940119760479044E-3</v>
+        <v>3.0674846625766872E-3</v>
       </c>
       <c r="G6" s="30">
         <v>42789</v>
@@ -4974,7 +4974,7 @@
       </c>
       <c r="F7" s="15">
         <f t="shared" si="2"/>
-        <v>8.2335329341317355E-3</v>
+        <v>8.4355828220858894E-3</v>
       </c>
       <c r="G7" s="30">
         <v>42789</v>
@@ -5005,7 +5005,7 @@
       </c>
       <c r="F8" s="15">
         <f t="shared" si="2"/>
-        <v>1.1976047904191616E-2</v>
+        <v>1.2269938650306749E-2</v>
       </c>
       <c r="G8" s="30">
         <v>42789</v>
@@ -5035,7 +5035,7 @@
       <c r="E9" s="27"/>
       <c r="F9" s="29">
         <f t="shared" si="2"/>
-        <v>1.1976047904191616E-2</v>
+        <v>1.2269938650306749E-2</v>
       </c>
       <c r="G9" s="41" t="str">
         <f>IF(COUNTA(G10:G32)=COUNTA(B10:B32), "COMPLETE", "")</f>
@@ -5067,7 +5067,7 @@
       </c>
       <c r="F10" s="15">
         <f t="shared" si="2"/>
-        <v>1.2724550898203593E-2</v>
+        <v>1.3036809815950921E-2</v>
       </c>
       <c r="G10" s="30">
         <v>42789</v>
@@ -5098,7 +5098,7 @@
       </c>
       <c r="F11" s="15">
         <f t="shared" si="2"/>
-        <v>1.6467065868263471E-2</v>
+        <v>1.6871165644171779E-2</v>
       </c>
       <c r="G11" s="30">
         <v>42789</v>
@@ -5129,7 +5129,7 @@
       </c>
       <c r="F12" s="15">
         <f t="shared" si="2"/>
-        <v>2.3203592814371257E-2</v>
+        <v>2.3773006134969327E-2</v>
       </c>
       <c r="G12" s="30">
         <v>42789</v>
@@ -5160,7 +5160,7 @@
       </c>
       <c r="F13" s="15">
         <f t="shared" si="2"/>
-        <v>2.5449101796407185E-2</v>
+        <v>2.6073619631901843E-2</v>
       </c>
       <c r="G13" s="30">
         <v>42789</v>
@@ -5191,7 +5191,7 @@
       </c>
       <c r="F14" s="15">
         <f t="shared" si="2"/>
-        <v>2.9940119760479042E-2</v>
+        <v>3.0674846625766874E-2</v>
       </c>
       <c r="G14" s="30">
         <v>42789</v>
@@ -5222,7 +5222,7 @@
       </c>
       <c r="F15" s="15">
         <f t="shared" si="2"/>
-        <v>3.2185628742514967E-2</v>
+        <v>3.297546012269939E-2</v>
       </c>
       <c r="G15" s="30">
         <v>42789</v>
@@ -5253,7 +5253,7 @@
       </c>
       <c r="F16" s="15">
         <f t="shared" si="2"/>
-        <v>4.1167664670658681E-2</v>
+        <v>4.2177914110429454E-2</v>
       </c>
       <c r="G16" s="30">
         <v>42789</v>
@@ -5284,7 +5284,7 @@
       </c>
       <c r="F17" s="15">
         <f t="shared" si="2"/>
-        <v>4.3413173652694606E-2</v>
+        <v>4.447852760736197E-2</v>
       </c>
       <c r="G17" s="30">
         <v>42789</v>
@@ -5315,7 +5315,7 @@
       </c>
       <c r="F18" s="15">
         <f t="shared" si="2"/>
-        <v>5.0149700598802388E-2</v>
+        <v>5.1380368098159518E-2</v>
       </c>
       <c r="G18" s="30">
         <v>42789</v>
@@ -5346,7 +5346,7 @@
       </c>
       <c r="F19" s="15">
         <f t="shared" si="2"/>
-        <v>5.2395209580838313E-2</v>
+        <v>5.3680981595092034E-2</v>
       </c>
       <c r="G19" s="30">
         <v>42789</v>
@@ -5377,7 +5377,7 @@
       </c>
       <c r="F20" s="15">
         <f t="shared" si="2"/>
-        <v>5.538922155688622E-2</v>
+        <v>5.6748466257668724E-2</v>
       </c>
       <c r="G20" s="30">
         <v>42789</v>
@@ -5408,7 +5408,7 @@
       </c>
       <c r="F21" s="15">
         <f t="shared" si="2"/>
-        <v>5.7634730538922145E-2</v>
+        <v>5.904907975460124E-2</v>
       </c>
       <c r="G21" s="30">
         <v>42789</v>
@@ -5439,7 +5439,7 @@
       </c>
       <c r="F22" s="15">
         <f t="shared" si="2"/>
-        <v>6.3622754491017952E-2</v>
+        <v>6.5184049079754613E-2</v>
       </c>
       <c r="G22" s="30">
         <v>42789</v>
@@ -5470,7 +5470,7 @@
       </c>
       <c r="F23" s="15">
         <f t="shared" si="2"/>
-        <v>6.5868263473053884E-2</v>
+        <v>6.7484662576687129E-2</v>
       </c>
       <c r="G23" s="30">
         <v>42789</v>
@@ -5501,7 +5501,7 @@
       </c>
       <c r="F24" s="15">
         <f t="shared" si="2"/>
-        <v>7.559880239520958E-2</v>
+        <v>7.7453987730061361E-2</v>
       </c>
       <c r="G24" s="30">
         <v>42789</v>
@@ -5532,7 +5532,7 @@
       </c>
       <c r="F25" s="15">
         <f t="shared" si="2"/>
-        <v>7.7844311377245512E-2</v>
+        <v>7.9754601226993876E-2</v>
       </c>
       <c r="G25" s="30">
         <v>42789</v>
@@ -5563,7 +5563,7 @@
       </c>
       <c r="F26" s="15">
         <f t="shared" si="2"/>
-        <v>8.4580838323353294E-2</v>
+        <v>8.6656441717791424E-2</v>
       </c>
       <c r="G26" s="30">
         <v>42789</v>
@@ -5594,7 +5594,7 @@
       </c>
       <c r="F27" s="15">
         <f t="shared" si="2"/>
-        <v>8.6826347305389226E-2</v>
+        <v>8.895705521472394E-2</v>
       </c>
       <c r="G27" s="30">
         <v>42789</v>
@@ -5625,7 +5625,7 @@
       </c>
       <c r="F28" s="15">
         <f t="shared" si="2"/>
-        <v>9.580838323353294E-2</v>
+        <v>9.8159509202454004E-2</v>
       </c>
       <c r="G28" s="30">
         <v>42789</v>
@@ -5656,7 +5656,7 @@
       </c>
       <c r="F29" s="15">
         <f t="shared" si="2"/>
-        <v>9.8053892215568872E-2</v>
+        <v>0.10046012269938652</v>
       </c>
       <c r="G29" s="30">
         <v>42789</v>
@@ -5687,7 +5687,7 @@
       </c>
       <c r="F30" s="15">
         <f t="shared" si="2"/>
-        <v>9.8802395209580854E-2</v>
+        <v>0.10122699386503069</v>
       </c>
       <c r="G30" s="30">
         <v>42789</v>
@@ -5718,7 +5718,7 @@
       </c>
       <c r="F31" s="15">
         <f t="shared" si="2"/>
-        <v>0.10104790419161679</v>
+        <v>0.1035276073619632</v>
       </c>
       <c r="G31" s="30">
         <v>42789</v>
@@ -5749,7 +5749,7 @@
       </c>
       <c r="F32" s="15">
         <f t="shared" si="2"/>
-        <v>0.10179640718562877</v>
+        <v>0.10429447852760737</v>
       </c>
       <c r="G32" s="30">
         <v>42789</v>
@@ -5779,7 +5779,7 @@
       <c r="E33" s="27"/>
       <c r="F33" s="29">
         <f t="shared" si="2"/>
-        <v>0.10179640718562877</v>
+        <v>0.10429447852760737</v>
       </c>
       <c r="G33" s="41" t="str">
         <f>IF(COUNTA(G34:G40)=COUNTA(B34:B40), "COMPLETE", "")</f>
@@ -5811,7 +5811,7 @@
       </c>
       <c r="F34" s="15">
         <f t="shared" si="2"/>
-        <v>0.10254491017964075</v>
+        <v>0.10506134969325154</v>
       </c>
       <c r="G34" s="30">
         <v>42790</v>
@@ -5842,7 +5842,7 @@
       </c>
       <c r="F35" s="15">
         <f t="shared" si="2"/>
-        <v>0.11152694610778446</v>
+        <v>0.1142638036809816</v>
       </c>
       <c r="G35" s="30">
         <v>42791</v>
@@ -5873,7 +5873,7 @@
       </c>
       <c r="F36" s="15">
         <f t="shared" si="2"/>
-        <v>0.1137724550898204</v>
+        <v>0.11656441717791412</v>
       </c>
       <c r="G36" s="30">
         <v>42791</v>
@@ -5904,7 +5904,7 @@
       </c>
       <c r="F37" s="15">
         <f t="shared" si="2"/>
-        <v>0.12125748502994016</v>
+        <v>0.12423312883435583</v>
       </c>
       <c r="G37" s="30">
         <v>42791</v>
@@ -5935,7 +5935,7 @@
       </c>
       <c r="F38" s="15">
         <f t="shared" si="2"/>
-        <v>0.12350299401197609</v>
+        <v>0.12653374233128833</v>
       </c>
       <c r="G38" s="30">
         <v>42791</v>
@@ -5966,7 +5966,7 @@
       </c>
       <c r="F39" s="15">
         <f t="shared" si="2"/>
-        <v>0.13173652694610782</v>
+        <v>0.13496932515337423</v>
       </c>
       <c r="G39" s="30">
         <v>42791</v>
@@ -5997,7 +5997,7 @@
       </c>
       <c r="F40" s="15">
         <f t="shared" si="2"/>
-        <v>0.13398203592814376</v>
+        <v>0.13726993865030673</v>
       </c>
       <c r="G40" s="30">
         <v>42791</v>
@@ -6027,7 +6027,7 @@
       <c r="E41" s="27"/>
       <c r="F41" s="29">
         <f t="shared" si="2"/>
-        <v>0.13398203592814376</v>
+        <v>0.13726993865030673</v>
       </c>
       <c r="G41" s="41" t="str">
         <f>IF(COUNTA(G42:G45)=COUNTA(B42:B45), "COMPLETE", "")</f>
@@ -6059,7 +6059,7 @@
       </c>
       <c r="F42" s="15">
         <f t="shared" si="2"/>
-        <v>0.14371257485029945</v>
+        <v>0.14723926380368096</v>
       </c>
       <c r="G42" s="30">
         <v>42791</v>
@@ -6090,7 +6090,7 @@
       </c>
       <c r="F43" s="15">
         <f t="shared" si="2"/>
-        <v>0.14595808383233538</v>
+        <v>0.14953987730061347</v>
       </c>
       <c r="G43" s="30">
         <v>42791</v>
@@ -6121,7 +6121,7 @@
       </c>
       <c r="F44" s="15">
         <f t="shared" si="2"/>
-        <v>0.15643712574850305</v>
+        <v>0.16027607361963186</v>
       </c>
       <c r="G44" s="30">
         <v>42791</v>
@@ -6152,7 +6152,7 @@
       </c>
       <c r="F45" s="15">
         <f t="shared" si="2"/>
-        <v>0.15868263473053898</v>
+        <v>0.16257668711656437</v>
       </c>
       <c r="G45" s="30">
         <v>42791</v>
@@ -6182,7 +6182,7 @@
       <c r="E46" s="27"/>
       <c r="F46" s="29">
         <f t="shared" si="2"/>
-        <v>0.15868263473053898</v>
+        <v>0.16257668711656437</v>
       </c>
       <c r="G46" s="41" t="str">
         <f>IF(COUNTA(G47:G60)=COUNTA(B47:B60), "COMPLETE", "")</f>
@@ -6214,7 +6214,7 @@
       </c>
       <c r="F47" s="15">
         <f t="shared" si="2"/>
-        <v>0.15943113772455095</v>
+        <v>0.16334355828220853</v>
       </c>
       <c r="G47" s="30">
         <v>42791</v>
@@ -6245,7 +6245,7 @@
       </c>
       <c r="F48" s="15">
         <f t="shared" si="2"/>
-        <v>0.16766467065868268</v>
+        <v>0.17177914110429443</v>
       </c>
       <c r="G48" s="30">
         <v>42791</v>
@@ -6276,7 +6276,7 @@
       </c>
       <c r="F49" s="15">
         <f t="shared" si="2"/>
-        <v>0.16991017964071861</v>
+        <v>0.17407975460122693</v>
       </c>
       <c r="G49" s="30">
         <v>42791</v>
@@ -6307,7 +6307,7 @@
       </c>
       <c r="F50" s="15">
         <f t="shared" si="2"/>
-        <v>0.17589820359281441</v>
+        <v>0.1802147239263803</v>
       </c>
       <c r="G50" s="30">
         <v>42791</v>
@@ -6338,7 +6338,7 @@
       </c>
       <c r="F51" s="15">
         <f t="shared" si="2"/>
-        <v>0.17814371257485034</v>
+        <v>0.1825153374233128</v>
       </c>
       <c r="G51" s="30">
         <v>42791</v>
@@ -6369,7 +6369,7 @@
       </c>
       <c r="F52" s="15">
         <f t="shared" si="2"/>
-        <v>0.18562874251497011</v>
+        <v>0.19018404907975453</v>
       </c>
       <c r="G52" s="30">
         <v>42791</v>
@@ -6400,7 +6400,7 @@
       </c>
       <c r="F53" s="15">
         <f t="shared" si="2"/>
-        <v>0.18787425149700604</v>
+        <v>0.19248466257668703</v>
       </c>
       <c r="G53" s="30">
         <v>42791</v>
@@ -6431,7 +6431,7 @@
       </c>
       <c r="F54" s="15">
         <f t="shared" si="2"/>
-        <v>0.19910179640718567</v>
+        <v>0.2039877300613496</v>
       </c>
       <c r="G54" s="30">
         <v>42791</v>
@@ -6462,7 +6462,7 @@
       </c>
       <c r="F55" s="15">
         <f t="shared" si="2"/>
-        <v>0.2013473053892216</v>
+        <v>0.2062883435582821</v>
       </c>
       <c r="G55" s="30">
         <v>42791</v>
@@ -6493,7 +6493,7 @@
       </c>
       <c r="F56" s="15">
         <f t="shared" si="2"/>
-        <v>0.20209580838323357</v>
+        <v>0.20705521472392627</v>
       </c>
       <c r="G56" s="30">
         <v>42791</v>
@@ -6524,7 +6524,7 @@
       </c>
       <c r="F57" s="15">
         <f t="shared" si="2"/>
-        <v>0.21107784431137727</v>
+        <v>0.21625766871165633</v>
       </c>
       <c r="G57" s="30">
         <v>42791</v>
@@ -6555,7 +6555,7 @@
       </c>
       <c r="F58" s="15">
         <f t="shared" si="2"/>
-        <v>0.2133233532934132</v>
+        <v>0.21855828220858883</v>
       </c>
       <c r="G58" s="30">
         <v>42791</v>
@@ -6586,7 +6586,7 @@
       </c>
       <c r="F59" s="15">
         <f t="shared" si="2"/>
-        <v>0.220059880239521</v>
+        <v>0.22546012269938637</v>
       </c>
       <c r="G59" s="30">
         <v>42791</v>
@@ -6617,7 +6617,7 @@
       </c>
       <c r="F60" s="15">
         <f t="shared" si="2"/>
-        <v>0.22230538922155693</v>
+        <v>0.22776073619631887</v>
       </c>
       <c r="G60" s="30">
         <v>42791</v>
@@ -6647,7 +6647,7 @@
       <c r="E61" s="27"/>
       <c r="F61" s="29">
         <f t="shared" si="2"/>
-        <v>0.22230538922155693</v>
+        <v>0.22776073619631887</v>
       </c>
       <c r="G61" s="41" t="str">
         <f>IF(COUNTA(G62:G71)=COUNTA(B62:B71), "COMPLETE", "")</f>
@@ -6679,7 +6679,7 @@
       </c>
       <c r="F62" s="15">
         <f t="shared" si="2"/>
-        <v>0.2230538922155689</v>
+        <v>0.22852760736196304</v>
       </c>
       <c r="G62" s="30">
         <v>42791</v>
@@ -6710,7 +6710,7 @@
       </c>
       <c r="F63" s="15">
         <f t="shared" si="2"/>
-        <v>0.2297904191616767</v>
+        <v>0.23542944785276057</v>
       </c>
       <c r="G63" s="30">
         <v>42791</v>
@@ -6741,7 +6741,7 @@
       </c>
       <c r="F64" s="15">
         <f t="shared" si="2"/>
-        <v>0.23203592814371263</v>
+        <v>0.23773006134969307</v>
       </c>
       <c r="G64" s="30">
         <v>42791</v>
@@ -6772,7 +6772,7 @@
       </c>
       <c r="F65" s="15">
         <f t="shared" si="2"/>
-        <v>0.23802395209580843</v>
+        <v>0.24386503067484644</v>
       </c>
       <c r="G65" s="30">
         <v>42791</v>
@@ -6803,7 +6803,7 @@
       </c>
       <c r="F66" s="15">
         <f t="shared" si="2"/>
-        <v>0.24026946107784436</v>
+        <v>0.24616564417177894</v>
       </c>
       <c r="G66" s="30">
         <v>42791</v>
@@ -6834,7 +6834,7 @@
       </c>
       <c r="F67" s="15">
         <f t="shared" si="2"/>
-        <v>0.24401197604790423</v>
+        <v>0.24999999999999981</v>
       </c>
       <c r="G67" s="30">
         <v>42791</v>
@@ -6865,7 +6865,7 @@
       </c>
       <c r="F68" s="15">
         <f t="shared" si="2"/>
-        <v>0.24625748502994016</v>
+        <v>0.25230061349693234</v>
       </c>
       <c r="G68" s="30">
         <v>42791</v>
@@ -6896,7 +6896,7 @@
       </c>
       <c r="F69" s="15">
         <f t="shared" si="2"/>
-        <v>0.25449101796407192</v>
+        <v>0.26073619631901823</v>
       </c>
       <c r="G69" s="30">
         <v>42791</v>
@@ -6927,7 +6927,7 @@
       </c>
       <c r="F70" s="15">
         <f t="shared" ref="F70:F133" si="11">F69+(C70/$C$245)</f>
-        <v>0.25523952095808389</v>
+        <v>0.2615030674846624</v>
       </c>
       <c r="G70" s="30">
         <v>42791</v>
@@ -6958,7 +6958,7 @@
       </c>
       <c r="F71" s="15">
         <f t="shared" si="11"/>
-        <v>0.25748502994011979</v>
+        <v>0.2638036809815949</v>
       </c>
       <c r="G71" s="30">
         <v>42791</v>
@@ -6988,7 +6988,7 @@
       <c r="E72" s="27"/>
       <c r="F72" s="29">
         <f t="shared" si="11"/>
-        <v>0.25748502994011979</v>
+        <v>0.2638036809815949</v>
       </c>
       <c r="G72" s="41" t="str">
         <f>IF(COUNTA(G73:G83)=COUNTA(B73:B83), "COMPLETE", "")</f>
@@ -7020,7 +7020,7 @@
       </c>
       <c r="F73" s="15">
         <f t="shared" si="11"/>
-        <v>0.25823353293413176</v>
+        <v>0.26457055214723907</v>
       </c>
       <c r="G73" s="30">
         <v>42792</v>
@@ -7051,7 +7051,7 @@
       </c>
       <c r="F74" s="15">
         <f t="shared" si="11"/>
-        <v>0.2657185628742515</v>
+        <v>0.2722392638036808</v>
       </c>
       <c r="G74" s="30">
         <v>42794</v>
@@ -7082,7 +7082,7 @@
       </c>
       <c r="F75" s="15">
         <f t="shared" si="11"/>
-        <v>0.2679640718562874</v>
+        <v>0.2745398773006133</v>
       </c>
       <c r="G75" s="30">
         <v>42794</v>
@@ -7113,7 +7113,7 @@
       </c>
       <c r="F76" s="15">
         <f t="shared" si="11"/>
-        <v>0.27544910179640714</v>
+        <v>0.28220858895705503</v>
       </c>
       <c r="G76" s="30">
         <v>42794</v>
@@ -7144,7 +7144,7 @@
       </c>
       <c r="F77" s="15">
         <f t="shared" si="11"/>
-        <v>0.27769461077844304</v>
+        <v>0.28450920245398753</v>
       </c>
       <c r="G77" s="30">
         <v>42794</v>
@@ -7175,7 +7175,7 @@
       </c>
       <c r="F78" s="15">
         <f t="shared" si="11"/>
-        <v>0.2859281437125748</v>
+        <v>0.29294478527607343</v>
       </c>
       <c r="G78" s="30">
         <v>42794</v>
@@ -7206,7 +7206,7 @@
       </c>
       <c r="F79" s="15">
         <f t="shared" si="11"/>
-        <v>0.2881736526946107</v>
+        <v>0.29524539877300593</v>
       </c>
       <c r="G79" s="30">
         <v>42794</v>
@@ -7237,7 +7237,7 @@
       </c>
       <c r="F80" s="15">
         <f t="shared" si="11"/>
-        <v>0.2941616766467065</v>
+        <v>0.30138036809815932</v>
       </c>
       <c r="G80" s="30">
         <v>42794</v>
@@ -7268,7 +7268,7 @@
       </c>
       <c r="F81" s="15">
         <f t="shared" si="11"/>
-        <v>0.29640718562874241</v>
+        <v>0.30368098159509183</v>
       </c>
       <c r="G81" s="30">
         <v>42794</v>
@@ -7299,7 +7299,7 @@
       </c>
       <c r="F82" s="15">
         <f t="shared" si="11"/>
-        <v>0.30314371257485018</v>
+        <v>0.31058282208588939</v>
       </c>
       <c r="G82" s="30">
         <v>42794</v>
@@ -7330,7 +7330,7 @@
       </c>
       <c r="F83" s="15">
         <f t="shared" si="11"/>
-        <v>0.30538922155688608</v>
+        <v>0.31288343558282189</v>
       </c>
       <c r="G83" s="30">
         <v>42794</v>
@@ -7360,11 +7360,11 @@
       <c r="E84" s="27"/>
       <c r="F84" s="29">
         <f t="shared" si="11"/>
-        <v>0.30538922155688608</v>
+        <v>0.31288343558282189</v>
       </c>
       <c r="G84" s="41" t="str">
         <f>IF(COUNTA(G85:G107)=COUNTA(B85:B107), "COMPLETE", "")</f>
-        <v/>
+        <v>COMPLETE</v>
       </c>
       <c r="I84" s="9" t="str">
         <f t="shared" si="12"/>
@@ -7392,7 +7392,7 @@
       </c>
       <c r="F85" s="15">
         <f t="shared" si="11"/>
-        <v>0.30613772455089805</v>
+        <v>0.31365030674846606</v>
       </c>
       <c r="G85" s="30">
         <v>42794</v>
@@ -7423,9 +7423,11 @@
       </c>
       <c r="F86" s="15">
         <f t="shared" si="11"/>
-        <v>0.31362275449101779</v>
-      </c>
-      <c r="G86" s="30"/>
+        <v>0.32131901840490779</v>
+      </c>
+      <c r="G86" s="30">
+        <v>42794</v>
+      </c>
       <c r="H86" s="30">
         <v>42794</v>
       </c>
@@ -7452,9 +7454,11 @@
       </c>
       <c r="F87" s="15">
         <f t="shared" si="11"/>
-        <v>0.31586826347305369</v>
-      </c>
-      <c r="G87" s="30"/>
+        <v>0.32361963190184029</v>
+      </c>
+      <c r="G87" s="30">
+        <v>42794</v>
+      </c>
       <c r="H87" s="30">
         <v>42794</v>
       </c>
@@ -7481,9 +7485,11 @@
       </c>
       <c r="F88" s="15">
         <f t="shared" si="11"/>
-        <v>0.32335329341317343</v>
-      </c>
-      <c r="G88" s="30"/>
+        <v>0.33128834355828202</v>
+      </c>
+      <c r="G88" s="30">
+        <v>42794</v>
+      </c>
       <c r="H88" s="30">
         <v>42794</v>
       </c>
@@ -7510,9 +7516,11 @@
       </c>
       <c r="F89" s="15">
         <f t="shared" si="11"/>
-        <v>0.32559880239520933</v>
-      </c>
-      <c r="G89" s="30"/>
+        <v>0.33358895705521452</v>
+      </c>
+      <c r="G89" s="30">
+        <v>42794</v>
+      </c>
       <c r="H89" s="30">
         <v>42794</v>
       </c>
@@ -7539,9 +7547,11 @@
       </c>
       <c r="F90" s="15">
         <f t="shared" si="11"/>
-        <v>0.33532934131736503</v>
-      </c>
-      <c r="G90" s="30"/>
+        <v>0.34355828220858875</v>
+      </c>
+      <c r="G90" s="30">
+        <v>42794</v>
+      </c>
       <c r="H90" s="30">
         <v>42794</v>
       </c>
@@ -7568,9 +7578,11 @@
       </c>
       <c r="F91" s="15">
         <f t="shared" si="11"/>
-        <v>0.33757485029940093</v>
-      </c>
-      <c r="G91" s="30"/>
+        <v>0.34585889570552125</v>
+      </c>
+      <c r="G91" s="30">
+        <v>42794</v>
+      </c>
       <c r="H91" s="30">
         <v>42794</v>
       </c>
@@ -7597,9 +7609,11 @@
       </c>
       <c r="F92" s="15">
         <f t="shared" si="11"/>
-        <v>0.34805389221556859</v>
-      </c>
-      <c r="G92" s="30"/>
+        <v>0.35659509202453965</v>
+      </c>
+      <c r="G92" s="30">
+        <v>42794</v>
+      </c>
       <c r="H92" s="30">
         <v>42794</v>
       </c>
@@ -7626,9 +7640,11 @@
       </c>
       <c r="F93" s="15">
         <f t="shared" si="11"/>
-        <v>0.3502994011976045</v>
-      </c>
-      <c r="G93" s="30"/>
+        <v>0.35889570552147215</v>
+      </c>
+      <c r="G93" s="30">
+        <v>42794</v>
+      </c>
       <c r="H93" s="30">
         <v>42794</v>
       </c>
@@ -7655,9 +7671,11 @@
       </c>
       <c r="F94" s="15">
         <f t="shared" si="11"/>
-        <v>0.35928143712574823</v>
-      </c>
-      <c r="G94" s="30"/>
+        <v>0.36809815950920222</v>
+      </c>
+      <c r="G94" s="30">
+        <v>42794</v>
+      </c>
       <c r="H94" s="30">
         <v>42794</v>
       </c>
@@ -7684,9 +7702,11 @@
       </c>
       <c r="F95" s="15">
         <f t="shared" si="11"/>
-        <v>0.36152694610778413</v>
-      </c>
-      <c r="G95" s="30"/>
+        <v>0.37039877300613472</v>
+      </c>
+      <c r="G95" s="30">
+        <v>42794</v>
+      </c>
       <c r="H95" s="30">
         <v>42794</v>
       </c>
@@ -7713,9 +7733,11 @@
       </c>
       <c r="F96" s="15">
         <f t="shared" si="11"/>
-        <v>0.36976047904191589</v>
-      </c>
-      <c r="G96" s="30"/>
+        <v>0.37883435582822061</v>
+      </c>
+      <c r="G96" s="30">
+        <v>42794</v>
+      </c>
       <c r="H96" s="30">
         <v>42794</v>
       </c>
@@ -7742,9 +7764,11 @@
       </c>
       <c r="F97" s="15">
         <f t="shared" si="11"/>
-        <v>0.37200598802395179</v>
-      </c>
-      <c r="G97" s="30"/>
+        <v>0.38113496932515312</v>
+      </c>
+      <c r="G97" s="30">
+        <v>42794</v>
+      </c>
       <c r="H97" s="30">
         <v>42794</v>
       </c>
@@ -7771,9 +7795,11 @@
       </c>
       <c r="F98" s="15">
         <f t="shared" si="11"/>
-        <v>0.37724550898203563</v>
-      </c>
-      <c r="G98" s="30"/>
+        <v>0.38650306748466234</v>
+      </c>
+      <c r="G98" s="30">
+        <v>42794</v>
+      </c>
       <c r="H98" s="30">
         <v>42794</v>
       </c>
@@ -7800,9 +7826,11 @@
       </c>
       <c r="F99" s="15">
         <f t="shared" si="11"/>
-        <v>0.37949101796407153</v>
-      </c>
-      <c r="G99" s="30"/>
+        <v>0.38880368098159485</v>
+      </c>
+      <c r="G99" s="30">
+        <v>42794</v>
+      </c>
       <c r="H99" s="30">
         <v>42794</v>
       </c>
@@ -7829,9 +7857,11 @@
       </c>
       <c r="F100" s="15">
         <f t="shared" si="11"/>
-        <v>0.38547904191616733</v>
-      </c>
-      <c r="G100" s="30"/>
+        <v>0.39493865030674824</v>
+      </c>
+      <c r="G100" s="30">
+        <v>42794</v>
+      </c>
       <c r="H100" s="30">
         <v>42794</v>
       </c>
@@ -7858,9 +7888,11 @@
       </c>
       <c r="F101" s="15">
         <f t="shared" si="11"/>
-        <v>0.38772455089820324</v>
-      </c>
-      <c r="G101" s="30"/>
+        <v>0.39723926380368074</v>
+      </c>
+      <c r="G101" s="30">
+        <v>42794</v>
+      </c>
       <c r="H101" s="30">
         <v>42794</v>
       </c>
@@ -7887,9 +7919,11 @@
       </c>
       <c r="F102" s="15">
         <f t="shared" si="11"/>
-        <v>0.39745508982035893</v>
-      </c>
-      <c r="G102" s="30"/>
+        <v>0.40720858895705497</v>
+      </c>
+      <c r="G102" s="30">
+        <v>42794</v>
+      </c>
       <c r="H102" s="30">
         <v>42794</v>
       </c>
@@ -7916,9 +7950,11 @@
       </c>
       <c r="F103" s="15">
         <f t="shared" si="11"/>
-        <v>0.40494011976047867</v>
-      </c>
-      <c r="G103" s="30"/>
+        <v>0.4148773006134967</v>
+      </c>
+      <c r="G103" s="30">
+        <v>42794</v>
+      </c>
       <c r="H103" s="30">
         <v>42794</v>
       </c>
@@ -7945,9 +7981,11 @@
       </c>
       <c r="F104" s="15">
         <f t="shared" si="11"/>
-        <v>0.40718562874251457</v>
-      </c>
-      <c r="G104" s="30"/>
+        <v>0.4171779141104292</v>
+      </c>
+      <c r="G104" s="30">
+        <v>42794</v>
+      </c>
       <c r="H104" s="30">
         <v>42794</v>
       </c>
@@ -7974,9 +8012,11 @@
       </c>
       <c r="F105" s="15">
         <f t="shared" si="11"/>
-        <v>0.4161676646706583</v>
-      </c>
-      <c r="G105" s="30"/>
+        <v>0.42638036809815927</v>
+      </c>
+      <c r="G105" s="30">
+        <v>42794</v>
+      </c>
       <c r="H105" s="30">
         <v>42794</v>
       </c>
@@ -8003,9 +8043,11 @@
       </c>
       <c r="F106" s="15">
         <f t="shared" si="11"/>
-        <v>0.4184131736526942</v>
-      </c>
-      <c r="G106" s="30"/>
+        <v>0.42868098159509177</v>
+      </c>
+      <c r="G106" s="30">
+        <v>42794</v>
+      </c>
       <c r="H106" s="30">
         <v>42794</v>
       </c>
@@ -8032,19 +8074,21 @@
       </c>
       <c r="F107" s="15">
         <f t="shared" si="11"/>
-        <v>0.42365269461077804</v>
-      </c>
-      <c r="G107" s="30"/>
+        <v>0.434049079754601</v>
+      </c>
+      <c r="G107" s="30">
+        <v>42794</v>
+      </c>
       <c r="H107" s="30">
         <v>42794</v>
       </c>
-      <c r="I107" s="9" t="str">
+      <c r="I107" s="9">
         <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="J107" s="38" t="str">
+        <v>222</v>
+      </c>
+      <c r="J107" s="38">
         <f t="shared" si="13"/>
-        <v/>
+        <v>3.7</v>
       </c>
     </row>
     <row r="108" spans="1:10" ht="21" thickBot="1">
@@ -8060,7 +8104,7 @@
       <c r="E108" s="27"/>
       <c r="F108" s="29">
         <f t="shared" si="11"/>
-        <v>0.42365269461077804</v>
+        <v>0.434049079754601</v>
       </c>
       <c r="G108" s="41" t="str">
         <f>IF(COUNTA(G109:G125)=COUNTA(B109:B125), "COMPLETE", "")</f>
@@ -8092,11 +8136,11 @@
       </c>
       <c r="F109" s="15">
         <f t="shared" si="11"/>
-        <v>0.42440119760479</v>
+        <v>0.43481595092024516</v>
       </c>
       <c r="G109" s="30"/>
       <c r="H109" s="30">
-        <v>42794</v>
+        <v>42795</v>
       </c>
       <c r="I109" s="9" t="str">
         <f t="shared" si="12"/>
@@ -8121,11 +8165,11 @@
       </c>
       <c r="F110" s="15">
         <f t="shared" si="11"/>
-        <v>0.43113772455089777</v>
+        <v>0.44171779141104273</v>
       </c>
       <c r="G110" s="30"/>
       <c r="H110" s="30">
-        <v>42794</v>
+        <v>42795</v>
       </c>
       <c r="I110" s="9" t="str">
         <f t="shared" si="12"/>
@@ -8150,11 +8194,11 @@
       </c>
       <c r="F111" s="15">
         <f t="shared" si="11"/>
-        <v>0.43338323353293368</v>
+        <v>0.44401840490797523</v>
       </c>
       <c r="G111" s="30"/>
       <c r="H111" s="30">
-        <v>42794</v>
+        <v>42795</v>
       </c>
       <c r="I111" s="9" t="str">
         <f t="shared" si="12"/>
@@ -8179,11 +8223,11 @@
       </c>
       <c r="F112" s="15">
         <f t="shared" si="11"/>
-        <v>0.44161676646706544</v>
+        <v>0.45245398773006112</v>
       </c>
       <c r="G112" s="30"/>
       <c r="H112" s="30">
-        <v>42794</v>
+        <v>42795</v>
       </c>
       <c r="I112" s="9" t="str">
         <f t="shared" si="12"/>
@@ -8208,11 +8252,11 @@
       </c>
       <c r="F113" s="15">
         <f t="shared" si="11"/>
-        <v>0.44386227544910134</v>
+        <v>0.45475460122699363</v>
       </c>
       <c r="G113" s="30"/>
       <c r="H113" s="30">
-        <v>42794</v>
+        <v>42795</v>
       </c>
       <c r="I113" s="9" t="str">
         <f t="shared" si="12"/>
@@ -8237,11 +8281,11 @@
       </c>
       <c r="F114" s="15">
         <f t="shared" si="11"/>
-        <v>0.45359281437125704</v>
+        <v>0.46472392638036786</v>
       </c>
       <c r="G114" s="30"/>
       <c r="H114" s="30">
-        <v>42794</v>
+        <v>42795</v>
       </c>
       <c r="I114" s="9" t="str">
         <f t="shared" si="12"/>
@@ -8266,11 +8310,11 @@
       </c>
       <c r="F115" s="15">
         <f t="shared" si="11"/>
-        <v>0.45583832335329294</v>
+        <v>0.46702453987730036</v>
       </c>
       <c r="G115" s="30"/>
       <c r="H115" s="30">
-        <v>42794</v>
+        <v>42795</v>
       </c>
       <c r="I115" s="9" t="str">
         <f t="shared" si="12"/>
@@ -8295,11 +8339,11 @@
       </c>
       <c r="F116" s="15">
         <f t="shared" si="11"/>
-        <v>0.46556886227544864</v>
+        <v>0.47699386503067459</v>
       </c>
       <c r="G116" s="30"/>
       <c r="H116" s="30">
-        <v>42794</v>
+        <v>42795</v>
       </c>
       <c r="I116" s="9" t="str">
         <f t="shared" si="12"/>
@@ -8324,11 +8368,11 @@
       </c>
       <c r="F117" s="15">
         <f t="shared" si="11"/>
-        <v>0.46781437125748454</v>
+        <v>0.47929447852760709</v>
       </c>
       <c r="G117" s="30"/>
       <c r="H117" s="30">
-        <v>42794</v>
+        <v>42795</v>
       </c>
       <c r="I117" s="9" t="str">
         <f t="shared" si="12"/>
@@ -8353,11 +8397,11 @@
       </c>
       <c r="F118" s="15">
         <f t="shared" si="11"/>
-        <v>0.47679640718562827</v>
+        <v>0.48849693251533716</v>
       </c>
       <c r="G118" s="30"/>
       <c r="H118" s="30">
-        <v>42794</v>
+        <v>42795</v>
       </c>
       <c r="I118" s="9" t="str">
         <f t="shared" si="12"/>
@@ -8382,11 +8426,11 @@
       </c>
       <c r="F119" s="15">
         <f t="shared" si="11"/>
-        <v>0.47904191616766417</v>
+        <v>0.49079754601226966</v>
       </c>
       <c r="G119" s="30"/>
       <c r="H119" s="30">
-        <v>42794</v>
+        <v>42795</v>
       </c>
       <c r="I119" s="9" t="str">
         <f t="shared" si="12"/>
@@ -8411,11 +8455,11 @@
       </c>
       <c r="F120" s="15">
         <f t="shared" si="11"/>
-        <v>0.48502994011975997</v>
+        <v>0.49693251533742305</v>
       </c>
       <c r="G120" s="30"/>
       <c r="H120" s="30">
-        <v>42794</v>
+        <v>42795</v>
       </c>
       <c r="I120" s="9" t="str">
         <f t="shared" si="12"/>
@@ -8440,11 +8484,11 @@
       </c>
       <c r="F121" s="15">
         <f t="shared" si="11"/>
-        <v>0.48727544910179588</v>
+        <v>0.49923312883435556</v>
       </c>
       <c r="G121" s="30"/>
       <c r="H121" s="30">
-        <v>42794</v>
+        <v>42795</v>
       </c>
       <c r="I121" s="9" t="str">
         <f t="shared" si="12"/>
@@ -8469,11 +8513,11 @@
       </c>
       <c r="F122" s="15">
         <f t="shared" si="11"/>
-        <v>0.49550898203592764</v>
+        <v>0.50766871165644145</v>
       </c>
       <c r="G122" s="30"/>
       <c r="H122" s="30">
-        <v>42794</v>
+        <v>42795</v>
       </c>
       <c r="I122" s="9" t="str">
         <f t="shared" si="12"/>
@@ -8498,11 +8542,11 @@
       </c>
       <c r="F123" s="15">
         <f t="shared" si="11"/>
-        <v>0.49775449101796354</v>
+        <v>0.50996932515337401</v>
       </c>
       <c r="G123" s="30"/>
       <c r="H123" s="30">
-        <v>42794</v>
+        <v>42795</v>
       </c>
       <c r="I123" s="9" t="str">
         <f t="shared" si="12"/>
@@ -8527,11 +8571,11 @@
       </c>
       <c r="F124" s="15">
         <f t="shared" si="11"/>
-        <v>0.50673652694610727</v>
+        <v>0.51917177914110402</v>
       </c>
       <c r="G124" s="30"/>
       <c r="H124" s="30">
-        <v>42794</v>
+        <v>42795</v>
       </c>
       <c r="I124" s="9" t="str">
         <f t="shared" si="12"/>
@@ -8556,19 +8600,19 @@
       </c>
       <c r="F125" s="15">
         <f t="shared" si="11"/>
-        <v>0.50898203592814317</v>
+        <v>0.52147239263803657</v>
       </c>
       <c r="G125" s="30"/>
       <c r="H125" s="30">
-        <v>42794</v>
-      </c>
-      <c r="I125" s="9">
+        <v>42795</v>
+      </c>
+      <c r="I125" s="9" t="str">
         <f t="shared" si="12"/>
-        <v>336</v>
-      </c>
-      <c r="J125" s="38">
+        <v/>
+      </c>
+      <c r="J125" s="38" t="str">
         <f t="shared" si="13"/>
-        <v>5.6</v>
+        <v/>
       </c>
     </row>
     <row r="126" spans="1:10" ht="21" thickBot="1">
@@ -8584,7 +8628,7 @@
       <c r="E126" s="27"/>
       <c r="F126" s="29">
         <f t="shared" si="11"/>
-        <v>0.50898203592814317</v>
+        <v>0.52147239263803657</v>
       </c>
       <c r="G126" s="41" t="str">
         <f>IF(COUNTA(G127:G143)=COUNTA(B127:B143), "COMPLETE", "")</f>
@@ -8616,7 +8660,7 @@
       </c>
       <c r="F127" s="15">
         <f t="shared" si="11"/>
-        <v>0.50973053892215514</v>
+        <v>0.5222392638036808</v>
       </c>
       <c r="G127" s="30"/>
       <c r="H127" s="30">
@@ -8645,7 +8689,7 @@
       </c>
       <c r="F128" s="15">
         <f t="shared" si="11"/>
-        <v>0.51946107784431084</v>
+        <v>0.53220858895705503</v>
       </c>
       <c r="G128" s="30"/>
       <c r="H128" s="30">
@@ -8674,7 +8718,7 @@
       </c>
       <c r="F129" s="15">
         <f t="shared" si="11"/>
-        <v>0.52170658682634674</v>
+        <v>0.53450920245398759</v>
       </c>
       <c r="G129" s="30"/>
       <c r="H129" s="30">
@@ -8703,7 +8747,7 @@
       </c>
       <c r="F130" s="15">
         <f t="shared" si="11"/>
-        <v>0.53293413173652637</v>
+        <v>0.54601226993865015</v>
       </c>
       <c r="G130" s="30"/>
       <c r="H130" s="30">
@@ -8732,7 +8776,7 @@
       </c>
       <c r="F131" s="15">
         <f t="shared" si="11"/>
-        <v>0.53517964071856228</v>
+        <v>0.54831288343558271</v>
       </c>
       <c r="G131" s="30"/>
       <c r="H131" s="30">
@@ -8761,7 +8805,7 @@
       </c>
       <c r="F132" s="15">
         <f t="shared" si="11"/>
-        <v>0.54341317365269404</v>
+        <v>0.55674846625766861</v>
       </c>
       <c r="G132" s="30"/>
       <c r="H132" s="30">
@@ -8790,7 +8834,7 @@
       </c>
       <c r="F133" s="15">
         <f t="shared" si="11"/>
-        <v>0.54565868263472994</v>
+        <v>0.55904907975460116</v>
       </c>
       <c r="G133" s="30"/>
       <c r="H133" s="30">
@@ -8819,7 +8863,7 @@
       </c>
       <c r="F134" s="15">
         <f t="shared" ref="F134:F197" si="18">F133+(C134/$C$245)</f>
-        <v>0.55538922155688564</v>
+        <v>0.56901840490797539</v>
       </c>
       <c r="G134" s="30"/>
       <c r="H134" s="30">
@@ -8848,7 +8892,7 @@
       </c>
       <c r="F135" s="15">
         <f t="shared" si="18"/>
-        <v>0.55763473053892154</v>
+        <v>0.57131901840490795</v>
       </c>
       <c r="G135" s="30"/>
       <c r="H135" s="30">
@@ -8877,7 +8921,7 @@
       </c>
       <c r="F136" s="15">
         <f t="shared" si="18"/>
-        <v>0.5658682634730533</v>
+        <v>0.57975460122699385</v>
       </c>
       <c r="G136" s="30"/>
       <c r="H136" s="30">
@@ -8906,7 +8950,7 @@
       </c>
       <c r="F137" s="15">
         <f t="shared" si="18"/>
-        <v>0.56811377245508921</v>
+        <v>0.58205521472392641</v>
       </c>
       <c r="G137" s="30"/>
       <c r="H137" s="30">
@@ -8935,7 +8979,7 @@
       </c>
       <c r="F138" s="15">
         <f t="shared" si="18"/>
-        <v>0.57634730538922097</v>
+        <v>0.5904907975460123</v>
       </c>
       <c r="G138" s="30"/>
       <c r="H138" s="30">
@@ -8964,7 +9008,7 @@
       </c>
       <c r="F139" s="15">
         <f t="shared" si="18"/>
-        <v>0.57859281437125687</v>
+        <v>0.59279141104294486</v>
       </c>
       <c r="G139" s="30"/>
       <c r="H139" s="30">
@@ -8993,7 +9037,7 @@
       </c>
       <c r="F140" s="15">
         <f t="shared" si="18"/>
-        <v>0.58607784431137666</v>
+        <v>0.60046012269938653</v>
       </c>
       <c r="G140" s="30"/>
       <c r="H140" s="30">
@@ -9022,7 +9066,7 @@
       </c>
       <c r="F141" s="15">
         <f t="shared" si="18"/>
-        <v>0.58832335329341257</v>
+        <v>0.60276073619631909</v>
       </c>
       <c r="G141" s="30"/>
       <c r="H141" s="30">
@@ -9051,7 +9095,7 @@
       </c>
       <c r="F142" s="15">
         <f t="shared" si="18"/>
-        <v>0.59805389221556826</v>
+        <v>0.61273006134969332</v>
       </c>
       <c r="G142" s="30"/>
       <c r="H142" s="30">
@@ -9080,7 +9124,7 @@
       </c>
       <c r="F143" s="15">
         <f t="shared" si="18"/>
-        <v>0.60029940119760417</v>
+        <v>0.61503067484662588</v>
       </c>
       <c r="G143" s="30"/>
       <c r="H143" s="30">
@@ -9108,7 +9152,7 @@
       <c r="E144" s="27"/>
       <c r="F144" s="29">
         <f t="shared" si="18"/>
-        <v>0.60029940119760417</v>
+        <v>0.61503067484662588</v>
       </c>
       <c r="G144" s="41" t="str">
         <f>IF(COUNTA(G145:G158)=COUNTA(B145:B158), "COMPLETE", "")</f>
@@ -9140,7 +9184,7 @@
       </c>
       <c r="F145" s="15">
         <f t="shared" si="18"/>
-        <v>0.60104790419161613</v>
+        <v>0.6157975460122701</v>
       </c>
       <c r="G145" s="30"/>
       <c r="H145" s="30">
@@ -9169,7 +9213,7 @@
       </c>
       <c r="F146" s="15">
         <f t="shared" si="18"/>
-        <v>0.60703592814371199</v>
+        <v>0.62193251533742344</v>
       </c>
       <c r="G146" s="30"/>
       <c r="H146" s="30">
@@ -9198,7 +9242,7 @@
       </c>
       <c r="F147" s="15">
         <f t="shared" si="18"/>
-        <v>0.60928143712574789</v>
+        <v>0.624233128834356</v>
       </c>
       <c r="G147" s="30"/>
       <c r="H147" s="30">
@@ -9227,7 +9271,7 @@
       </c>
       <c r="F148" s="15">
         <f t="shared" si="18"/>
-        <v>0.61826347305389162</v>
+        <v>0.63343558282208601</v>
       </c>
       <c r="G148" s="30"/>
       <c r="H148" s="30">
@@ -9256,7 +9300,7 @@
       </c>
       <c r="F149" s="15">
         <f t="shared" si="18"/>
-        <v>0.62050898203592753</v>
+        <v>0.63573619631901856</v>
       </c>
       <c r="G149" s="30"/>
       <c r="H149" s="30">
@@ -9285,7 +9329,7 @@
       </c>
       <c r="F150" s="15">
         <f t="shared" si="18"/>
-        <v>0.63098802395209519</v>
+        <v>0.64647239263803702</v>
       </c>
       <c r="G150" s="30"/>
       <c r="H150" s="30">
@@ -9314,7 +9358,7 @@
       </c>
       <c r="F151" s="15">
         <f t="shared" si="18"/>
-        <v>0.63323353293413109</v>
+        <v>0.64877300613496958</v>
       </c>
       <c r="G151" s="30"/>
       <c r="H151" s="30">
@@ -9343,7 +9387,7 @@
       </c>
       <c r="F152" s="15">
         <f t="shared" si="18"/>
-        <v>0.64371257485029876</v>
+        <v>0.65950920245398803</v>
       </c>
       <c r="G152" s="30"/>
       <c r="H152" s="30">
@@ -9372,7 +9416,7 @@
       </c>
       <c r="F153" s="15">
         <f t="shared" si="18"/>
-        <v>0.64595808383233466</v>
+        <v>0.66180981595092059</v>
       </c>
       <c r="G153" s="30"/>
       <c r="H153" s="30">
@@ -9401,7 +9445,7 @@
       </c>
       <c r="F154" s="15">
         <f t="shared" si="18"/>
-        <v>0.65269461077844249</v>
+        <v>0.66871165644171815</v>
       </c>
       <c r="G154" s="30"/>
       <c r="H154" s="30">
@@ -9430,7 +9474,7 @@
       </c>
       <c r="F155" s="15">
         <f t="shared" si="18"/>
-        <v>0.65494011976047839</v>
+        <v>0.67101226993865071</v>
       </c>
       <c r="G155" s="30"/>
       <c r="H155" s="30">
@@ -9459,7 +9503,7 @@
       </c>
       <c r="F156" s="15">
         <f t="shared" si="18"/>
-        <v>0.66017964071856228</v>
+        <v>0.67638036809815993</v>
       </c>
       <c r="G156" s="30"/>
       <c r="H156" s="30">
@@ -9488,7 +9532,7 @@
       </c>
       <c r="F157" s="15">
         <f t="shared" si="18"/>
-        <v>0.66242514970059818</v>
+        <v>0.67868098159509249</v>
       </c>
       <c r="G157" s="30"/>
       <c r="H157" s="30">
@@ -9517,7 +9561,7 @@
       </c>
       <c r="F158" s="15">
         <f t="shared" si="18"/>
-        <v>0.66841317365269404</v>
+        <v>0.68481595092024583</v>
       </c>
       <c r="G158" s="30"/>
       <c r="H158" s="30">
@@ -9545,7 +9589,7 @@
       <c r="E159" s="27"/>
       <c r="F159" s="29">
         <f t="shared" si="18"/>
-        <v>0.66841317365269404</v>
+        <v>0.68481595092024583</v>
       </c>
       <c r="G159" s="41" t="str">
         <f>IF(COUNTA(G160:G162)=COUNTA(B160:B162), "COMPLETE", "")</f>
@@ -9577,7 +9621,7 @@
       </c>
       <c r="F160" s="15">
         <f t="shared" si="18"/>
-        <v>0.66916167664670601</v>
+        <v>0.68558282208589005</v>
       </c>
       <c r="G160" s="30"/>
       <c r="H160" s="30">
@@ -9606,7 +9650,7 @@
       </c>
       <c r="F161" s="15">
         <f t="shared" si="18"/>
-        <v>0.67589820359281383</v>
+        <v>0.69248466257668762</v>
       </c>
       <c r="G161" s="30"/>
       <c r="H161" s="30">
@@ -9635,7 +9679,7 @@
       </c>
       <c r="F162" s="15">
         <f t="shared" si="18"/>
-        <v>0.67814371257484973</v>
+        <v>0.69478527607362017</v>
       </c>
       <c r="G162" s="30"/>
       <c r="H162" s="30">
@@ -9664,7 +9708,7 @@
       </c>
       <c r="F163" s="15">
         <f t="shared" si="18"/>
-        <v>0.68562874251496952</v>
+        <v>0.70245398773006185</v>
       </c>
       <c r="G163" s="30"/>
       <c r="H163" s="30">
@@ -9693,19 +9737,19 @@
       </c>
       <c r="F164" s="15">
         <f t="shared" si="18"/>
-        <v>0.68787425149700543</v>
+        <v>0.7047546012269944</v>
       </c>
       <c r="G164" s="30"/>
       <c r="H164" s="30">
         <v>42795</v>
       </c>
-      <c r="I164" s="9" t="str">
+      <c r="I164" s="9">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="J164" s="38" t="str">
+        <v>353</v>
+      </c>
+      <c r="J164" s="38">
         <f t="shared" si="20"/>
-        <v/>
+        <v>5.8833333333333337</v>
       </c>
     </row>
     <row r="165" spans="1:10" outlineLevel="1">
@@ -9722,11 +9766,11 @@
       </c>
       <c r="F165" s="15">
         <f t="shared" si="18"/>
-        <v>0.69461077844311325</v>
+        <v>0.71165644171779197</v>
       </c>
       <c r="G165" s="30"/>
       <c r="H165" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I165" s="9" t="str">
         <f t="shared" si="19"/>
@@ -9751,11 +9795,11 @@
       </c>
       <c r="F166" s="15">
         <f t="shared" si="18"/>
-        <v>0.69685628742514916</v>
+        <v>0.71395705521472452</v>
       </c>
       <c r="G166" s="30"/>
       <c r="H166" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I166" s="9" t="str">
         <f t="shared" si="19"/>
@@ -9780,11 +9824,11 @@
       </c>
       <c r="F167" s="15">
         <f t="shared" si="18"/>
-        <v>0.70583832335329288</v>
+        <v>0.72315950920245453</v>
       </c>
       <c r="G167" s="30"/>
       <c r="H167" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I167" s="9" t="str">
         <f t="shared" si="19"/>
@@ -9809,11 +9853,11 @@
       </c>
       <c r="F168" s="15">
         <f t="shared" si="18"/>
-        <v>0.70808383233532879</v>
+        <v>0.72546012269938709</v>
       </c>
       <c r="G168" s="30"/>
       <c r="H168" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I168" s="9" t="str">
         <f t="shared" si="19"/>
@@ -9838,11 +9882,11 @@
       </c>
       <c r="F169" s="15">
         <f t="shared" si="18"/>
-        <v>0.71631736526946055</v>
+        <v>0.73389570552147299</v>
       </c>
       <c r="G169" s="30"/>
       <c r="H169" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I169" s="9" t="str">
         <f t="shared" si="19"/>
@@ -9867,11 +9911,11 @@
       </c>
       <c r="F170" s="15">
         <f t="shared" si="18"/>
-        <v>0.71856287425149645</v>
+        <v>0.73619631901840554</v>
       </c>
       <c r="G170" s="30"/>
       <c r="H170" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I170" s="9" t="str">
         <f t="shared" si="19"/>
@@ -9896,11 +9940,11 @@
       </c>
       <c r="F171" s="15">
         <f t="shared" si="18"/>
-        <v>0.72604790419161624</v>
+        <v>0.74386503067484722</v>
       </c>
       <c r="G171" s="30"/>
       <c r="H171" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I171" s="9" t="str">
         <f t="shared" si="19"/>
@@ -9925,11 +9969,11 @@
       </c>
       <c r="F172" s="15">
         <f t="shared" si="18"/>
-        <v>0.72829341317365215</v>
+        <v>0.74616564417177977</v>
       </c>
       <c r="G172" s="30"/>
       <c r="H172" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I172" s="9" t="str">
         <f t="shared" si="19"/>
@@ -9953,7 +9997,7 @@
       <c r="E173" s="27"/>
       <c r="F173" s="29">
         <f t="shared" si="18"/>
-        <v>0.72829341317365215</v>
+        <v>0.74616564417177977</v>
       </c>
       <c r="G173" s="41" t="str">
         <f>IF(COUNTA(G174:G176)=COUNTA(B174:B176), "COMPLETE", "")</f>
@@ -9985,11 +10029,11 @@
       </c>
       <c r="F174" s="15">
         <f t="shared" si="18"/>
-        <v>0.72904191616766412</v>
+        <v>0.746932515337424</v>
       </c>
       <c r="G174" s="30"/>
       <c r="H174" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I174" s="9" t="str">
         <f t="shared" si="19"/>
@@ -10014,11 +10058,11 @@
       </c>
       <c r="F175" s="15">
         <f t="shared" si="18"/>
-        <v>0.73577844311377194</v>
+        <v>0.75383435582822156</v>
       </c>
       <c r="G175" s="30"/>
       <c r="H175" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I175" s="9" t="str">
         <f t="shared" si="19"/>
@@ -10043,11 +10087,11 @@
       </c>
       <c r="F176" s="15">
         <f t="shared" si="18"/>
-        <v>0.73802395209580784</v>
+        <v>0.75613496932515412</v>
       </c>
       <c r="G176" s="30"/>
       <c r="H176" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I176" s="9" t="str">
         <f t="shared" si="19"/>
@@ -10072,11 +10116,11 @@
       </c>
       <c r="F177" s="15">
         <f t="shared" si="18"/>
-        <v>0.74326347305389162</v>
+        <v>0.76150306748466334</v>
       </c>
       <c r="G177" s="30"/>
       <c r="H177" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I177" s="9" t="str">
         <f t="shared" si="19"/>
@@ -10101,11 +10145,11 @@
       </c>
       <c r="F178" s="15">
         <f t="shared" si="18"/>
-        <v>0.74550898203592753</v>
+        <v>0.7638036809815959</v>
       </c>
       <c r="G178" s="30"/>
       <c r="H178" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I178" s="9" t="str">
         <f t="shared" si="19"/>
@@ -10130,11 +10174,11 @@
       </c>
       <c r="F179" s="15">
         <f t="shared" si="18"/>
-        <v>0.75224550898203535</v>
+        <v>0.77070552147239346</v>
       </c>
       <c r="G179" s="30"/>
       <c r="H179" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I179" s="9" t="str">
         <f t="shared" si="19"/>
@@ -10159,11 +10203,11 @@
       </c>
       <c r="F180" s="15">
         <f t="shared" si="18"/>
-        <v>0.75449101796407125</v>
+        <v>0.77300613496932602</v>
       </c>
       <c r="G180" s="30"/>
       <c r="H180" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I180" s="9" t="str">
         <f t="shared" si="19"/>
@@ -10188,11 +10232,11 @@
       </c>
       <c r="F181" s="15">
         <f t="shared" si="18"/>
-        <v>0.76272455089820301</v>
+        <v>0.78144171779141192</v>
       </c>
       <c r="G181" s="30"/>
       <c r="H181" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I181" s="9" t="str">
         <f t="shared" si="19"/>
@@ -10217,19 +10261,19 @@
       </c>
       <c r="F182" s="15">
         <f t="shared" si="18"/>
-        <v>0.76497005988023892</v>
+        <v>0.78374233128834447</v>
       </c>
       <c r="G182" s="30"/>
       <c r="H182" s="30">
-        <v>42795</v>
-      </c>
-      <c r="I182" s="9">
+        <v>42796</v>
+      </c>
+      <c r="I182" s="9" t="str">
         <f t="shared" si="19"/>
-        <v>342</v>
-      </c>
-      <c r="J182" s="38">
+        <v/>
+      </c>
+      <c r="J182" s="38" t="str">
         <f t="shared" si="20"/>
-        <v>5.7</v>
+        <v/>
       </c>
     </row>
     <row r="183" spans="2:10" outlineLevel="1">
@@ -10246,7 +10290,7 @@
       </c>
       <c r="F183" s="15">
         <f t="shared" si="18"/>
-        <v>0.77245508982035871</v>
+        <v>0.79141104294478615</v>
       </c>
       <c r="G183" s="30"/>
       <c r="H183" s="30">
@@ -10275,7 +10319,7 @@
       </c>
       <c r="F184" s="15">
         <f t="shared" si="18"/>
-        <v>0.77470059880239461</v>
+        <v>0.7937116564417187</v>
       </c>
       <c r="G184" s="30"/>
       <c r="H184" s="30">
@@ -10304,7 +10348,7 @@
       </c>
       <c r="F185" s="15">
         <f t="shared" si="18"/>
-        <v>0.7821856287425144</v>
+        <v>0.80138036809816038</v>
       </c>
       <c r="G185" s="30"/>
       <c r="H185" s="30">
@@ -10333,7 +10377,7 @@
       </c>
       <c r="F186" s="15">
         <f t="shared" si="18"/>
-        <v>0.78443113772455031</v>
+        <v>0.80368098159509294</v>
       </c>
       <c r="G186" s="30"/>
       <c r="H186" s="30">
@@ -10362,7 +10406,7 @@
       </c>
       <c r="F187" s="15">
         <f t="shared" si="18"/>
-        <v>0.79116766467065813</v>
+        <v>0.8105828220858905</v>
       </c>
       <c r="G187" s="30"/>
       <c r="H187" s="30">
@@ -10391,7 +10435,7 @@
       </c>
       <c r="F188" s="15">
         <f t="shared" si="18"/>
-        <v>0.80239520958083776</v>
+        <v>0.82208588957055306</v>
       </c>
       <c r="G188" s="30"/>
       <c r="H188" s="30">
@@ -10420,7 +10464,7 @@
       </c>
       <c r="F189" s="15">
         <f t="shared" si="18"/>
-        <v>0.80464071856287367</v>
+        <v>0.82438650306748562</v>
       </c>
       <c r="G189" s="30"/>
       <c r="H189" s="30">
@@ -10449,7 +10493,7 @@
       </c>
       <c r="F190" s="15">
         <f t="shared" si="18"/>
-        <v>0.81212574850299346</v>
+        <v>0.83205521472392729</v>
       </c>
       <c r="G190" s="30"/>
       <c r="H190" s="30">
@@ -10478,7 +10522,7 @@
       </c>
       <c r="F191" s="15">
         <f t="shared" si="18"/>
-        <v>0.81961077844311325</v>
+        <v>0.83972392638036897</v>
       </c>
       <c r="G191" s="30"/>
       <c r="H191" s="30">
@@ -10507,7 +10551,7 @@
       </c>
       <c r="F192" s="15">
         <f t="shared" si="18"/>
-        <v>0.82185628742514916</v>
+        <v>0.84202453987730153</v>
       </c>
       <c r="G192" s="30"/>
       <c r="H192" s="30">
@@ -10535,7 +10579,7 @@
       <c r="E193" s="27"/>
       <c r="F193" s="29">
         <f t="shared" si="18"/>
-        <v>0.82185628742514916</v>
+        <v>0.84202453987730153</v>
       </c>
       <c r="G193" s="41" t="str">
         <f>IF(COUNTA(G194:G196)=COUNTA(B194:B196), "COMPLETE", "")</f>
@@ -10567,7 +10611,7 @@
       </c>
       <c r="F194" s="15">
         <f t="shared" si="18"/>
-        <v>0.82260479041916112</v>
+        <v>0.84279141104294575</v>
       </c>
       <c r="G194" s="30"/>
       <c r="H194" s="30">
@@ -10596,7 +10640,7 @@
       </c>
       <c r="F195" s="15">
         <f t="shared" si="18"/>
-        <v>0.83083832335329288</v>
+        <v>0.85122699386503164</v>
       </c>
       <c r="G195" s="30"/>
       <c r="H195" s="30">
@@ -10625,7 +10669,7 @@
       </c>
       <c r="F196" s="15">
         <f t="shared" si="18"/>
-        <v>0.83308383233532879</v>
+        <v>0.8535276073619642</v>
       </c>
       <c r="G196" s="30"/>
       <c r="H196" s="30">
@@ -10654,7 +10698,7 @@
       </c>
       <c r="F197" s="15">
         <f t="shared" si="18"/>
-        <v>0.84056886227544858</v>
+        <v>0.86119631901840588</v>
       </c>
       <c r="G197" s="30"/>
       <c r="H197" s="30">
@@ -10683,7 +10727,7 @@
       </c>
       <c r="F198" s="15">
         <f t="shared" ref="F198:F243" si="26">F197+(C198/$C$245)</f>
-        <v>0.84281437125748448</v>
+        <v>0.86349693251533843</v>
       </c>
       <c r="G198" s="30"/>
       <c r="H198" s="30">
@@ -10712,7 +10756,7 @@
       </c>
       <c r="F199" s="15">
         <f t="shared" si="26"/>
-        <v>0.84805389221556826</v>
+        <v>0.86886503067484766</v>
       </c>
       <c r="G199" s="30"/>
       <c r="H199" s="30">
@@ -10741,7 +10785,7 @@
       </c>
       <c r="F200" s="15">
         <f t="shared" si="26"/>
-        <v>0.85029940119760417</v>
+        <v>0.87116564417178022</v>
       </c>
       <c r="G200" s="30"/>
       <c r="H200" s="30">
@@ -10769,7 +10813,7 @@
       <c r="E201" s="27"/>
       <c r="F201" s="29">
         <f t="shared" si="26"/>
-        <v>0.85029940119760417</v>
+        <v>0.87116564417178022</v>
       </c>
       <c r="G201" s="41" t="str">
         <f>IF(COUNTA(G202:G204)=COUNTA(B202:B204), "COMPLETE", "")</f>
@@ -10801,7 +10845,7 @@
       </c>
       <c r="F202" s="15">
         <f t="shared" si="26"/>
-        <v>0.85104790419161613</v>
+        <v>0.87193251533742444</v>
       </c>
       <c r="G202" s="30"/>
       <c r="H202" s="30">
@@ -10830,7 +10874,7 @@
       </c>
       <c r="F203" s="15">
         <f t="shared" si="26"/>
-        <v>0.85853293413173593</v>
+        <v>0.87960122699386611</v>
       </c>
       <c r="G203" s="30"/>
       <c r="H203" s="30">
@@ -10859,7 +10903,7 @@
       </c>
       <c r="F204" s="15">
         <f t="shared" si="26"/>
-        <v>0.86077844311377183</v>
+        <v>0.88190184049079867</v>
       </c>
       <c r="G204" s="30"/>
       <c r="H204" s="30">
@@ -10888,7 +10932,7 @@
       </c>
       <c r="F205" s="15">
         <f t="shared" si="26"/>
-        <v>0.87050898203592753</v>
+        <v>0.8918711656441729</v>
       </c>
       <c r="G205" s="30"/>
       <c r="H205" s="30">
@@ -10917,7 +10961,7 @@
       </c>
       <c r="F206" s="15">
         <f t="shared" si="26"/>
-        <v>0.87275449101796343</v>
+        <v>0.89417177914110546</v>
       </c>
       <c r="G206" s="30"/>
       <c r="H206" s="30">
@@ -10946,7 +10990,7 @@
       </c>
       <c r="F207" s="15">
         <f t="shared" si="26"/>
-        <v>0.885479041916167</v>
+        <v>0.90720858895705636</v>
       </c>
       <c r="G207" s="30"/>
       <c r="H207" s="30">
@@ -10975,7 +11019,7 @@
       </c>
       <c r="F208" s="15">
         <f t="shared" si="26"/>
-        <v>0.8877245508982029</v>
+        <v>0.90950920245398892</v>
       </c>
       <c r="G208" s="30"/>
       <c r="H208" s="30">
@@ -11004,7 +11048,7 @@
       </c>
       <c r="F209" s="15">
         <f t="shared" si="26"/>
-        <v>0.89371257485029876</v>
+        <v>0.91564417177914226</v>
       </c>
       <c r="G209" s="30"/>
       <c r="H209" s="30">
@@ -11033,7 +11077,7 @@
       </c>
       <c r="F210" s="15">
         <f t="shared" si="26"/>
-        <v>0.89595808383233466</v>
+        <v>0.91794478527607481</v>
       </c>
       <c r="G210" s="30"/>
       <c r="H210" s="30">
@@ -11061,7 +11105,7 @@
       <c r="E211" s="27"/>
       <c r="F211" s="29">
         <f t="shared" si="26"/>
-        <v>0.89595808383233466</v>
+        <v>0.91794478527607481</v>
       </c>
       <c r="G211" s="41" t="str">
         <f>IF(COUNTA(G212:G214)=COUNTA(B212:B214), "COMPLETE", "")</f>
@@ -11093,7 +11137,7 @@
       </c>
       <c r="F212" s="15">
         <f t="shared" si="26"/>
-        <v>0.89670658682634663</v>
+        <v>0.91871165644171904</v>
       </c>
       <c r="G212" s="30"/>
       <c r="H212" s="30">
@@ -11122,7 +11166,7 @@
       </c>
       <c r="F213" s="15">
         <f t="shared" si="26"/>
-        <v>0.90568862275449036</v>
+        <v>0.92791411042944905</v>
       </c>
       <c r="G213" s="30"/>
       <c r="H213" s="30">
@@ -11151,7 +11195,7 @@
       </c>
       <c r="F214" s="15">
         <f t="shared" si="26"/>
-        <v>0.90793413173652626</v>
+        <v>0.9302147239263816</v>
       </c>
       <c r="G214" s="30"/>
       <c r="H214" s="30">
@@ -11180,7 +11224,7 @@
       </c>
       <c r="F215" s="15">
         <f t="shared" si="26"/>
-        <v>0.91317365269461015</v>
+        <v>0.93558282208589083</v>
       </c>
       <c r="G215" s="30"/>
       <c r="H215" s="30">
@@ -11209,7 +11253,7 @@
       </c>
       <c r="F216" s="15">
         <f t="shared" si="26"/>
-        <v>0.91541916167664605</v>
+        <v>0.93788343558282339</v>
       </c>
       <c r="G216" s="30"/>
       <c r="H216" s="30">
@@ -11237,7 +11281,7 @@
       <c r="E217" s="27"/>
       <c r="F217" s="29">
         <f t="shared" si="26"/>
-        <v>0.91541916167664605</v>
+        <v>0.93788343558282339</v>
       </c>
       <c r="G217" s="41" t="str">
         <f>IF(COUNTA(G218:G220)=COUNTA(B218:B220), "COMPLETE", "")</f>
@@ -11269,7 +11313,7 @@
       </c>
       <c r="F218" s="15">
         <f t="shared" si="26"/>
-        <v>0.92215568862275388</v>
+        <v>0.94478527607362095</v>
       </c>
       <c r="G218" s="30"/>
       <c r="H218" s="30">
@@ -11298,7 +11342,7 @@
       </c>
       <c r="F219" s="15">
         <f t="shared" si="26"/>
-        <v>0.92440119760478978</v>
+        <v>0.94708588957055351</v>
       </c>
       <c r="G219" s="30"/>
       <c r="H219" s="30">
@@ -11327,7 +11371,7 @@
       </c>
       <c r="F220" s="15">
         <f t="shared" si="26"/>
-        <v>0.92664670658682569</v>
+        <v>0.94938650306748606</v>
       </c>
       <c r="G220" s="30"/>
       <c r="H220" s="30">
@@ -11356,7 +11400,7 @@
       </c>
       <c r="F221" s="15">
         <f t="shared" si="26"/>
-        <v>0.93488023952095745</v>
+        <v>0.95782208588957196</v>
       </c>
       <c r="G221" s="30"/>
       <c r="H221" s="30">
@@ -11385,7 +11429,7 @@
       </c>
       <c r="F222" s="15">
         <f t="shared" si="26"/>
-        <v>0.93712574850299335</v>
+        <v>0.96012269938650452</v>
       </c>
       <c r="G222" s="30"/>
       <c r="H222" s="30">
@@ -11414,19 +11458,19 @@
       </c>
       <c r="F223" s="15">
         <f t="shared" si="26"/>
-        <v>0.93787425149700532</v>
+        <v>0.96088957055214874</v>
       </c>
       <c r="G223" s="30"/>
       <c r="H223" s="30">
         <v>42796</v>
       </c>
-      <c r="I223" s="9" t="str">
+      <c r="I223" s="9">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-      <c r="J223" s="38" t="str">
+        <v>334</v>
+      </c>
+      <c r="J223" s="38">
         <f t="shared" si="28"/>
-        <v/>
+        <v>5.5666666666666664</v>
       </c>
     </row>
     <row r="224" spans="1:10" ht="21" thickBot="1">
@@ -11442,7 +11486,7 @@
       <c r="E224" s="27"/>
       <c r="F224" s="29">
         <f t="shared" si="26"/>
-        <v>0.93787425149700532</v>
+        <v>0.96088957055214874</v>
       </c>
       <c r="G224" s="41" t="str">
         <f>IF(COUNTA(G225:G225)=COUNTA(B225:B225), "COMPLETE", "")</f>
@@ -11473,11 +11517,11 @@
       </c>
       <c r="F225" s="15">
         <f t="shared" si="26"/>
-        <v>0.93862275449101729</v>
+        <v>0.96165644171779296</v>
       </c>
       <c r="G225" s="30"/>
       <c r="H225" s="30">
-        <v>42796</v>
+        <v>42797</v>
       </c>
       <c r="I225" s="9" t="str">
         <f t="shared" si="27"/>
@@ -11496,12 +11540,12 @@
       <c r="C226" s="26"/>
       <c r="D226" s="20">
         <f>SUM(C226:C244)</f>
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="E226" s="27"/>
       <c r="F226" s="29">
         <f t="shared" si="26"/>
-        <v>0.93862275449101729</v>
+        <v>0.96165644171779296</v>
       </c>
       <c r="G226" s="41" t="str">
         <f>IF(COUNTA(G227:G229)=COUNTA(B227:B229), "COMPLETE", "")</f>
@@ -11521,23 +11565,23 @@
         <v>282</v>
       </c>
       <c r="C227" s="14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D227" s="21">
         <f>D226/60</f>
-        <v>1.3666666666666667</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="E227" s="15">
         <f>E226+(C227/$D$226)</f>
-        <v>6.097560975609756E-2</v>
+        <v>0.06</v>
       </c>
       <c r="F227" s="15">
         <f t="shared" si="26"/>
-        <v>0.94236526946107713</v>
+        <v>0.96395705521472552</v>
       </c>
       <c r="G227" s="30"/>
       <c r="H227" s="30">
-        <v>42796</v>
+        <v>42797</v>
       </c>
       <c r="I227" s="9" t="str">
         <f t="shared" si="27"/>
@@ -11553,20 +11597,20 @@
         <v>283</v>
       </c>
       <c r="C228" s="14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D228" s="19"/>
       <c r="E228" s="15">
         <f t="shared" ref="E228:E243" si="32">E227+(C228/$D$226)</f>
-        <v>0.12195121951219512</v>
+        <v>0.12</v>
       </c>
       <c r="F228" s="15">
         <f t="shared" si="26"/>
-        <v>0.94610778443113697</v>
+        <v>0.96625766871165808</v>
       </c>
       <c r="G228" s="30"/>
       <c r="H228" s="30">
-        <v>42796</v>
+        <v>42797</v>
       </c>
       <c r="I228" s="9" t="str">
         <f t="shared" si="27"/>
@@ -11582,20 +11626,20 @@
         <v>284</v>
       </c>
       <c r="C229" s="14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D229" s="19"/>
       <c r="E229" s="15">
         <f t="shared" si="32"/>
-        <v>0.18292682926829268</v>
+        <v>0.18</v>
       </c>
       <c r="F229" s="15">
         <f t="shared" si="26"/>
-        <v>0.94985029940119681</v>
+        <v>0.96855828220859064</v>
       </c>
       <c r="G229" s="30"/>
       <c r="H229" s="30">
-        <v>42796</v>
+        <v>42797</v>
       </c>
       <c r="I229" s="9" t="str">
         <f t="shared" si="27"/>
@@ -11611,20 +11655,20 @@
         <v>285</v>
       </c>
       <c r="C230" s="14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D230" s="19"/>
       <c r="E230" s="15">
         <f t="shared" si="32"/>
-        <v>0.24390243902439024</v>
+        <v>0.24</v>
       </c>
       <c r="F230" s="15">
         <f t="shared" si="26"/>
-        <v>0.95359281437125665</v>
+        <v>0.97085889570552319</v>
       </c>
       <c r="G230" s="30"/>
       <c r="H230" s="30">
-        <v>42796</v>
+        <v>42797</v>
       </c>
       <c r="I230" s="9" t="str">
         <f t="shared" si="27"/>
@@ -11640,20 +11684,20 @@
         <v>286</v>
       </c>
       <c r="C231" s="14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D231" s="19"/>
       <c r="E231" s="15">
         <f t="shared" si="32"/>
-        <v>0.3048780487804878</v>
+        <v>0.3</v>
       </c>
       <c r="F231" s="15">
         <f t="shared" si="26"/>
-        <v>0.95733532934131649</v>
+        <v>0.97315950920245575</v>
       </c>
       <c r="G231" s="30"/>
       <c r="H231" s="30">
-        <v>42796</v>
+        <v>42797</v>
       </c>
       <c r="I231" s="9" t="str">
         <f t="shared" si="27"/>
@@ -11669,20 +11713,20 @@
         <v>287</v>
       </c>
       <c r="C232" s="14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D232" s="19"/>
       <c r="E232" s="15">
         <f t="shared" si="32"/>
-        <v>0.36585365853658536</v>
+        <v>0.36</v>
       </c>
       <c r="F232" s="15">
         <f t="shared" si="26"/>
-        <v>0.96107784431137633</v>
+        <v>0.97546012269938831</v>
       </c>
       <c r="G232" s="30"/>
       <c r="H232" s="30">
-        <v>42796</v>
+        <v>42797</v>
       </c>
       <c r="I232" s="9" t="str">
         <f t="shared" si="27"/>
@@ -11698,20 +11742,20 @@
         <v>288</v>
       </c>
       <c r="C233" s="14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D233" s="19"/>
       <c r="E233" s="15">
         <f t="shared" si="32"/>
-        <v>0.42682926829268292</v>
+        <v>0.42</v>
       </c>
       <c r="F233" s="15">
         <f t="shared" si="26"/>
-        <v>0.96482035928143617</v>
+        <v>0.97776073619632087</v>
       </c>
       <c r="G233" s="30"/>
       <c r="H233" s="30">
-        <v>42796</v>
+        <v>42797</v>
       </c>
       <c r="I233" s="9" t="str">
         <f t="shared" si="27"/>
@@ -11727,20 +11771,20 @@
         <v>289</v>
       </c>
       <c r="C234" s="14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D234" s="19"/>
       <c r="E234" s="15">
         <f t="shared" si="32"/>
-        <v>0.48780487804878048</v>
+        <v>0.48</v>
       </c>
       <c r="F234" s="15">
         <f t="shared" si="26"/>
-        <v>0.96856287425149601</v>
+        <v>0.98006134969325343</v>
       </c>
       <c r="G234" s="30"/>
       <c r="H234" s="30">
-        <v>42796</v>
+        <v>42797</v>
       </c>
       <c r="I234" s="9" t="str">
         <f t="shared" si="27"/>
@@ -11756,20 +11800,20 @@
         <v>290</v>
       </c>
       <c r="C235" s="14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D235" s="19"/>
       <c r="E235" s="15">
         <f t="shared" si="32"/>
-        <v>0.54878048780487809</v>
+        <v>0.54</v>
       </c>
       <c r="F235" s="15">
         <f t="shared" si="26"/>
-        <v>0.97230538922155585</v>
+        <v>0.98236196319018598</v>
       </c>
       <c r="G235" s="30"/>
       <c r="H235" s="30">
-        <v>42796</v>
+        <v>42797</v>
       </c>
       <c r="I235" s="9" t="str">
         <f t="shared" si="27"/>
@@ -11785,20 +11829,20 @@
         <v>291</v>
       </c>
       <c r="C236" s="14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D236" s="19"/>
       <c r="E236" s="15">
         <f t="shared" si="32"/>
-        <v>0.60975609756097571</v>
+        <v>0.60000000000000009</v>
       </c>
       <c r="F236" s="15">
         <f t="shared" si="26"/>
-        <v>0.97604790419161569</v>
+        <v>0.98466257668711854</v>
       </c>
       <c r="G236" s="30"/>
       <c r="H236" s="30">
-        <v>42796</v>
+        <v>42797</v>
       </c>
       <c r="I236" s="9" t="str">
         <f t="shared" si="27"/>
@@ -11814,20 +11858,20 @@
         <v>292</v>
       </c>
       <c r="C237" s="14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D237" s="19"/>
       <c r="E237" s="15">
         <f t="shared" si="32"/>
-        <v>0.67073170731707332</v>
+        <v>0.66000000000000014</v>
       </c>
       <c r="F237" s="15">
         <f t="shared" si="26"/>
-        <v>0.97979041916167553</v>
+        <v>0.9869631901840511</v>
       </c>
       <c r="G237" s="30"/>
       <c r="H237" s="30">
-        <v>42796</v>
+        <v>42797</v>
       </c>
       <c r="I237" s="9" t="str">
         <f t="shared" si="27"/>
@@ -11843,20 +11887,20 @@
         <v>293</v>
       </c>
       <c r="C238" s="14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D238" s="19"/>
       <c r="E238" s="15">
         <f t="shared" si="32"/>
-        <v>0.73170731707317094</v>
+        <v>0.7200000000000002</v>
       </c>
       <c r="F238" s="15">
         <f t="shared" si="26"/>
-        <v>0.98353293413173537</v>
+        <v>0.98926380368098366</v>
       </c>
       <c r="G238" s="30"/>
       <c r="H238" s="30">
-        <v>42796</v>
+        <v>42797</v>
       </c>
       <c r="I238" s="9" t="str">
         <f t="shared" si="27"/>
@@ -11872,20 +11916,20 @@
         <v>294</v>
       </c>
       <c r="C239" s="14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D239" s="19"/>
       <c r="E239" s="15">
         <f t="shared" si="32"/>
-        <v>0.79268292682926855</v>
+        <v>0.78000000000000025</v>
       </c>
       <c r="F239" s="15">
         <f t="shared" si="26"/>
-        <v>0.98727544910179521</v>
+        <v>0.99156441717791621</v>
       </c>
       <c r="G239" s="30"/>
       <c r="H239" s="30">
-        <v>42796</v>
+        <v>42797</v>
       </c>
       <c r="I239" s="9" t="str">
         <f t="shared" si="27"/>
@@ -11901,20 +11945,20 @@
         <v>295</v>
       </c>
       <c r="C240" s="14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D240" s="19"/>
       <c r="E240" s="15">
         <f t="shared" si="32"/>
-        <v>0.85365853658536617</v>
+        <v>0.8400000000000003</v>
       </c>
       <c r="F240" s="15">
         <f t="shared" si="26"/>
-        <v>0.99101796407185505</v>
+        <v>0.99386503067484877</v>
       </c>
       <c r="G240" s="30"/>
       <c r="H240" s="30">
-        <v>42796</v>
+        <v>42797</v>
       </c>
       <c r="I240" s="9" t="str">
         <f t="shared" si="27"/>
@@ -11930,20 +11974,20 @@
         <v>296</v>
       </c>
       <c r="C241" s="14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D241" s="19"/>
       <c r="E241" s="15">
         <f t="shared" si="32"/>
-        <v>0.91463414634146378</v>
+        <v>0.90000000000000036</v>
       </c>
       <c r="F241" s="15">
         <f t="shared" si="26"/>
-        <v>0.99476047904191489</v>
+        <v>0.99616564417178133</v>
       </c>
       <c r="G241" s="30"/>
       <c r="H241" s="30">
-        <v>42796</v>
+        <v>42797</v>
       </c>
       <c r="I241" s="9" t="str">
         <f t="shared" si="27"/>
@@ -11959,20 +12003,20 @@
         <v>297</v>
       </c>
       <c r="C242" s="14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D242" s="19"/>
       <c r="E242" s="15">
         <f t="shared" si="32"/>
-        <v>0.9756097560975614</v>
+        <v>0.96000000000000041</v>
       </c>
       <c r="F242" s="15">
         <f t="shared" si="26"/>
-        <v>0.99850299401197473</v>
+        <v>0.99846625766871389</v>
       </c>
       <c r="G242" s="30"/>
       <c r="H242" s="30">
-        <v>42796</v>
+        <v>42797</v>
       </c>
       <c r="I242" s="9" t="str">
         <f t="shared" si="27"/>
@@ -11997,19 +12041,19 @@
       </c>
       <c r="F243" s="15">
         <f t="shared" si="26"/>
-        <v>0.99999999999999867</v>
+        <v>1.0000000000000022</v>
       </c>
       <c r="G243" s="30"/>
       <c r="H243" s="30">
-        <v>42796</v>
+        <v>42797</v>
       </c>
       <c r="I243" s="9">
         <f t="shared" si="27"/>
-        <v>314</v>
+        <v>51</v>
       </c>
       <c r="J243" s="38">
         <f t="shared" si="28"/>
-        <v>5.2333333333333334</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="245" spans="2:10" ht="15.75" thickBot="1">
@@ -12018,7 +12062,7 @@
       </c>
       <c r="C245" s="40">
         <f>SUM(C4:C244)</f>
-        <v>1336</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="246" spans="2:10" ht="15.75" thickTop="1">
@@ -12027,7 +12071,7 @@
       </c>
       <c r="C246" s="12">
         <f>+C245/60</f>
-        <v>22.266666666666666</v>
+        <v>21.733333333333334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Section 9: Materials & Effects completed
</commit_message>
<xml_diff>
--- a/Unity Certification Course (Udemy) - Video Listing.xlsx
+++ b/Unity Certification Course (Udemy) - Video Listing.xlsx
@@ -4804,8 +4804,8 @@
   <dimension ref="A1:J246"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G107" sqref="G107"/>
+      <pane ySplit="3" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G125" sqref="G125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -4833,7 +4833,7 @@
       </c>
       <c r="F1" s="34">
         <f>SUMIF(G4:G244, "&gt;0", C4:C244)</f>
-        <v>566</v>
+        <v>680</v>
       </c>
       <c r="G1" s="35">
         <f>+C245</f>
@@ -4841,7 +4841,7 @@
       </c>
       <c r="H1" s="36">
         <f>+F1/G1</f>
-        <v>0.43404907975460122</v>
+        <v>0.5214723926380368</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -8108,7 +8108,7 @@
       </c>
       <c r="G108" s="41" t="str">
         <f>IF(COUNTA(G109:G125)=COUNTA(B109:B125), "COMPLETE", "")</f>
-        <v/>
+        <v>COMPLETE</v>
       </c>
       <c r="I108" s="9" t="str">
         <f t="shared" si="12"/>
@@ -8138,7 +8138,9 @@
         <f t="shared" si="11"/>
         <v>0.43481595092024516</v>
       </c>
-      <c r="G109" s="30"/>
+      <c r="G109" s="30">
+        <v>42795</v>
+      </c>
       <c r="H109" s="30">
         <v>42795</v>
       </c>
@@ -8167,7 +8169,9 @@
         <f t="shared" si="11"/>
         <v>0.44171779141104273</v>
       </c>
-      <c r="G110" s="30"/>
+      <c r="G110" s="30">
+        <v>42795</v>
+      </c>
       <c r="H110" s="30">
         <v>42795</v>
       </c>
@@ -8196,7 +8200,9 @@
         <f t="shared" si="11"/>
         <v>0.44401840490797523</v>
       </c>
-      <c r="G111" s="30"/>
+      <c r="G111" s="30">
+        <v>42795</v>
+      </c>
       <c r="H111" s="30">
         <v>42795</v>
       </c>
@@ -8225,7 +8231,9 @@
         <f t="shared" si="11"/>
         <v>0.45245398773006112</v>
       </c>
-      <c r="G112" s="30"/>
+      <c r="G112" s="30">
+        <v>42795</v>
+      </c>
       <c r="H112" s="30">
         <v>42795</v>
       </c>
@@ -8254,7 +8262,9 @@
         <f t="shared" si="11"/>
         <v>0.45475460122699363</v>
       </c>
-      <c r="G113" s="30"/>
+      <c r="G113" s="30">
+        <v>42795</v>
+      </c>
       <c r="H113" s="30">
         <v>42795</v>
       </c>
@@ -8283,7 +8293,9 @@
         <f t="shared" si="11"/>
         <v>0.46472392638036786</v>
       </c>
-      <c r="G114" s="30"/>
+      <c r="G114" s="30">
+        <v>42795</v>
+      </c>
       <c r="H114" s="30">
         <v>42795</v>
       </c>
@@ -8312,7 +8324,9 @@
         <f t="shared" si="11"/>
         <v>0.46702453987730036</v>
       </c>
-      <c r="G115" s="30"/>
+      <c r="G115" s="30">
+        <v>42795</v>
+      </c>
       <c r="H115" s="30">
         <v>42795</v>
       </c>
@@ -8341,7 +8355,9 @@
         <f t="shared" si="11"/>
         <v>0.47699386503067459</v>
       </c>
-      <c r="G116" s="30"/>
+      <c r="G116" s="30">
+        <v>42795</v>
+      </c>
       <c r="H116" s="30">
         <v>42795</v>
       </c>
@@ -8370,7 +8386,9 @@
         <f t="shared" si="11"/>
         <v>0.47929447852760709</v>
       </c>
-      <c r="G117" s="30"/>
+      <c r="G117" s="30">
+        <v>42795</v>
+      </c>
       <c r="H117" s="30">
         <v>42795</v>
       </c>
@@ -8399,7 +8417,9 @@
         <f t="shared" si="11"/>
         <v>0.48849693251533716</v>
       </c>
-      <c r="G118" s="30"/>
+      <c r="G118" s="30">
+        <v>42795</v>
+      </c>
       <c r="H118" s="30">
         <v>42795</v>
       </c>
@@ -8428,7 +8448,9 @@
         <f t="shared" si="11"/>
         <v>0.49079754601226966</v>
       </c>
-      <c r="G119" s="30"/>
+      <c r="G119" s="30">
+        <v>42795</v>
+      </c>
       <c r="H119" s="30">
         <v>42795</v>
       </c>
@@ -8457,7 +8479,9 @@
         <f t="shared" si="11"/>
         <v>0.49693251533742305</v>
       </c>
-      <c r="G120" s="30"/>
+      <c r="G120" s="30">
+        <v>42795</v>
+      </c>
       <c r="H120" s="30">
         <v>42795</v>
       </c>
@@ -8486,7 +8510,9 @@
         <f t="shared" si="11"/>
         <v>0.49923312883435556</v>
       </c>
-      <c r="G121" s="30"/>
+      <c r="G121" s="30">
+        <v>42795</v>
+      </c>
       <c r="H121" s="30">
         <v>42795</v>
       </c>
@@ -8515,7 +8541,9 @@
         <f t="shared" si="11"/>
         <v>0.50766871165644145</v>
       </c>
-      <c r="G122" s="30"/>
+      <c r="G122" s="30">
+        <v>42795</v>
+      </c>
       <c r="H122" s="30">
         <v>42795</v>
       </c>
@@ -8544,7 +8572,9 @@
         <f t="shared" si="11"/>
         <v>0.50996932515337401</v>
       </c>
-      <c r="G123" s="30"/>
+      <c r="G123" s="30">
+        <v>42795</v>
+      </c>
       <c r="H123" s="30">
         <v>42795</v>
       </c>
@@ -8573,7 +8603,9 @@
         <f t="shared" si="11"/>
         <v>0.51917177914110402</v>
       </c>
-      <c r="G124" s="30"/>
+      <c r="G124" s="30">
+        <v>42795</v>
+      </c>
       <c r="H124" s="30">
         <v>42795</v>
       </c>
@@ -8602,17 +8634,19 @@
         <f t="shared" si="11"/>
         <v>0.52147239263803657</v>
       </c>
-      <c r="G125" s="30"/>
+      <c r="G125" s="30">
+        <v>42795</v>
+      </c>
       <c r="H125" s="30">
         <v>42795</v>
       </c>
-      <c r="I125" s="9" t="str">
+      <c r="I125" s="9">
         <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="J125" s="38" t="str">
+        <v>114</v>
+      </c>
+      <c r="J125" s="38">
         <f t="shared" si="13"/>
-        <v/>
+        <v>1.9</v>
       </c>
     </row>
     <row r="126" spans="1:10" ht="21" thickBot="1">
@@ -8664,7 +8698,7 @@
       </c>
       <c r="G127" s="30"/>
       <c r="H127" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I127" s="9" t="str">
         <f t="shared" si="12"/>
@@ -8693,7 +8727,7 @@
       </c>
       <c r="G128" s="30"/>
       <c r="H128" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I128" s="9" t="str">
         <f t="shared" si="12"/>
@@ -8722,7 +8756,7 @@
       </c>
       <c r="G129" s="30"/>
       <c r="H129" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I129" s="9" t="str">
         <f t="shared" si="12"/>
@@ -8751,7 +8785,7 @@
       </c>
       <c r="G130" s="30"/>
       <c r="H130" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I130" s="9" t="str">
         <f t="shared" si="12"/>
@@ -8780,7 +8814,7 @@
       </c>
       <c r="G131" s="30"/>
       <c r="H131" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I131" s="9" t="str">
         <f t="shared" si="12"/>
@@ -8809,7 +8843,7 @@
       </c>
       <c r="G132" s="30"/>
       <c r="H132" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I132" s="9" t="str">
         <f t="shared" si="12"/>
@@ -8838,7 +8872,7 @@
       </c>
       <c r="G133" s="30"/>
       <c r="H133" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I133" s="9" t="str">
         <f t="shared" si="12"/>
@@ -8867,7 +8901,7 @@
       </c>
       <c r="G134" s="30"/>
       <c r="H134" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I134" s="9" t="str">
         <f t="shared" si="12"/>
@@ -8896,7 +8930,7 @@
       </c>
       <c r="G135" s="30"/>
       <c r="H135" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I135" s="9" t="str">
         <f t="shared" ref="I135:I198" si="19">IF(H135="", "", IF(ISBLANK(H136), IF(H135&lt;&gt;H137, SUMIF(H:H,H135,C:C), ""), IF(H135&lt;&gt;H136, SUMIF(H:H,H135,C:C), "")))</f>
@@ -8925,7 +8959,7 @@
       </c>
       <c r="G136" s="30"/>
       <c r="H136" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I136" s="9" t="str">
         <f t="shared" si="19"/>
@@ -8954,7 +8988,7 @@
       </c>
       <c r="G137" s="30"/>
       <c r="H137" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I137" s="9" t="str">
         <f t="shared" si="19"/>
@@ -8983,7 +9017,7 @@
       </c>
       <c r="G138" s="30"/>
       <c r="H138" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I138" s="9" t="str">
         <f t="shared" si="19"/>
@@ -9012,7 +9046,7 @@
       </c>
       <c r="G139" s="30"/>
       <c r="H139" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I139" s="9" t="str">
         <f t="shared" si="19"/>
@@ -9041,7 +9075,7 @@
       </c>
       <c r="G140" s="30"/>
       <c r="H140" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I140" s="9" t="str">
         <f t="shared" si="19"/>
@@ -9070,7 +9104,7 @@
       </c>
       <c r="G141" s="30"/>
       <c r="H141" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I141" s="9" t="str">
         <f t="shared" si="19"/>
@@ -9099,7 +9133,7 @@
       </c>
       <c r="G142" s="30"/>
       <c r="H142" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I142" s="9" t="str">
         <f t="shared" si="19"/>
@@ -9128,7 +9162,7 @@
       </c>
       <c r="G143" s="30"/>
       <c r="H143" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I143" s="9" t="str">
         <f t="shared" si="19"/>
@@ -9188,7 +9222,7 @@
       </c>
       <c r="G145" s="30"/>
       <c r="H145" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I145" s="9" t="str">
         <f t="shared" si="19"/>
@@ -9217,7 +9251,7 @@
       </c>
       <c r="G146" s="30"/>
       <c r="H146" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I146" s="9" t="str">
         <f t="shared" si="19"/>
@@ -9246,7 +9280,7 @@
       </c>
       <c r="G147" s="30"/>
       <c r="H147" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I147" s="9" t="str">
         <f t="shared" si="19"/>
@@ -9275,7 +9309,7 @@
       </c>
       <c r="G148" s="30"/>
       <c r="H148" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I148" s="9" t="str">
         <f t="shared" si="19"/>
@@ -9304,7 +9338,7 @@
       </c>
       <c r="G149" s="30"/>
       <c r="H149" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I149" s="9" t="str">
         <f t="shared" si="19"/>
@@ -9333,7 +9367,7 @@
       </c>
       <c r="G150" s="30"/>
       <c r="H150" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I150" s="9" t="str">
         <f t="shared" si="19"/>
@@ -9362,7 +9396,7 @@
       </c>
       <c r="G151" s="30"/>
       <c r="H151" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I151" s="9" t="str">
         <f t="shared" si="19"/>
@@ -9391,7 +9425,7 @@
       </c>
       <c r="G152" s="30"/>
       <c r="H152" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I152" s="9" t="str">
         <f t="shared" si="19"/>
@@ -9420,7 +9454,7 @@
       </c>
       <c r="G153" s="30"/>
       <c r="H153" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I153" s="9" t="str">
         <f t="shared" si="19"/>
@@ -9449,7 +9483,7 @@
       </c>
       <c r="G154" s="30"/>
       <c r="H154" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I154" s="9" t="str">
         <f t="shared" si="19"/>
@@ -9478,7 +9512,7 @@
       </c>
       <c r="G155" s="30"/>
       <c r="H155" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I155" s="9" t="str">
         <f t="shared" si="19"/>
@@ -9507,7 +9541,7 @@
       </c>
       <c r="G156" s="30"/>
       <c r="H156" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I156" s="9" t="str">
         <f t="shared" si="19"/>
@@ -9536,7 +9570,7 @@
       </c>
       <c r="G157" s="30"/>
       <c r="H157" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I157" s="9" t="str">
         <f t="shared" si="19"/>
@@ -9565,7 +9599,7 @@
       </c>
       <c r="G158" s="30"/>
       <c r="H158" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I158" s="9" t="str">
         <f t="shared" si="19"/>
@@ -9625,7 +9659,7 @@
       </c>
       <c r="G160" s="30"/>
       <c r="H160" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I160" s="9" t="str">
         <f t="shared" si="19"/>
@@ -9654,7 +9688,7 @@
       </c>
       <c r="G161" s="30"/>
       <c r="H161" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I161" s="9" t="str">
         <f t="shared" si="19"/>
@@ -9683,7 +9717,7 @@
       </c>
       <c r="G162" s="30"/>
       <c r="H162" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I162" s="9" t="str">
         <f t="shared" si="19"/>
@@ -9712,7 +9746,7 @@
       </c>
       <c r="G163" s="30"/>
       <c r="H163" s="30">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="I163" s="9" t="str">
         <f t="shared" si="19"/>
@@ -9741,15 +9775,15 @@
       </c>
       <c r="G164" s="30"/>
       <c r="H164" s="30">
-        <v>42795</v>
-      </c>
-      <c r="I164" s="9">
+        <v>42796</v>
+      </c>
+      <c r="I164" s="9" t="str">
         <f t="shared" si="19"/>
-        <v>353</v>
-      </c>
-      <c r="J164" s="38">
+        <v/>
+      </c>
+      <c r="J164" s="38" t="str">
         <f t="shared" si="20"/>
-        <v>5.8833333333333337</v>
+        <v/>
       </c>
     </row>
     <row r="165" spans="1:10" outlineLevel="1">
@@ -11083,13 +11117,13 @@
       <c r="H210" s="30">
         <v>42796</v>
       </c>
-      <c r="I210" s="9" t="str">
+      <c r="I210" s="9">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-      <c r="J210" s="38" t="str">
+        <v>517</v>
+      </c>
+      <c r="J210" s="38">
         <f t="shared" si="28"/>
-        <v/>
+        <v>8.6166666666666671</v>
       </c>
     </row>
     <row r="211" spans="1:10" ht="21" thickBot="1">
@@ -11141,7 +11175,7 @@
       </c>
       <c r="G212" s="30"/>
       <c r="H212" s="30">
-        <v>42796</v>
+        <v>42797</v>
       </c>
       <c r="I212" s="9" t="str">
         <f t="shared" si="27"/>
@@ -11170,7 +11204,7 @@
       </c>
       <c r="G213" s="30"/>
       <c r="H213" s="30">
-        <v>42796</v>
+        <v>42797</v>
       </c>
       <c r="I213" s="9" t="str">
         <f t="shared" si="27"/>
@@ -11199,7 +11233,7 @@
       </c>
       <c r="G214" s="30"/>
       <c r="H214" s="30">
-        <v>42796</v>
+        <v>42797</v>
       </c>
       <c r="I214" s="9" t="str">
         <f t="shared" si="27"/>
@@ -11228,7 +11262,7 @@
       </c>
       <c r="G215" s="30"/>
       <c r="H215" s="30">
-        <v>42796</v>
+        <v>42797</v>
       </c>
       <c r="I215" s="9" t="str">
         <f t="shared" si="27"/>
@@ -11257,7 +11291,7 @@
       </c>
       <c r="G216" s="30"/>
       <c r="H216" s="30">
-        <v>42796</v>
+        <v>42797</v>
       </c>
       <c r="I216" s="9" t="str">
         <f t="shared" si="27"/>
@@ -11317,7 +11351,7 @@
       </c>
       <c r="G218" s="30"/>
       <c r="H218" s="30">
-        <v>42796</v>
+        <v>42797</v>
       </c>
       <c r="I218" s="9" t="str">
         <f t="shared" si="27"/>
@@ -11346,7 +11380,7 @@
       </c>
       <c r="G219" s="30"/>
       <c r="H219" s="30">
-        <v>42796</v>
+        <v>42797</v>
       </c>
       <c r="I219" s="9" t="str">
         <f t="shared" si="27"/>
@@ -11375,7 +11409,7 @@
       </c>
       <c r="G220" s="30"/>
       <c r="H220" s="30">
-        <v>42796</v>
+        <v>42797</v>
       </c>
       <c r="I220" s="9" t="str">
         <f t="shared" si="27"/>
@@ -11404,7 +11438,7 @@
       </c>
       <c r="G221" s="30"/>
       <c r="H221" s="30">
-        <v>42796</v>
+        <v>42797</v>
       </c>
       <c r="I221" s="9" t="str">
         <f t="shared" si="27"/>
@@ -11433,7 +11467,7 @@
       </c>
       <c r="G222" s="30"/>
       <c r="H222" s="30">
-        <v>42796</v>
+        <v>42797</v>
       </c>
       <c r="I222" s="9" t="str">
         <f t="shared" si="27"/>
@@ -11462,15 +11496,15 @@
       </c>
       <c r="G223" s="30"/>
       <c r="H223" s="30">
-        <v>42796</v>
-      </c>
-      <c r="I223" s="9">
+        <v>42797</v>
+      </c>
+      <c r="I223" s="9" t="str">
         <f t="shared" si="27"/>
-        <v>334</v>
-      </c>
-      <c r="J223" s="38">
+        <v/>
+      </c>
+      <c r="J223" s="38" t="str">
         <f t="shared" si="28"/>
-        <v>5.5666666666666664</v>
+        <v/>
       </c>
     </row>
     <row r="224" spans="1:10" ht="21" thickBot="1">
@@ -12049,11 +12083,11 @@
       </c>
       <c r="I243" s="9">
         <f t="shared" si="27"/>
-        <v>51</v>
+        <v>107</v>
       </c>
       <c r="J243" s="38">
         <f t="shared" si="28"/>
-        <v>0.85</v>
+        <v>1.7833333333333334</v>
       </c>
     </row>
     <row r="245" spans="2:10" ht="15.75" thickBot="1">

</xml_diff>

<commit_message>
Section 10: Lighting completed
</commit_message>
<xml_diff>
--- a/Unity Certification Course (Udemy) - Video Listing.xlsx
+++ b/Unity Certification Course (Udemy) - Video Listing.xlsx
@@ -4804,8 +4804,8 @@
   <dimension ref="A1:J246"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G125" sqref="G125"/>
+      <pane ySplit="3" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G143" sqref="G143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -4833,7 +4833,7 @@
       </c>
       <c r="F1" s="34">
         <f>SUMIF(G4:G244, "&gt;0", C4:C244)</f>
-        <v>680</v>
+        <v>802</v>
       </c>
       <c r="G1" s="35">
         <f>+C245</f>
@@ -4841,7 +4841,7 @@
       </c>
       <c r="H1" s="36">
         <f>+F1/G1</f>
-        <v>0.5214723926380368</v>
+        <v>0.61503067484662577</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -8666,7 +8666,7 @@
       </c>
       <c r="G126" s="41" t="str">
         <f>IF(COUNTA(G127:G143)=COUNTA(B127:B143), "COMPLETE", "")</f>
-        <v/>
+        <v>COMPLETE</v>
       </c>
       <c r="I126" s="9" t="str">
         <f t="shared" si="12"/>
@@ -8696,7 +8696,9 @@
         <f t="shared" si="11"/>
         <v>0.5222392638036808</v>
       </c>
-      <c r="G127" s="30"/>
+      <c r="G127" s="30">
+        <v>42796</v>
+      </c>
       <c r="H127" s="30">
         <v>42796</v>
       </c>
@@ -8725,7 +8727,9 @@
         <f t="shared" si="11"/>
         <v>0.53220858895705503</v>
       </c>
-      <c r="G128" s="30"/>
+      <c r="G128" s="30">
+        <v>42796</v>
+      </c>
       <c r="H128" s="30">
         <v>42796</v>
       </c>
@@ -8754,7 +8758,9 @@
         <f t="shared" si="11"/>
         <v>0.53450920245398759</v>
       </c>
-      <c r="G129" s="30"/>
+      <c r="G129" s="30">
+        <v>42796</v>
+      </c>
       <c r="H129" s="30">
         <v>42796</v>
       </c>
@@ -8783,7 +8789,9 @@
         <f t="shared" si="11"/>
         <v>0.54601226993865015</v>
       </c>
-      <c r="G130" s="30"/>
+      <c r="G130" s="30">
+        <v>42796</v>
+      </c>
       <c r="H130" s="30">
         <v>42796</v>
       </c>
@@ -8812,7 +8820,9 @@
         <f t="shared" si="11"/>
         <v>0.54831288343558271</v>
       </c>
-      <c r="G131" s="30"/>
+      <c r="G131" s="30">
+        <v>42796</v>
+      </c>
       <c r="H131" s="30">
         <v>42796</v>
       </c>
@@ -8841,7 +8851,9 @@
         <f t="shared" si="11"/>
         <v>0.55674846625766861</v>
       </c>
-      <c r="G132" s="30"/>
+      <c r="G132" s="30">
+        <v>42796</v>
+      </c>
       <c r="H132" s="30">
         <v>42796</v>
       </c>
@@ -8870,7 +8882,9 @@
         <f t="shared" si="11"/>
         <v>0.55904907975460116</v>
       </c>
-      <c r="G133" s="30"/>
+      <c r="G133" s="30">
+        <v>42796</v>
+      </c>
       <c r="H133" s="30">
         <v>42796</v>
       </c>
@@ -8899,7 +8913,9 @@
         <f t="shared" ref="F134:F197" si="18">F133+(C134/$C$245)</f>
         <v>0.56901840490797539</v>
       </c>
-      <c r="G134" s="30"/>
+      <c r="G134" s="30">
+        <v>42796</v>
+      </c>
       <c r="H134" s="30">
         <v>42796</v>
       </c>
@@ -8928,7 +8944,9 @@
         <f t="shared" si="18"/>
         <v>0.57131901840490795</v>
       </c>
-      <c r="G135" s="30"/>
+      <c r="G135" s="30">
+        <v>42796</v>
+      </c>
       <c r="H135" s="30">
         <v>42796</v>
       </c>
@@ -8957,7 +8975,9 @@
         <f t="shared" si="18"/>
         <v>0.57975460122699385</v>
       </c>
-      <c r="G136" s="30"/>
+      <c r="G136" s="30">
+        <v>42796</v>
+      </c>
       <c r="H136" s="30">
         <v>42796</v>
       </c>
@@ -8986,7 +9006,9 @@
         <f t="shared" si="18"/>
         <v>0.58205521472392641</v>
       </c>
-      <c r="G137" s="30"/>
+      <c r="G137" s="30">
+        <v>42796</v>
+      </c>
       <c r="H137" s="30">
         <v>42796</v>
       </c>
@@ -9015,7 +9037,9 @@
         <f t="shared" si="18"/>
         <v>0.5904907975460123</v>
       </c>
-      <c r="G138" s="30"/>
+      <c r="G138" s="30">
+        <v>42796</v>
+      </c>
       <c r="H138" s="30">
         <v>42796</v>
       </c>
@@ -9044,7 +9068,9 @@
         <f t="shared" si="18"/>
         <v>0.59279141104294486</v>
       </c>
-      <c r="G139" s="30"/>
+      <c r="G139" s="30">
+        <v>42796</v>
+      </c>
       <c r="H139" s="30">
         <v>42796</v>
       </c>
@@ -9073,7 +9099,9 @@
         <f t="shared" si="18"/>
         <v>0.60046012269938653</v>
       </c>
-      <c r="G140" s="30"/>
+      <c r="G140" s="30">
+        <v>42796</v>
+      </c>
       <c r="H140" s="30">
         <v>42796</v>
       </c>
@@ -9102,7 +9130,9 @@
         <f t="shared" si="18"/>
         <v>0.60276073619631909</v>
       </c>
-      <c r="G141" s="30"/>
+      <c r="G141" s="30">
+        <v>42796</v>
+      </c>
       <c r="H141" s="30">
         <v>42796</v>
       </c>
@@ -9131,7 +9161,9 @@
         <f t="shared" si="18"/>
         <v>0.61273006134969332</v>
       </c>
-      <c r="G142" s="30"/>
+      <c r="G142" s="30">
+        <v>42796</v>
+      </c>
       <c r="H142" s="30">
         <v>42796</v>
       </c>
@@ -9160,7 +9192,9 @@
         <f t="shared" si="18"/>
         <v>0.61503067484662588</v>
       </c>
-      <c r="G143" s="30"/>
+      <c r="G143" s="30">
+        <v>42796</v>
+      </c>
       <c r="H143" s="30">
         <v>42796</v>
       </c>
@@ -11117,13 +11151,13 @@
       <c r="H210" s="30">
         <v>42796</v>
       </c>
-      <c r="I210" s="9">
+      <c r="I210" s="9" t="str">
         <f t="shared" si="27"/>
-        <v>517</v>
-      </c>
-      <c r="J210" s="38">
+        <v/>
+      </c>
+      <c r="J210" s="38" t="str">
         <f t="shared" si="28"/>
-        <v>8.6166666666666671</v>
+        <v/>
       </c>
     </row>
     <row r="211" spans="1:10" ht="21" thickBot="1">
@@ -11175,7 +11209,7 @@
       </c>
       <c r="G212" s="30"/>
       <c r="H212" s="30">
-        <v>42797</v>
+        <v>42796</v>
       </c>
       <c r="I212" s="9" t="str">
         <f t="shared" si="27"/>
@@ -11204,7 +11238,7 @@
       </c>
       <c r="G213" s="30"/>
       <c r="H213" s="30">
-        <v>42797</v>
+        <v>42796</v>
       </c>
       <c r="I213" s="9" t="str">
         <f t="shared" si="27"/>
@@ -11233,7 +11267,7 @@
       </c>
       <c r="G214" s="30"/>
       <c r="H214" s="30">
-        <v>42797</v>
+        <v>42796</v>
       </c>
       <c r="I214" s="9" t="str">
         <f t="shared" si="27"/>
@@ -11262,7 +11296,7 @@
       </c>
       <c r="G215" s="30"/>
       <c r="H215" s="30">
-        <v>42797</v>
+        <v>42796</v>
       </c>
       <c r="I215" s="9" t="str">
         <f t="shared" si="27"/>
@@ -11291,7 +11325,7 @@
       </c>
       <c r="G216" s="30"/>
       <c r="H216" s="30">
-        <v>42797</v>
+        <v>42796</v>
       </c>
       <c r="I216" s="9" t="str">
         <f t="shared" si="27"/>
@@ -11351,7 +11385,7 @@
       </c>
       <c r="G218" s="30"/>
       <c r="H218" s="30">
-        <v>42797</v>
+        <v>42796</v>
       </c>
       <c r="I218" s="9" t="str">
         <f t="shared" si="27"/>
@@ -11380,7 +11414,7 @@
       </c>
       <c r="G219" s="30"/>
       <c r="H219" s="30">
-        <v>42797</v>
+        <v>42796</v>
       </c>
       <c r="I219" s="9" t="str">
         <f t="shared" si="27"/>
@@ -11409,7 +11443,7 @@
       </c>
       <c r="G220" s="30"/>
       <c r="H220" s="30">
-        <v>42797</v>
+        <v>42796</v>
       </c>
       <c r="I220" s="9" t="str">
         <f t="shared" si="27"/>
@@ -11438,7 +11472,7 @@
       </c>
       <c r="G221" s="30"/>
       <c r="H221" s="30">
-        <v>42797</v>
+        <v>42796</v>
       </c>
       <c r="I221" s="9" t="str">
         <f t="shared" si="27"/>
@@ -11467,7 +11501,7 @@
       </c>
       <c r="G222" s="30"/>
       <c r="H222" s="30">
-        <v>42797</v>
+        <v>42796</v>
       </c>
       <c r="I222" s="9" t="str">
         <f t="shared" si="27"/>
@@ -11496,15 +11530,15 @@
       </c>
       <c r="G223" s="30"/>
       <c r="H223" s="30">
-        <v>42797</v>
-      </c>
-      <c r="I223" s="9" t="str">
+        <v>42796</v>
+      </c>
+      <c r="I223" s="9">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-      <c r="J223" s="38" t="str">
+        <v>573</v>
+      </c>
+      <c r="J223" s="38">
         <f t="shared" si="28"/>
-        <v/>
+        <v>9.5500000000000007</v>
       </c>
     </row>
     <row r="224" spans="1:10" ht="21" thickBot="1">
@@ -12083,11 +12117,11 @@
       </c>
       <c r="I243" s="9">
         <f t="shared" si="27"/>
-        <v>107</v>
+        <v>51</v>
       </c>
       <c r="J243" s="38">
         <f t="shared" si="28"/>
-        <v>1.7833333333333334</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="245" spans="2:10" ht="15.75" thickBot="1">

</xml_diff>

<commit_message>
Section 11: Physics completed
</commit_message>
<xml_diff>
--- a/Unity Certification Course (Udemy) - Video Listing.xlsx
+++ b/Unity Certification Course (Udemy) - Video Listing.xlsx
@@ -2625,7 +2625,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1189" uniqueCount="365">
   <si>
     <t>VIDEO NAME</t>
   </si>
@@ -3938,6 +3938,9 @@
   </si>
   <si>
     <t>Quiz 65: Audio Source » Audio Properties 2/2   0:00</t>
+  </si>
+  <si>
+    <t>skipped-no time</t>
   </si>
 </sst>
 </file>
@@ -4801,11 +4804,11 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J246"/>
+  <dimension ref="A1:K246"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G143" sqref="G143"/>
+      <pane ySplit="3" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G160" sqref="G160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -4833,15 +4836,15 @@
       </c>
       <c r="F1" s="34">
         <f>SUMIF(G4:G244, "&gt;0", C4:C244)</f>
-        <v>802</v>
+        <v>886</v>
       </c>
       <c r="G1" s="35">
         <f>+C245</f>
-        <v>1304</v>
+        <v>1296</v>
       </c>
       <c r="H1" s="36">
         <f>+F1/G1</f>
-        <v>0.61503067484662577</v>
+        <v>0.68364197530864201</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -4852,7 +4855,7 @@
       <c r="C2" s="4"/>
       <c r="G2" s="38">
         <f>+G1/60</f>
-        <v>21.733333333333334</v>
+        <v>21.6</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="45.75" thickBot="1">
@@ -4912,7 +4915,7 @@
       </c>
       <c r="F5" s="15">
         <f>F4+(C5/$C$245)</f>
-        <v>1.5337423312883436E-3</v>
+        <v>1.5432098765432098E-3</v>
       </c>
       <c r="G5" s="30">
         <v>42789</v>
@@ -4943,7 +4946,7 @@
       </c>
       <c r="F6" s="15">
         <f t="shared" ref="F6:F69" si="2">F5+(C6/$C$245)</f>
-        <v>3.0674846625766872E-3</v>
+        <v>3.0864197530864196E-3</v>
       </c>
       <c r="G6" s="30">
         <v>42789</v>
@@ -4974,7 +4977,7 @@
       </c>
       <c r="F7" s="15">
         <f t="shared" si="2"/>
-        <v>8.4355828220858894E-3</v>
+        <v>8.4876543209876538E-3</v>
       </c>
       <c r="G7" s="30">
         <v>42789</v>
@@ -5005,7 +5008,7 @@
       </c>
       <c r="F8" s="15">
         <f t="shared" si="2"/>
-        <v>1.2269938650306749E-2</v>
+        <v>1.2345679012345678E-2</v>
       </c>
       <c r="G8" s="30">
         <v>42789</v>
@@ -5035,7 +5038,7 @@
       <c r="E9" s="27"/>
       <c r="F9" s="29">
         <f t="shared" si="2"/>
-        <v>1.2269938650306749E-2</v>
+        <v>1.2345679012345678E-2</v>
       </c>
       <c r="G9" s="41" t="str">
         <f>IF(COUNTA(G10:G32)=COUNTA(B10:B32), "COMPLETE", "")</f>
@@ -5067,7 +5070,7 @@
       </c>
       <c r="F10" s="15">
         <f t="shared" si="2"/>
-        <v>1.3036809815950921E-2</v>
+        <v>1.3117283950617283E-2</v>
       </c>
       <c r="G10" s="30">
         <v>42789</v>
@@ -5098,7 +5101,7 @@
       </c>
       <c r="F11" s="15">
         <f t="shared" si="2"/>
-        <v>1.6871165644171779E-2</v>
+        <v>1.6975308641975308E-2</v>
       </c>
       <c r="G11" s="30">
         <v>42789</v>
@@ -5129,7 +5132,7 @@
       </c>
       <c r="F12" s="15">
         <f t="shared" si="2"/>
-        <v>2.3773006134969327E-2</v>
+        <v>2.3919753086419752E-2</v>
       </c>
       <c r="G12" s="30">
         <v>42789</v>
@@ -5160,7 +5163,7 @@
       </c>
       <c r="F13" s="15">
         <f t="shared" si="2"/>
-        <v>2.6073619631901843E-2</v>
+        <v>2.6234567901234566E-2</v>
       </c>
       <c r="G13" s="30">
         <v>42789</v>
@@ -5191,7 +5194,7 @@
       </c>
       <c r="F14" s="15">
         <f t="shared" si="2"/>
-        <v>3.0674846625766874E-2</v>
+        <v>3.0864197530864196E-2</v>
       </c>
       <c r="G14" s="30">
         <v>42789</v>
@@ -5222,7 +5225,7 @@
       </c>
       <c r="F15" s="15">
         <f t="shared" si="2"/>
-        <v>3.297546012269939E-2</v>
+        <v>3.3179012345679007E-2</v>
       </c>
       <c r="G15" s="30">
         <v>42789</v>
@@ -5253,7 +5256,7 @@
       </c>
       <c r="F16" s="15">
         <f t="shared" si="2"/>
-        <v>4.2177914110429454E-2</v>
+        <v>4.2438271604938266E-2</v>
       </c>
       <c r="G16" s="30">
         <v>42789</v>
@@ -5284,7 +5287,7 @@
       </c>
       <c r="F17" s="15">
         <f t="shared" si="2"/>
-        <v>4.447852760736197E-2</v>
+        <v>4.4753086419753077E-2</v>
       </c>
       <c r="G17" s="30">
         <v>42789</v>
@@ -5315,7 +5318,7 @@
       </c>
       <c r="F18" s="15">
         <f t="shared" si="2"/>
-        <v>5.1380368098159518E-2</v>
+        <v>5.1697530864197525E-2</v>
       </c>
       <c r="G18" s="30">
         <v>42789</v>
@@ -5346,7 +5349,7 @@
       </c>
       <c r="F19" s="15">
         <f t="shared" si="2"/>
-        <v>5.3680981595092034E-2</v>
+        <v>5.4012345679012336E-2</v>
       </c>
       <c r="G19" s="30">
         <v>42789</v>
@@ -5377,7 +5380,7 @@
       </c>
       <c r="F20" s="15">
         <f t="shared" si="2"/>
-        <v>5.6748466257668724E-2</v>
+        <v>5.7098765432098755E-2</v>
       </c>
       <c r="G20" s="30">
         <v>42789</v>
@@ -5408,7 +5411,7 @@
       </c>
       <c r="F21" s="15">
         <f t="shared" si="2"/>
-        <v>5.904907975460124E-2</v>
+        <v>5.9413580246913567E-2</v>
       </c>
       <c r="G21" s="30">
         <v>42789</v>
@@ -5439,7 +5442,7 @@
       </c>
       <c r="F22" s="15">
         <f t="shared" si="2"/>
-        <v>6.5184049079754613E-2</v>
+        <v>6.5586419753086406E-2</v>
       </c>
       <c r="G22" s="30">
         <v>42789</v>
@@ -5470,7 +5473,7 @@
       </c>
       <c r="F23" s="15">
         <f t="shared" si="2"/>
-        <v>6.7484662576687129E-2</v>
+        <v>6.7901234567901217E-2</v>
       </c>
       <c r="G23" s="30">
         <v>42789</v>
@@ -5501,7 +5504,7 @@
       </c>
       <c r="F24" s="15">
         <f t="shared" si="2"/>
-        <v>7.7453987730061361E-2</v>
+        <v>7.7932098765432084E-2</v>
       </c>
       <c r="G24" s="30">
         <v>42789</v>
@@ -5532,7 +5535,7 @@
       </c>
       <c r="F25" s="15">
         <f t="shared" si="2"/>
-        <v>7.9754601226993876E-2</v>
+        <v>8.0246913580246895E-2</v>
       </c>
       <c r="G25" s="30">
         <v>42789</v>
@@ -5563,7 +5566,7 @@
       </c>
       <c r="F26" s="15">
         <f t="shared" si="2"/>
-        <v>8.6656441717791424E-2</v>
+        <v>8.7191358024691343E-2</v>
       </c>
       <c r="G26" s="30">
         <v>42789</v>
@@ -5594,7 +5597,7 @@
       </c>
       <c r="F27" s="15">
         <f t="shared" si="2"/>
-        <v>8.895705521472394E-2</v>
+        <v>8.9506172839506154E-2</v>
       </c>
       <c r="G27" s="30">
         <v>42789</v>
@@ -5625,7 +5628,7 @@
       </c>
       <c r="F28" s="15">
         <f t="shared" si="2"/>
-        <v>9.8159509202454004E-2</v>
+        <v>9.8765432098765413E-2</v>
       </c>
       <c r="G28" s="30">
         <v>42789</v>
@@ -5656,7 +5659,7 @@
       </c>
       <c r="F29" s="15">
         <f t="shared" si="2"/>
-        <v>0.10046012269938652</v>
+        <v>0.10108024691358022</v>
       </c>
       <c r="G29" s="30">
         <v>42789</v>
@@ -5687,7 +5690,7 @@
       </c>
       <c r="F30" s="15">
         <f t="shared" si="2"/>
-        <v>0.10122699386503069</v>
+        <v>0.10185185185185183</v>
       </c>
       <c r="G30" s="30">
         <v>42789</v>
@@ -5718,7 +5721,7 @@
       </c>
       <c r="F31" s="15">
         <f t="shared" si="2"/>
-        <v>0.1035276073619632</v>
+        <v>0.10416666666666664</v>
       </c>
       <c r="G31" s="30">
         <v>42789</v>
@@ -5749,7 +5752,7 @@
       </c>
       <c r="F32" s="15">
         <f t="shared" si="2"/>
-        <v>0.10429447852760737</v>
+        <v>0.10493827160493825</v>
       </c>
       <c r="G32" s="30">
         <v>42789</v>
@@ -5779,7 +5782,7 @@
       <c r="E33" s="27"/>
       <c r="F33" s="29">
         <f t="shared" si="2"/>
-        <v>0.10429447852760737</v>
+        <v>0.10493827160493825</v>
       </c>
       <c r="G33" s="41" t="str">
         <f>IF(COUNTA(G34:G40)=COUNTA(B34:B40), "COMPLETE", "")</f>
@@ -5811,7 +5814,7 @@
       </c>
       <c r="F34" s="15">
         <f t="shared" si="2"/>
-        <v>0.10506134969325154</v>
+        <v>0.10570987654320986</v>
       </c>
       <c r="G34" s="30">
         <v>42790</v>
@@ -5842,7 +5845,7 @@
       </c>
       <c r="F35" s="15">
         <f t="shared" si="2"/>
-        <v>0.1142638036809816</v>
+        <v>0.11496913580246912</v>
       </c>
       <c r="G35" s="30">
         <v>42791</v>
@@ -5873,7 +5876,7 @@
       </c>
       <c r="F36" s="15">
         <f t="shared" si="2"/>
-        <v>0.11656441717791412</v>
+        <v>0.11728395061728393</v>
       </c>
       <c r="G36" s="30">
         <v>42791</v>
@@ -5904,7 +5907,7 @@
       </c>
       <c r="F37" s="15">
         <f t="shared" si="2"/>
-        <v>0.12423312883435583</v>
+        <v>0.12499999999999997</v>
       </c>
       <c r="G37" s="30">
         <v>42791</v>
@@ -5935,7 +5938,7 @@
       </c>
       <c r="F38" s="15">
         <f t="shared" si="2"/>
-        <v>0.12653374233128833</v>
+        <v>0.1273148148148148</v>
       </c>
       <c r="G38" s="30">
         <v>42791</v>
@@ -5966,7 +5969,7 @@
       </c>
       <c r="F39" s="15">
         <f t="shared" si="2"/>
-        <v>0.13496932515337423</v>
+        <v>0.13580246913580246</v>
       </c>
       <c r="G39" s="30">
         <v>42791</v>
@@ -5997,7 +6000,7 @@
       </c>
       <c r="F40" s="15">
         <f t="shared" si="2"/>
-        <v>0.13726993865030673</v>
+        <v>0.13811728395061729</v>
       </c>
       <c r="G40" s="30">
         <v>42791</v>
@@ -6027,7 +6030,7 @@
       <c r="E41" s="27"/>
       <c r="F41" s="29">
         <f t="shared" si="2"/>
-        <v>0.13726993865030673</v>
+        <v>0.13811728395061729</v>
       </c>
       <c r="G41" s="41" t="str">
         <f>IF(COUNTA(G42:G45)=COUNTA(B42:B45), "COMPLETE", "")</f>
@@ -6059,7 +6062,7 @@
       </c>
       <c r="F42" s="15">
         <f t="shared" si="2"/>
-        <v>0.14723926380368096</v>
+        <v>0.14814814814814814</v>
       </c>
       <c r="G42" s="30">
         <v>42791</v>
@@ -6090,7 +6093,7 @@
       </c>
       <c r="F43" s="15">
         <f t="shared" si="2"/>
-        <v>0.14953987730061347</v>
+        <v>0.15046296296296297</v>
       </c>
       <c r="G43" s="30">
         <v>42791</v>
@@ -6121,7 +6124,7 @@
       </c>
       <c r="F44" s="15">
         <f t="shared" si="2"/>
-        <v>0.16027607361963186</v>
+        <v>0.16126543209876543</v>
       </c>
       <c r="G44" s="30">
         <v>42791</v>
@@ -6152,7 +6155,7 @@
       </c>
       <c r="F45" s="15">
         <f t="shared" si="2"/>
-        <v>0.16257668711656437</v>
+        <v>0.16358024691358025</v>
       </c>
       <c r="G45" s="30">
         <v>42791</v>
@@ -6182,7 +6185,7 @@
       <c r="E46" s="27"/>
       <c r="F46" s="29">
         <f t="shared" si="2"/>
-        <v>0.16257668711656437</v>
+        <v>0.16358024691358025</v>
       </c>
       <c r="G46" s="41" t="str">
         <f>IF(COUNTA(G47:G60)=COUNTA(B47:B60), "COMPLETE", "")</f>
@@ -6214,7 +6217,7 @@
       </c>
       <c r="F47" s="15">
         <f t="shared" si="2"/>
-        <v>0.16334355828220853</v>
+        <v>0.16435185185185186</v>
       </c>
       <c r="G47" s="30">
         <v>42791</v>
@@ -6245,7 +6248,7 @@
       </c>
       <c r="F48" s="15">
         <f t="shared" si="2"/>
-        <v>0.17177914110429443</v>
+        <v>0.17283950617283952</v>
       </c>
       <c r="G48" s="30">
         <v>42791</v>
@@ -6276,7 +6279,7 @@
       </c>
       <c r="F49" s="15">
         <f t="shared" si="2"/>
-        <v>0.17407975460122693</v>
+        <v>0.17515432098765435</v>
       </c>
       <c r="G49" s="30">
         <v>42791</v>
@@ -6307,7 +6310,7 @@
       </c>
       <c r="F50" s="15">
         <f t="shared" si="2"/>
-        <v>0.1802147239263803</v>
+        <v>0.18132716049382719</v>
       </c>
       <c r="G50" s="30">
         <v>42791</v>
@@ -6338,7 +6341,7 @@
       </c>
       <c r="F51" s="15">
         <f t="shared" si="2"/>
-        <v>0.1825153374233128</v>
+        <v>0.18364197530864201</v>
       </c>
       <c r="G51" s="30">
         <v>42791</v>
@@ -6369,7 +6372,7 @@
       </c>
       <c r="F52" s="15">
         <f t="shared" si="2"/>
-        <v>0.19018404907975453</v>
+        <v>0.19135802469135807</v>
       </c>
       <c r="G52" s="30">
         <v>42791</v>
@@ -6400,7 +6403,7 @@
       </c>
       <c r="F53" s="15">
         <f t="shared" si="2"/>
-        <v>0.19248466257668703</v>
+        <v>0.19367283950617289</v>
       </c>
       <c r="G53" s="30">
         <v>42791</v>
@@ -6431,7 +6434,7 @@
       </c>
       <c r="F54" s="15">
         <f t="shared" si="2"/>
-        <v>0.2039877300613496</v>
+        <v>0.20524691358024696</v>
       </c>
       <c r="G54" s="30">
         <v>42791</v>
@@ -6462,7 +6465,7 @@
       </c>
       <c r="F55" s="15">
         <f t="shared" si="2"/>
-        <v>0.2062883435582821</v>
+        <v>0.20756172839506179</v>
       </c>
       <c r="G55" s="30">
         <v>42791</v>
@@ -6493,7 +6496,7 @@
       </c>
       <c r="F56" s="15">
         <f t="shared" si="2"/>
-        <v>0.20705521472392627</v>
+        <v>0.2083333333333334</v>
       </c>
       <c r="G56" s="30">
         <v>42791</v>
@@ -6524,7 +6527,7 @@
       </c>
       <c r="F57" s="15">
         <f t="shared" si="2"/>
-        <v>0.21625766871165633</v>
+        <v>0.21759259259259267</v>
       </c>
       <c r="G57" s="30">
         <v>42791</v>
@@ -6555,7 +6558,7 @@
       </c>
       <c r="F58" s="15">
         <f t="shared" si="2"/>
-        <v>0.21855828220858883</v>
+        <v>0.2199074074074075</v>
       </c>
       <c r="G58" s="30">
         <v>42791</v>
@@ -6586,7 +6589,7 @@
       </c>
       <c r="F59" s="15">
         <f t="shared" si="2"/>
-        <v>0.22546012269938637</v>
+        <v>0.22685185185185194</v>
       </c>
       <c r="G59" s="30">
         <v>42791</v>
@@ -6617,7 +6620,7 @@
       </c>
       <c r="F60" s="15">
         <f t="shared" si="2"/>
-        <v>0.22776073619631887</v>
+        <v>0.22916666666666677</v>
       </c>
       <c r="G60" s="30">
         <v>42791</v>
@@ -6647,7 +6650,7 @@
       <c r="E61" s="27"/>
       <c r="F61" s="29">
         <f t="shared" si="2"/>
-        <v>0.22776073619631887</v>
+        <v>0.22916666666666677</v>
       </c>
       <c r="G61" s="41" t="str">
         <f>IF(COUNTA(G62:G71)=COUNTA(B62:B71), "COMPLETE", "")</f>
@@ -6679,7 +6682,7 @@
       </c>
       <c r="F62" s="15">
         <f t="shared" si="2"/>
-        <v>0.22852760736196304</v>
+        <v>0.22993827160493838</v>
       </c>
       <c r="G62" s="30">
         <v>42791</v>
@@ -6710,7 +6713,7 @@
       </c>
       <c r="F63" s="15">
         <f t="shared" si="2"/>
-        <v>0.23542944785276057</v>
+        <v>0.23688271604938282</v>
       </c>
       <c r="G63" s="30">
         <v>42791</v>
@@ -6741,7 +6744,7 @@
       </c>
       <c r="F64" s="15">
         <f t="shared" si="2"/>
-        <v>0.23773006134969307</v>
+        <v>0.23919753086419765</v>
       </c>
       <c r="G64" s="30">
         <v>42791</v>
@@ -6772,7 +6775,7 @@
       </c>
       <c r="F65" s="15">
         <f t="shared" si="2"/>
-        <v>0.24386503067484644</v>
+        <v>0.24537037037037049</v>
       </c>
       <c r="G65" s="30">
         <v>42791</v>
@@ -6803,7 +6806,7 @@
       </c>
       <c r="F66" s="15">
         <f t="shared" si="2"/>
-        <v>0.24616564417177894</v>
+        <v>0.24768518518518531</v>
       </c>
       <c r="G66" s="30">
         <v>42791</v>
@@ -6834,7 +6837,7 @@
       </c>
       <c r="F67" s="15">
         <f t="shared" si="2"/>
-        <v>0.24999999999999981</v>
+        <v>0.25154320987654333</v>
       </c>
       <c r="G67" s="30">
         <v>42791</v>
@@ -6865,7 +6868,7 @@
       </c>
       <c r="F68" s="15">
         <f t="shared" si="2"/>
-        <v>0.25230061349693234</v>
+        <v>0.25385802469135815</v>
       </c>
       <c r="G68" s="30">
         <v>42791</v>
@@ -6896,7 +6899,7 @@
       </c>
       <c r="F69" s="15">
         <f t="shared" si="2"/>
-        <v>0.26073619631901823</v>
+        <v>0.26234567901234579</v>
       </c>
       <c r="G69" s="30">
         <v>42791</v>
@@ -6927,7 +6930,7 @@
       </c>
       <c r="F70" s="15">
         <f t="shared" ref="F70:F133" si="11">F69+(C70/$C$245)</f>
-        <v>0.2615030674846624</v>
+        <v>0.2631172839506174</v>
       </c>
       <c r="G70" s="30">
         <v>42791</v>
@@ -6958,7 +6961,7 @@
       </c>
       <c r="F71" s="15">
         <f t="shared" si="11"/>
-        <v>0.2638036809815949</v>
+        <v>0.26543209876543222</v>
       </c>
       <c r="G71" s="30">
         <v>42791</v>
@@ -6988,7 +6991,7 @@
       <c r="E72" s="27"/>
       <c r="F72" s="29">
         <f t="shared" si="11"/>
-        <v>0.2638036809815949</v>
+        <v>0.26543209876543222</v>
       </c>
       <c r="G72" s="41" t="str">
         <f>IF(COUNTA(G73:G83)=COUNTA(B73:B83), "COMPLETE", "")</f>
@@ -7020,7 +7023,7 @@
       </c>
       <c r="F73" s="15">
         <f t="shared" si="11"/>
-        <v>0.26457055214723907</v>
+        <v>0.26620370370370383</v>
       </c>
       <c r="G73" s="30">
         <v>42792</v>
@@ -7051,7 +7054,7 @@
       </c>
       <c r="F74" s="15">
         <f t="shared" si="11"/>
-        <v>0.2722392638036808</v>
+        <v>0.27391975308641986</v>
       </c>
       <c r="G74" s="30">
         <v>42794</v>
@@ -7082,7 +7085,7 @@
       </c>
       <c r="F75" s="15">
         <f t="shared" si="11"/>
-        <v>0.2745398773006133</v>
+        <v>0.27623456790123468</v>
       </c>
       <c r="G75" s="30">
         <v>42794</v>
@@ -7113,7 +7116,7 @@
       </c>
       <c r="F76" s="15">
         <f t="shared" si="11"/>
-        <v>0.28220858895705503</v>
+        <v>0.28395061728395071</v>
       </c>
       <c r="G76" s="30">
         <v>42794</v>
@@ -7144,7 +7147,7 @@
       </c>
       <c r="F77" s="15">
         <f t="shared" si="11"/>
-        <v>0.28450920245398753</v>
+        <v>0.28626543209876554</v>
       </c>
       <c r="G77" s="30">
         <v>42794</v>
@@ -7175,7 +7178,7 @@
       </c>
       <c r="F78" s="15">
         <f t="shared" si="11"/>
-        <v>0.29294478527607343</v>
+        <v>0.29475308641975317</v>
       </c>
       <c r="G78" s="30">
         <v>42794</v>
@@ -7206,7 +7209,7 @@
       </c>
       <c r="F79" s="15">
         <f t="shared" si="11"/>
-        <v>0.29524539877300593</v>
+        <v>0.297067901234568</v>
       </c>
       <c r="G79" s="30">
         <v>42794</v>
@@ -7237,7 +7240,7 @@
       </c>
       <c r="F80" s="15">
         <f t="shared" si="11"/>
-        <v>0.30138036809815932</v>
+        <v>0.30324074074074081</v>
       </c>
       <c r="G80" s="30">
         <v>42794</v>
@@ -7268,7 +7271,7 @@
       </c>
       <c r="F81" s="15">
         <f t="shared" si="11"/>
-        <v>0.30368098159509183</v>
+        <v>0.30555555555555564</v>
       </c>
       <c r="G81" s="30">
         <v>42794</v>
@@ -7299,7 +7302,7 @@
       </c>
       <c r="F82" s="15">
         <f t="shared" si="11"/>
-        <v>0.31058282208588939</v>
+        <v>0.31250000000000006</v>
       </c>
       <c r="G82" s="30">
         <v>42794</v>
@@ -7330,7 +7333,7 @@
       </c>
       <c r="F83" s="15">
         <f t="shared" si="11"/>
-        <v>0.31288343558282189</v>
+        <v>0.31481481481481488</v>
       </c>
       <c r="G83" s="30">
         <v>42794</v>
@@ -7360,7 +7363,7 @@
       <c r="E84" s="27"/>
       <c r="F84" s="29">
         <f t="shared" si="11"/>
-        <v>0.31288343558282189</v>
+        <v>0.31481481481481488</v>
       </c>
       <c r="G84" s="41" t="str">
         <f>IF(COUNTA(G85:G107)=COUNTA(B85:B107), "COMPLETE", "")</f>
@@ -7392,7 +7395,7 @@
       </c>
       <c r="F85" s="15">
         <f t="shared" si="11"/>
-        <v>0.31365030674846606</v>
+        <v>0.31558641975308649</v>
       </c>
       <c r="G85" s="30">
         <v>42794</v>
@@ -7423,7 +7426,7 @@
       </c>
       <c r="F86" s="15">
         <f t="shared" si="11"/>
-        <v>0.32131901840490779</v>
+        <v>0.32330246913580252</v>
       </c>
       <c r="G86" s="30">
         <v>42794</v>
@@ -7454,7 +7457,7 @@
       </c>
       <c r="F87" s="15">
         <f t="shared" si="11"/>
-        <v>0.32361963190184029</v>
+        <v>0.32561728395061734</v>
       </c>
       <c r="G87" s="30">
         <v>42794</v>
@@ -7485,7 +7488,7 @@
       </c>
       <c r="F88" s="15">
         <f t="shared" si="11"/>
-        <v>0.33128834355828202</v>
+        <v>0.33333333333333337</v>
       </c>
       <c r="G88" s="30">
         <v>42794</v>
@@ -7516,7 +7519,7 @@
       </c>
       <c r="F89" s="15">
         <f t="shared" si="11"/>
-        <v>0.33358895705521452</v>
+        <v>0.3356481481481482</v>
       </c>
       <c r="G89" s="30">
         <v>42794</v>
@@ -7547,7 +7550,7 @@
       </c>
       <c r="F90" s="15">
         <f t="shared" si="11"/>
-        <v>0.34355828220858875</v>
+        <v>0.34567901234567905</v>
       </c>
       <c r="G90" s="30">
         <v>42794</v>
@@ -7578,7 +7581,7 @@
       </c>
       <c r="F91" s="15">
         <f t="shared" si="11"/>
-        <v>0.34585889570552125</v>
+        <v>0.34799382716049387</v>
       </c>
       <c r="G91" s="30">
         <v>42794</v>
@@ -7609,7 +7612,7 @@
       </c>
       <c r="F92" s="15">
         <f t="shared" si="11"/>
-        <v>0.35659509202453965</v>
+        <v>0.35879629629629634</v>
       </c>
       <c r="G92" s="30">
         <v>42794</v>
@@ -7640,7 +7643,7 @@
       </c>
       <c r="F93" s="15">
         <f t="shared" si="11"/>
-        <v>0.35889570552147215</v>
+        <v>0.36111111111111116</v>
       </c>
       <c r="G93" s="30">
         <v>42794</v>
@@ -7671,7 +7674,7 @@
       </c>
       <c r="F94" s="15">
         <f t="shared" si="11"/>
-        <v>0.36809815950920222</v>
+        <v>0.37037037037037041</v>
       </c>
       <c r="G94" s="30">
         <v>42794</v>
@@ -7702,7 +7705,7 @@
       </c>
       <c r="F95" s="15">
         <f t="shared" si="11"/>
-        <v>0.37039877300613472</v>
+        <v>0.37268518518518523</v>
       </c>
       <c r="G95" s="30">
         <v>42794</v>
@@ -7733,7 +7736,7 @@
       </c>
       <c r="F96" s="15">
         <f t="shared" si="11"/>
-        <v>0.37883435582822061</v>
+        <v>0.38117283950617287</v>
       </c>
       <c r="G96" s="30">
         <v>42794</v>
@@ -7764,7 +7767,7 @@
       </c>
       <c r="F97" s="15">
         <f t="shared" si="11"/>
-        <v>0.38113496932515312</v>
+        <v>0.38348765432098769</v>
       </c>
       <c r="G97" s="30">
         <v>42794</v>
@@ -7795,7 +7798,7 @@
       </c>
       <c r="F98" s="15">
         <f t="shared" si="11"/>
-        <v>0.38650306748466234</v>
+        <v>0.38888888888888895</v>
       </c>
       <c r="G98" s="30">
         <v>42794</v>
@@ -7826,7 +7829,7 @@
       </c>
       <c r="F99" s="15">
         <f t="shared" si="11"/>
-        <v>0.38880368098159485</v>
+        <v>0.39120370370370378</v>
       </c>
       <c r="G99" s="30">
         <v>42794</v>
@@ -7857,7 +7860,7 @@
       </c>
       <c r="F100" s="15">
         <f t="shared" si="11"/>
-        <v>0.39493865030674824</v>
+        <v>0.39737654320987659</v>
       </c>
       <c r="G100" s="30">
         <v>42794</v>
@@ -7888,7 +7891,7 @@
       </c>
       <c r="F101" s="15">
         <f t="shared" si="11"/>
-        <v>0.39723926380368074</v>
+        <v>0.39969135802469141</v>
       </c>
       <c r="G101" s="30">
         <v>42794</v>
@@ -7919,7 +7922,7 @@
       </c>
       <c r="F102" s="15">
         <f t="shared" si="11"/>
-        <v>0.40720858895705497</v>
+        <v>0.40972222222222227</v>
       </c>
       <c r="G102" s="30">
         <v>42794</v>
@@ -7950,7 +7953,7 @@
       </c>
       <c r="F103" s="15">
         <f t="shared" si="11"/>
-        <v>0.4148773006134967</v>
+        <v>0.41743827160493829</v>
       </c>
       <c r="G103" s="30">
         <v>42794</v>
@@ -7981,7 +7984,7 @@
       </c>
       <c r="F104" s="15">
         <f t="shared" si="11"/>
-        <v>0.4171779141104292</v>
+        <v>0.41975308641975312</v>
       </c>
       <c r="G104" s="30">
         <v>42794</v>
@@ -8012,7 +8015,7 @@
       </c>
       <c r="F105" s="15">
         <f t="shared" si="11"/>
-        <v>0.42638036809815927</v>
+        <v>0.42901234567901236</v>
       </c>
       <c r="G105" s="30">
         <v>42794</v>
@@ -8043,7 +8046,7 @@
       </c>
       <c r="F106" s="15">
         <f t="shared" si="11"/>
-        <v>0.42868098159509177</v>
+        <v>0.43132716049382719</v>
       </c>
       <c r="G106" s="30">
         <v>42794</v>
@@ -8074,7 +8077,7 @@
       </c>
       <c r="F107" s="15">
         <f t="shared" si="11"/>
-        <v>0.434049079754601</v>
+        <v>0.43672839506172845</v>
       </c>
       <c r="G107" s="30">
         <v>42794</v>
@@ -8104,7 +8107,7 @@
       <c r="E108" s="27"/>
       <c r="F108" s="29">
         <f t="shared" si="11"/>
-        <v>0.434049079754601</v>
+        <v>0.43672839506172845</v>
       </c>
       <c r="G108" s="41" t="str">
         <f>IF(COUNTA(G109:G125)=COUNTA(B109:B125), "COMPLETE", "")</f>
@@ -8136,7 +8139,7 @@
       </c>
       <c r="F109" s="15">
         <f t="shared" si="11"/>
-        <v>0.43481595092024516</v>
+        <v>0.43750000000000006</v>
       </c>
       <c r="G109" s="30">
         <v>42795</v>
@@ -8167,7 +8170,7 @@
       </c>
       <c r="F110" s="15">
         <f t="shared" si="11"/>
-        <v>0.44171779141104273</v>
+        <v>0.44444444444444448</v>
       </c>
       <c r="G110" s="30">
         <v>42795</v>
@@ -8198,7 +8201,7 @@
       </c>
       <c r="F111" s="15">
         <f t="shared" si="11"/>
-        <v>0.44401840490797523</v>
+        <v>0.4467592592592593</v>
       </c>
       <c r="G111" s="30">
         <v>42795</v>
@@ -8229,7 +8232,7 @@
       </c>
       <c r="F112" s="15">
         <f t="shared" si="11"/>
-        <v>0.45245398773006112</v>
+        <v>0.45524691358024694</v>
       </c>
       <c r="G112" s="30">
         <v>42795</v>
@@ -8260,7 +8263,7 @@
       </c>
       <c r="F113" s="15">
         <f t="shared" si="11"/>
-        <v>0.45475460122699363</v>
+        <v>0.45756172839506176</v>
       </c>
       <c r="G113" s="30">
         <v>42795</v>
@@ -8291,7 +8294,7 @@
       </c>
       <c r="F114" s="15">
         <f t="shared" si="11"/>
-        <v>0.46472392638036786</v>
+        <v>0.46759259259259262</v>
       </c>
       <c r="G114" s="30">
         <v>42795</v>
@@ -8322,7 +8325,7 @@
       </c>
       <c r="F115" s="15">
         <f t="shared" si="11"/>
-        <v>0.46702453987730036</v>
+        <v>0.46990740740740744</v>
       </c>
       <c r="G115" s="30">
         <v>42795</v>
@@ -8353,7 +8356,7 @@
       </c>
       <c r="F116" s="15">
         <f t="shared" si="11"/>
-        <v>0.47699386503067459</v>
+        <v>0.47993827160493829</v>
       </c>
       <c r="G116" s="30">
         <v>42795</v>
@@ -8384,7 +8387,7 @@
       </c>
       <c r="F117" s="15">
         <f t="shared" si="11"/>
-        <v>0.47929447852760709</v>
+        <v>0.48225308641975312</v>
       </c>
       <c r="G117" s="30">
         <v>42795</v>
@@ -8415,7 +8418,7 @@
       </c>
       <c r="F118" s="15">
         <f t="shared" si="11"/>
-        <v>0.48849693251533716</v>
+        <v>0.49151234567901236</v>
       </c>
       <c r="G118" s="30">
         <v>42795</v>
@@ -8446,7 +8449,7 @@
       </c>
       <c r="F119" s="15">
         <f t="shared" si="11"/>
-        <v>0.49079754601226966</v>
+        <v>0.49382716049382719</v>
       </c>
       <c r="G119" s="30">
         <v>42795</v>
@@ -8477,7 +8480,7 @@
       </c>
       <c r="F120" s="15">
         <f t="shared" si="11"/>
-        <v>0.49693251533742305</v>
+        <v>0.5</v>
       </c>
       <c r="G120" s="30">
         <v>42795</v>
@@ -8508,7 +8511,7 @@
       </c>
       <c r="F121" s="15">
         <f t="shared" si="11"/>
-        <v>0.49923312883435556</v>
+        <v>0.50231481481481477</v>
       </c>
       <c r="G121" s="30">
         <v>42795</v>
@@ -8539,7 +8542,7 @@
       </c>
       <c r="F122" s="15">
         <f t="shared" si="11"/>
-        <v>0.50766871165644145</v>
+        <v>0.51080246913580241</v>
       </c>
       <c r="G122" s="30">
         <v>42795</v>
@@ -8570,7 +8573,7 @@
       </c>
       <c r="F123" s="15">
         <f t="shared" si="11"/>
-        <v>0.50996932515337401</v>
+        <v>0.51311728395061718</v>
       </c>
       <c r="G123" s="30">
         <v>42795</v>
@@ -8601,7 +8604,7 @@
       </c>
       <c r="F124" s="15">
         <f t="shared" si="11"/>
-        <v>0.51917177914110402</v>
+        <v>0.52237654320987648</v>
       </c>
       <c r="G124" s="30">
         <v>42795</v>
@@ -8632,7 +8635,7 @@
       </c>
       <c r="F125" s="15">
         <f t="shared" si="11"/>
-        <v>0.52147239263803657</v>
+        <v>0.52469135802469125</v>
       </c>
       <c r="G125" s="30">
         <v>42795</v>
@@ -8662,7 +8665,7 @@
       <c r="E126" s="27"/>
       <c r="F126" s="29">
         <f t="shared" si="11"/>
-        <v>0.52147239263803657</v>
+        <v>0.52469135802469125</v>
       </c>
       <c r="G126" s="41" t="str">
         <f>IF(COUNTA(G127:G143)=COUNTA(B127:B143), "COMPLETE", "")</f>
@@ -8694,7 +8697,7 @@
       </c>
       <c r="F127" s="15">
         <f t="shared" si="11"/>
-        <v>0.5222392638036808</v>
+        <v>0.5254629629629628</v>
       </c>
       <c r="G127" s="30">
         <v>42796</v>
@@ -8725,7 +8728,7 @@
       </c>
       <c r="F128" s="15">
         <f t="shared" si="11"/>
-        <v>0.53220858895705503</v>
+        <v>0.53549382716049365</v>
       </c>
       <c r="G128" s="30">
         <v>42796</v>
@@ -8756,7 +8759,7 @@
       </c>
       <c r="F129" s="15">
         <f t="shared" si="11"/>
-        <v>0.53450920245398759</v>
+        <v>0.53780864197530842</v>
       </c>
       <c r="G129" s="30">
         <v>42796</v>
@@ -8787,7 +8790,7 @@
       </c>
       <c r="F130" s="15">
         <f t="shared" si="11"/>
-        <v>0.54601226993865015</v>
+        <v>0.54938271604938249</v>
       </c>
       <c r="G130" s="30">
         <v>42796</v>
@@ -8818,7 +8821,7 @@
       </c>
       <c r="F131" s="15">
         <f t="shared" si="11"/>
-        <v>0.54831288343558271</v>
+        <v>0.55169753086419726</v>
       </c>
       <c r="G131" s="30">
         <v>42796</v>
@@ -8849,7 +8852,7 @@
       </c>
       <c r="F132" s="15">
         <f t="shared" si="11"/>
-        <v>0.55674846625766861</v>
+        <v>0.5601851851851849</v>
       </c>
       <c r="G132" s="30">
         <v>42796</v>
@@ -8880,7 +8883,7 @@
       </c>
       <c r="F133" s="15">
         <f t="shared" si="11"/>
-        <v>0.55904907975460116</v>
+        <v>0.56249999999999967</v>
       </c>
       <c r="G133" s="30">
         <v>42796</v>
@@ -8911,7 +8914,7 @@
       </c>
       <c r="F134" s="15">
         <f t="shared" ref="F134:F197" si="18">F133+(C134/$C$245)</f>
-        <v>0.56901840490797539</v>
+        <v>0.57253086419753052</v>
       </c>
       <c r="G134" s="30">
         <v>42796</v>
@@ -8942,7 +8945,7 @@
       </c>
       <c r="F135" s="15">
         <f t="shared" si="18"/>
-        <v>0.57131901840490795</v>
+        <v>0.57484567901234529</v>
       </c>
       <c r="G135" s="30">
         <v>42796</v>
@@ -8973,7 +8976,7 @@
       </c>
       <c r="F136" s="15">
         <f t="shared" si="18"/>
-        <v>0.57975460122699385</v>
+        <v>0.58333333333333293</v>
       </c>
       <c r="G136" s="30">
         <v>42796</v>
@@ -9004,7 +9007,7 @@
       </c>
       <c r="F137" s="15">
         <f t="shared" si="18"/>
-        <v>0.58205521472392641</v>
+        <v>0.5856481481481477</v>
       </c>
       <c r="G137" s="30">
         <v>42796</v>
@@ -9035,7 +9038,7 @@
       </c>
       <c r="F138" s="15">
         <f t="shared" si="18"/>
-        <v>0.5904907975460123</v>
+        <v>0.59413580246913533</v>
       </c>
       <c r="G138" s="30">
         <v>42796</v>
@@ -9066,7 +9069,7 @@
       </c>
       <c r="F139" s="15">
         <f t="shared" si="18"/>
-        <v>0.59279141104294486</v>
+        <v>0.5964506172839501</v>
       </c>
       <c r="G139" s="30">
         <v>42796</v>
@@ -9097,7 +9100,7 @@
       </c>
       <c r="F140" s="15">
         <f t="shared" si="18"/>
-        <v>0.60046012269938653</v>
+        <v>0.60416666666666619</v>
       </c>
       <c r="G140" s="30">
         <v>42796</v>
@@ -9128,7 +9131,7 @@
       </c>
       <c r="F141" s="15">
         <f t="shared" si="18"/>
-        <v>0.60276073619631909</v>
+        <v>0.60648148148148096</v>
       </c>
       <c r="G141" s="30">
         <v>42796</v>
@@ -9159,7 +9162,7 @@
       </c>
       <c r="F142" s="15">
         <f t="shared" si="18"/>
-        <v>0.61273006134969332</v>
+        <v>0.61651234567901181</v>
       </c>
       <c r="G142" s="30">
         <v>42796</v>
@@ -9190,7 +9193,7 @@
       </c>
       <c r="F143" s="15">
         <f t="shared" si="18"/>
-        <v>0.61503067484662588</v>
+        <v>0.61882716049382658</v>
       </c>
       <c r="G143" s="30">
         <v>42796</v>
@@ -9215,16 +9218,16 @@
       <c r="C144" s="26"/>
       <c r="D144" s="20">
         <f>SUM(C144:C159)</f>
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="E144" s="27"/>
       <c r="F144" s="29">
         <f t="shared" si="18"/>
-        <v>0.61503067484662588</v>
+        <v>0.61882716049382658</v>
       </c>
       <c r="G144" s="41" t="str">
         <f>IF(COUNTA(G145:G158)=COUNTA(B145:B158), "COMPLETE", "")</f>
-        <v/>
+        <v>COMPLETE</v>
       </c>
       <c r="I144" s="9" t="str">
         <f t="shared" si="19"/>
@@ -9235,7 +9238,7 @@
         <v/>
       </c>
     </row>
-    <row r="145" spans="1:10" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="145" spans="1:11" ht="15.75" outlineLevel="1" thickBot="1">
       <c r="B145" s="18" t="s">
         <v>177</v>
       </c>
@@ -9244,17 +9247,19 @@
       </c>
       <c r="D145" s="21">
         <f>D144/60</f>
-        <v>1.5166666666666666</v>
+        <v>1.3833333333333333</v>
       </c>
       <c r="E145" s="15">
         <f>E144+(C145/$D$144)</f>
-        <v>1.098901098901099E-2</v>
+        <v>1.2048192771084338E-2</v>
       </c>
       <c r="F145" s="15">
         <f t="shared" si="18"/>
-        <v>0.6157975460122701</v>
-      </c>
-      <c r="G145" s="30"/>
+        <v>0.61959876543209813</v>
+      </c>
+      <c r="G145" s="30">
+        <v>42796</v>
+      </c>
       <c r="H145" s="30">
         <v>42796</v>
       </c>
@@ -9267,7 +9272,7 @@
         <v/>
       </c>
     </row>
-    <row r="146" spans="1:10" outlineLevel="1">
+    <row r="146" spans="1:11" outlineLevel="1">
       <c r="B146" s="18" t="s">
         <v>178</v>
       </c>
@@ -9277,13 +9282,15 @@
       <c r="D146" s="19"/>
       <c r="E146" s="15">
         <f t="shared" ref="E146:E158" si="21">E145+(C146/$D$144)</f>
-        <v>9.8901098901098911E-2</v>
+        <v>0.10843373493975904</v>
       </c>
       <c r="F146" s="15">
         <f t="shared" si="18"/>
-        <v>0.62193251533742344</v>
-      </c>
-      <c r="G146" s="30"/>
+        <v>0.625771604938271</v>
+      </c>
+      <c r="G146" s="30">
+        <v>42796</v>
+      </c>
       <c r="H146" s="30">
         <v>42796</v>
       </c>
@@ -9296,7 +9303,7 @@
         <v/>
       </c>
     </row>
-    <row r="147" spans="1:10" outlineLevel="1">
+    <row r="147" spans="1:11" outlineLevel="1">
       <c r="B147" s="18" t="s">
         <v>180</v>
       </c>
@@ -9306,13 +9313,15 @@
       <c r="D147" s="19"/>
       <c r="E147" s="15">
         <f t="shared" si="21"/>
-        <v>0.13186813186813187</v>
+        <v>0.14457831325301204</v>
       </c>
       <c r="F147" s="15">
         <f t="shared" si="18"/>
-        <v>0.624233128834356</v>
-      </c>
-      <c r="G147" s="30"/>
+        <v>0.62808641975308577</v>
+      </c>
+      <c r="G147" s="30">
+        <v>42796</v>
+      </c>
       <c r="H147" s="30">
         <v>42796</v>
       </c>
@@ -9325,7 +9334,7 @@
         <v/>
       </c>
     </row>
-    <row r="148" spans="1:10" outlineLevel="1">
+    <row r="148" spans="1:11" outlineLevel="1">
       <c r="B148" s="18" t="s">
         <v>181</v>
       </c>
@@ -9335,13 +9344,15 @@
       <c r="D148" s="19"/>
       <c r="E148" s="15">
         <f t="shared" si="21"/>
-        <v>0.26373626373626374</v>
+        <v>0.28915662650602408</v>
       </c>
       <c r="F148" s="15">
         <f t="shared" si="18"/>
-        <v>0.63343558282208601</v>
-      </c>
-      <c r="G148" s="30"/>
+        <v>0.63734567901234507</v>
+      </c>
+      <c r="G148" s="30">
+        <v>42796</v>
+      </c>
       <c r="H148" s="30">
         <v>42796</v>
       </c>
@@ -9354,7 +9365,7 @@
         <v/>
       </c>
     </row>
-    <row r="149" spans="1:10" outlineLevel="1">
+    <row r="149" spans="1:11" outlineLevel="1">
       <c r="B149" s="18" t="s">
         <v>182</v>
       </c>
@@ -9364,13 +9375,15 @@
       <c r="D149" s="19"/>
       <c r="E149" s="15">
         <f t="shared" si="21"/>
-        <v>0.2967032967032967</v>
+        <v>0.3253012048192771</v>
       </c>
       <c r="F149" s="15">
         <f t="shared" si="18"/>
-        <v>0.63573619631901856</v>
-      </c>
-      <c r="G149" s="30"/>
+        <v>0.63966049382715984</v>
+      </c>
+      <c r="G149" s="30">
+        <v>42796</v>
+      </c>
       <c r="H149" s="30">
         <v>42796</v>
       </c>
@@ -9383,7 +9396,7 @@
         <v/>
       </c>
     </row>
-    <row r="150" spans="1:10" outlineLevel="1">
+    <row r="150" spans="1:11" outlineLevel="1">
       <c r="B150" s="18" t="s">
         <v>183</v>
       </c>
@@ -9393,13 +9406,15 @@
       <c r="D150" s="19"/>
       <c r="E150" s="15">
         <f t="shared" si="21"/>
-        <v>0.45054945054945056</v>
+        <v>0.49397590361445781</v>
       </c>
       <c r="F150" s="15">
         <f t="shared" si="18"/>
-        <v>0.64647239263803702</v>
-      </c>
-      <c r="G150" s="30"/>
+        <v>0.65046296296296235</v>
+      </c>
+      <c r="G150" s="30">
+        <v>42796</v>
+      </c>
       <c r="H150" s="30">
         <v>42796</v>
       </c>
@@ -9412,7 +9427,7 @@
         <v/>
       </c>
     </row>
-    <row r="151" spans="1:10" outlineLevel="1">
+    <row r="151" spans="1:11" outlineLevel="1">
       <c r="B151" s="18" t="s">
         <v>184</v>
       </c>
@@ -9422,13 +9437,15 @@
       <c r="D151" s="19"/>
       <c r="E151" s="15">
         <f t="shared" si="21"/>
-        <v>0.48351648351648352</v>
+        <v>0.53012048192771077</v>
       </c>
       <c r="F151" s="15">
         <f t="shared" si="18"/>
-        <v>0.64877300613496958</v>
-      </c>
-      <c r="G151" s="30"/>
+        <v>0.65277777777777712</v>
+      </c>
+      <c r="G151" s="30">
+        <v>42796</v>
+      </c>
       <c r="H151" s="30">
         <v>42796</v>
       </c>
@@ -9441,7 +9458,7 @@
         <v/>
       </c>
     </row>
-    <row r="152" spans="1:10" outlineLevel="1">
+    <row r="152" spans="1:11" outlineLevel="1">
       <c r="B152" s="18" t="s">
         <v>185</v>
       </c>
@@ -9451,13 +9468,15 @@
       <c r="D152" s="19"/>
       <c r="E152" s="15">
         <f t="shared" si="21"/>
-        <v>0.63736263736263732</v>
+        <v>0.69879518072289148</v>
       </c>
       <c r="F152" s="15">
         <f t="shared" si="18"/>
-        <v>0.65950920245398803</v>
-      </c>
-      <c r="G152" s="30"/>
+        <v>0.66358024691357964</v>
+      </c>
+      <c r="G152" s="30">
+        <v>42796</v>
+      </c>
       <c r="H152" s="30">
         <v>42796</v>
       </c>
@@ -9470,7 +9489,7 @@
         <v/>
       </c>
     </row>
-    <row r="153" spans="1:10" outlineLevel="1">
+    <row r="153" spans="1:11" outlineLevel="1">
       <c r="B153" s="18" t="s">
         <v>186</v>
       </c>
@@ -9480,13 +9499,15 @@
       <c r="D153" s="19"/>
       <c r="E153" s="15">
         <f t="shared" si="21"/>
-        <v>0.67032967032967028</v>
+        <v>0.7349397590361445</v>
       </c>
       <c r="F153" s="15">
         <f t="shared" si="18"/>
-        <v>0.66180981595092059</v>
-      </c>
-      <c r="G153" s="30"/>
+        <v>0.66589506172839441</v>
+      </c>
+      <c r="G153" s="30">
+        <v>42796</v>
+      </c>
       <c r="H153" s="30">
         <v>42796</v>
       </c>
@@ -9499,7 +9520,7 @@
         <v/>
       </c>
     </row>
-    <row r="154" spans="1:10" outlineLevel="1">
+    <row r="154" spans="1:11" outlineLevel="1">
       <c r="B154" s="18" t="s">
         <v>187</v>
       </c>
@@ -9509,13 +9530,15 @@
       <c r="D154" s="19"/>
       <c r="E154" s="15">
         <f t="shared" si="21"/>
-        <v>0.76923076923076916</v>
+        <v>0.84337349397590355</v>
       </c>
       <c r="F154" s="15">
         <f t="shared" si="18"/>
-        <v>0.66871165644171815</v>
-      </c>
-      <c r="G154" s="30"/>
+        <v>0.67283950617283883</v>
+      </c>
+      <c r="G154" s="30">
+        <v>42796</v>
+      </c>
       <c r="H154" s="30">
         <v>42796</v>
       </c>
@@ -9528,7 +9551,7 @@
         <v/>
       </c>
     </row>
-    <row r="155" spans="1:10" outlineLevel="1">
+    <row r="155" spans="1:11" outlineLevel="1">
       <c r="B155" s="18" t="s">
         <v>188</v>
       </c>
@@ -9538,13 +9561,15 @@
       <c r="D155" s="19"/>
       <c r="E155" s="15">
         <f t="shared" si="21"/>
-        <v>0.80219780219780212</v>
+        <v>0.87951807228915657</v>
       </c>
       <c r="F155" s="15">
         <f t="shared" si="18"/>
-        <v>0.67101226993865071</v>
-      </c>
-      <c r="G155" s="30"/>
+        <v>0.6751543209876536</v>
+      </c>
+      <c r="G155" s="30">
+        <v>42796</v>
+      </c>
       <c r="H155" s="30">
         <v>42796</v>
       </c>
@@ -9557,7 +9582,7 @@
         <v/>
       </c>
     </row>
-    <row r="156" spans="1:10" outlineLevel="1">
+    <row r="156" spans="1:11" outlineLevel="1">
       <c r="B156" s="18" t="s">
         <v>189</v>
       </c>
@@ -9567,13 +9592,15 @@
       <c r="D156" s="19"/>
       <c r="E156" s="15">
         <f t="shared" si="21"/>
-        <v>0.87912087912087911</v>
+        <v>0.96385542168674698</v>
       </c>
       <c r="F156" s="15">
         <f t="shared" si="18"/>
-        <v>0.67638036809815993</v>
-      </c>
-      <c r="G156" s="30"/>
+        <v>0.6805555555555548</v>
+      </c>
+      <c r="G156" s="30">
+        <v>42796</v>
+      </c>
       <c r="H156" s="30">
         <v>42796</v>
       </c>
@@ -9586,7 +9613,7 @@
         <v/>
       </c>
     </row>
-    <row r="157" spans="1:10" outlineLevel="1">
+    <row r="157" spans="1:11" outlineLevel="1">
       <c r="B157" s="18" t="s">
         <v>191</v>
       </c>
@@ -9596,13 +9623,15 @@
       <c r="D157" s="19"/>
       <c r="E157" s="15">
         <f t="shared" si="21"/>
-        <v>0.91208791208791207</v>
+        <v>1</v>
       </c>
       <c r="F157" s="15">
         <f t="shared" si="18"/>
-        <v>0.67868098159509249</v>
-      </c>
-      <c r="G157" s="30"/>
+        <v>0.68287037037036957</v>
+      </c>
+      <c r="G157" s="30">
+        <v>42796</v>
+      </c>
       <c r="H157" s="30">
         <v>42796</v>
       </c>
@@ -9615,12 +9644,12 @@
         <v/>
       </c>
     </row>
-    <row r="158" spans="1:10" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="158" spans="1:11" ht="15.75" outlineLevel="1" thickBot="1">
       <c r="B158" s="18" t="s">
         <v>192</v>
       </c>
       <c r="C158" s="13">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D158" s="19"/>
       <c r="E158" s="15">
@@ -9629,9 +9658,11 @@
       </c>
       <c r="F158" s="15">
         <f t="shared" si="18"/>
-        <v>0.68481595092024583</v>
-      </c>
-      <c r="G158" s="30"/>
+        <v>0.68287037037036957</v>
+      </c>
+      <c r="G158" s="30">
+        <v>42796</v>
+      </c>
       <c r="H158" s="30">
         <v>42796</v>
       </c>
@@ -9643,8 +9674,11 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-    </row>
-    <row r="159" spans="1:10" ht="21" thickBot="1">
+      <c r="K158" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11" ht="21" thickBot="1">
       <c r="A159" s="28" t="s">
         <v>314</v>
       </c>
@@ -9657,7 +9691,7 @@
       <c r="E159" s="27"/>
       <c r="F159" s="29">
         <f t="shared" si="18"/>
-        <v>0.68481595092024583</v>
+        <v>0.68287037037036957</v>
       </c>
       <c r="G159" s="41" t="str">
         <f>IF(COUNTA(G160:G162)=COUNTA(B160:B162), "COMPLETE", "")</f>
@@ -9672,7 +9706,7 @@
         <v/>
       </c>
     </row>
-    <row r="160" spans="1:10" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="160" spans="1:11" ht="15.75" outlineLevel="1" thickBot="1">
       <c r="B160" s="18" t="s">
         <v>195</v>
       </c>
@@ -9689,9 +9723,11 @@
       </c>
       <c r="F160" s="15">
         <f t="shared" si="18"/>
-        <v>0.68558282208589005</v>
-      </c>
-      <c r="G160" s="30"/>
+        <v>0.68364197530864113</v>
+      </c>
+      <c r="G160" s="30">
+        <v>42796</v>
+      </c>
       <c r="H160" s="30">
         <v>42796</v>
       </c>
@@ -9718,7 +9754,7 @@
       </c>
       <c r="F161" s="15">
         <f t="shared" si="18"/>
-        <v>0.69248466257668762</v>
+        <v>0.69058641975308555</v>
       </c>
       <c r="G161" s="30"/>
       <c r="H161" s="30">
@@ -9747,7 +9783,7 @@
       </c>
       <c r="F162" s="15">
         <f t="shared" si="18"/>
-        <v>0.69478527607362017</v>
+        <v>0.69290123456790031</v>
       </c>
       <c r="G162" s="30"/>
       <c r="H162" s="30">
@@ -9776,7 +9812,7 @@
       </c>
       <c r="F163" s="15">
         <f t="shared" si="18"/>
-        <v>0.70245398773006185</v>
+        <v>0.7006172839506164</v>
       </c>
       <c r="G163" s="30"/>
       <c r="H163" s="30">
@@ -9805,7 +9841,7 @@
       </c>
       <c r="F164" s="15">
         <f t="shared" si="18"/>
-        <v>0.7047546012269944</v>
+        <v>0.70293209876543117</v>
       </c>
       <c r="G164" s="30"/>
       <c r="H164" s="30">
@@ -9834,7 +9870,7 @@
       </c>
       <c r="F165" s="15">
         <f t="shared" si="18"/>
-        <v>0.71165644171779197</v>
+        <v>0.70987654320987559</v>
       </c>
       <c r="G165" s="30"/>
       <c r="H165" s="30">
@@ -9863,7 +9899,7 @@
       </c>
       <c r="F166" s="15">
         <f t="shared" si="18"/>
-        <v>0.71395705521472452</v>
+        <v>0.71219135802469036</v>
       </c>
       <c r="G166" s="30"/>
       <c r="H166" s="30">
@@ -9892,7 +9928,7 @@
       </c>
       <c r="F167" s="15">
         <f t="shared" si="18"/>
-        <v>0.72315950920245453</v>
+        <v>0.72145061728394966</v>
       </c>
       <c r="G167" s="30"/>
       <c r="H167" s="30">
@@ -9921,7 +9957,7 @@
       </c>
       <c r="F168" s="15">
         <f t="shared" si="18"/>
-        <v>0.72546012269938709</v>
+        <v>0.72376543209876443</v>
       </c>
       <c r="G168" s="30"/>
       <c r="H168" s="30">
@@ -9950,7 +9986,7 @@
       </c>
       <c r="F169" s="15">
         <f t="shared" si="18"/>
-        <v>0.73389570552147299</v>
+        <v>0.73225308641975206</v>
       </c>
       <c r="G169" s="30"/>
       <c r="H169" s="30">
@@ -9979,7 +10015,7 @@
       </c>
       <c r="F170" s="15">
         <f t="shared" si="18"/>
-        <v>0.73619631901840554</v>
+        <v>0.73456790123456683</v>
       </c>
       <c r="G170" s="30"/>
       <c r="H170" s="30">
@@ -10008,7 +10044,7 @@
       </c>
       <c r="F171" s="15">
         <f t="shared" si="18"/>
-        <v>0.74386503067484722</v>
+        <v>0.74228395061728292</v>
       </c>
       <c r="G171" s="30"/>
       <c r="H171" s="30">
@@ -10037,7 +10073,7 @@
       </c>
       <c r="F172" s="15">
         <f t="shared" si="18"/>
-        <v>0.74616564417177977</v>
+        <v>0.74459876543209769</v>
       </c>
       <c r="G172" s="30"/>
       <c r="H172" s="30">
@@ -10065,7 +10101,7 @@
       <c r="E173" s="27"/>
       <c r="F173" s="29">
         <f t="shared" si="18"/>
-        <v>0.74616564417177977</v>
+        <v>0.74459876543209769</v>
       </c>
       <c r="G173" s="41" t="str">
         <f>IF(COUNTA(G174:G176)=COUNTA(B174:B176), "COMPLETE", "")</f>
@@ -10097,7 +10133,7 @@
       </c>
       <c r="F174" s="15">
         <f t="shared" si="18"/>
-        <v>0.746932515337424</v>
+        <v>0.74537037037036924</v>
       </c>
       <c r="G174" s="30"/>
       <c r="H174" s="30">
@@ -10126,7 +10162,7 @@
       </c>
       <c r="F175" s="15">
         <f t="shared" si="18"/>
-        <v>0.75383435582822156</v>
+        <v>0.75231481481481366</v>
       </c>
       <c r="G175" s="30"/>
       <c r="H175" s="30">
@@ -10155,7 +10191,7 @@
       </c>
       <c r="F176" s="15">
         <f t="shared" si="18"/>
-        <v>0.75613496932515412</v>
+        <v>0.75462962962962843</v>
       </c>
       <c r="G176" s="30"/>
       <c r="H176" s="30">
@@ -10184,7 +10220,7 @@
       </c>
       <c r="F177" s="15">
         <f t="shared" si="18"/>
-        <v>0.76150306748466334</v>
+        <v>0.76003086419752963</v>
       </c>
       <c r="G177" s="30"/>
       <c r="H177" s="30">
@@ -10213,7 +10249,7 @@
       </c>
       <c r="F178" s="15">
         <f t="shared" si="18"/>
-        <v>0.7638036809815959</v>
+        <v>0.7623456790123444</v>
       </c>
       <c r="G178" s="30"/>
       <c r="H178" s="30">
@@ -10242,7 +10278,7 @@
       </c>
       <c r="F179" s="15">
         <f t="shared" si="18"/>
-        <v>0.77070552147239346</v>
+        <v>0.76929012345678882</v>
       </c>
       <c r="G179" s="30"/>
       <c r="H179" s="30">
@@ -10271,7 +10307,7 @@
       </c>
       <c r="F180" s="15">
         <f t="shared" si="18"/>
-        <v>0.77300613496932602</v>
+        <v>0.77160493827160359</v>
       </c>
       <c r="G180" s="30"/>
       <c r="H180" s="30">
@@ -10300,7 +10336,7 @@
       </c>
       <c r="F181" s="15">
         <f t="shared" si="18"/>
-        <v>0.78144171779141192</v>
+        <v>0.78009259259259123</v>
       </c>
       <c r="G181" s="30"/>
       <c r="H181" s="30">
@@ -10329,7 +10365,7 @@
       </c>
       <c r="F182" s="15">
         <f t="shared" si="18"/>
-        <v>0.78374233128834447</v>
+        <v>0.782407407407406</v>
       </c>
       <c r="G182" s="30"/>
       <c r="H182" s="30">
@@ -10358,7 +10394,7 @@
       </c>
       <c r="F183" s="15">
         <f t="shared" si="18"/>
-        <v>0.79141104294478615</v>
+        <v>0.79012345679012208</v>
       </c>
       <c r="G183" s="30"/>
       <c r="H183" s="30">
@@ -10387,7 +10423,7 @@
       </c>
       <c r="F184" s="15">
         <f t="shared" si="18"/>
-        <v>0.7937116564417187</v>
+        <v>0.79243827160493685</v>
       </c>
       <c r="G184" s="30"/>
       <c r="H184" s="30">
@@ -10416,7 +10452,7 @@
       </c>
       <c r="F185" s="15">
         <f t="shared" si="18"/>
-        <v>0.80138036809816038</v>
+        <v>0.80015432098765293</v>
       </c>
       <c r="G185" s="30"/>
       <c r="H185" s="30">
@@ -10445,7 +10481,7 @@
       </c>
       <c r="F186" s="15">
         <f t="shared" si="18"/>
-        <v>0.80368098159509294</v>
+        <v>0.8024691358024677</v>
       </c>
       <c r="G186" s="30"/>
       <c r="H186" s="30">
@@ -10474,7 +10510,7 @@
       </c>
       <c r="F187" s="15">
         <f t="shared" si="18"/>
-        <v>0.8105828220858905</v>
+        <v>0.80941358024691212</v>
       </c>
       <c r="G187" s="30"/>
       <c r="H187" s="30">
@@ -10503,7 +10539,7 @@
       </c>
       <c r="F188" s="15">
         <f t="shared" si="18"/>
-        <v>0.82208588957055306</v>
+        <v>0.82098765432098619</v>
       </c>
       <c r="G188" s="30"/>
       <c r="H188" s="30">
@@ -10532,7 +10568,7 @@
       </c>
       <c r="F189" s="15">
         <f t="shared" si="18"/>
-        <v>0.82438650306748562</v>
+        <v>0.82330246913580096</v>
       </c>
       <c r="G189" s="30"/>
       <c r="H189" s="30">
@@ -10561,7 +10597,7 @@
       </c>
       <c r="F190" s="15">
         <f t="shared" si="18"/>
-        <v>0.83205521472392729</v>
+        <v>0.83101851851851705</v>
       </c>
       <c r="G190" s="30"/>
       <c r="H190" s="30">
@@ -10590,7 +10626,7 @@
       </c>
       <c r="F191" s="15">
         <f t="shared" si="18"/>
-        <v>0.83972392638036897</v>
+        <v>0.83873456790123313</v>
       </c>
       <c r="G191" s="30"/>
       <c r="H191" s="30">
@@ -10619,7 +10655,7 @@
       </c>
       <c r="F192" s="15">
         <f t="shared" si="18"/>
-        <v>0.84202453987730153</v>
+        <v>0.8410493827160479</v>
       </c>
       <c r="G192" s="30"/>
       <c r="H192" s="30">
@@ -10647,7 +10683,7 @@
       <c r="E193" s="27"/>
       <c r="F193" s="29">
         <f t="shared" si="18"/>
-        <v>0.84202453987730153</v>
+        <v>0.8410493827160479</v>
       </c>
       <c r="G193" s="41" t="str">
         <f>IF(COUNTA(G194:G196)=COUNTA(B194:B196), "COMPLETE", "")</f>
@@ -10679,7 +10715,7 @@
       </c>
       <c r="F194" s="15">
         <f t="shared" si="18"/>
-        <v>0.84279141104294575</v>
+        <v>0.84182098765431945</v>
       </c>
       <c r="G194" s="30"/>
       <c r="H194" s="30">
@@ -10708,7 +10744,7 @@
       </c>
       <c r="F195" s="15">
         <f t="shared" si="18"/>
-        <v>0.85122699386503164</v>
+        <v>0.85030864197530709</v>
       </c>
       <c r="G195" s="30"/>
       <c r="H195" s="30">
@@ -10737,7 +10773,7 @@
       </c>
       <c r="F196" s="15">
         <f t="shared" si="18"/>
-        <v>0.8535276073619642</v>
+        <v>0.85262345679012186</v>
       </c>
       <c r="G196" s="30"/>
       <c r="H196" s="30">
@@ -10766,7 +10802,7 @@
       </c>
       <c r="F197" s="15">
         <f t="shared" si="18"/>
-        <v>0.86119631901840588</v>
+        <v>0.86033950617283794</v>
       </c>
       <c r="G197" s="30"/>
       <c r="H197" s="30">
@@ -10795,7 +10831,7 @@
       </c>
       <c r="F198" s="15">
         <f t="shared" ref="F198:F243" si="26">F197+(C198/$C$245)</f>
-        <v>0.86349693251533843</v>
+        <v>0.86265432098765271</v>
       </c>
       <c r="G198" s="30"/>
       <c r="H198" s="30">
@@ -10824,7 +10860,7 @@
       </c>
       <c r="F199" s="15">
         <f t="shared" si="26"/>
-        <v>0.86886503067484766</v>
+        <v>0.86805555555555391</v>
       </c>
       <c r="G199" s="30"/>
       <c r="H199" s="30">
@@ -10853,7 +10889,7 @@
       </c>
       <c r="F200" s="15">
         <f t="shared" si="26"/>
-        <v>0.87116564417178022</v>
+        <v>0.87037037037036868</v>
       </c>
       <c r="G200" s="30"/>
       <c r="H200" s="30">
@@ -10881,7 +10917,7 @@
       <c r="E201" s="27"/>
       <c r="F201" s="29">
         <f t="shared" si="26"/>
-        <v>0.87116564417178022</v>
+        <v>0.87037037037036868</v>
       </c>
       <c r="G201" s="41" t="str">
         <f>IF(COUNTA(G202:G204)=COUNTA(B202:B204), "COMPLETE", "")</f>
@@ -10913,7 +10949,7 @@
       </c>
       <c r="F202" s="15">
         <f t="shared" si="26"/>
-        <v>0.87193251533742444</v>
+        <v>0.87114197530864024</v>
       </c>
       <c r="G202" s="30"/>
       <c r="H202" s="30">
@@ -10942,7 +10978,7 @@
       </c>
       <c r="F203" s="15">
         <f t="shared" si="26"/>
-        <v>0.87960122699386611</v>
+        <v>0.87885802469135632</v>
       </c>
       <c r="G203" s="30"/>
       <c r="H203" s="30">
@@ -10971,7 +11007,7 @@
       </c>
       <c r="F204" s="15">
         <f t="shared" si="26"/>
-        <v>0.88190184049079867</v>
+        <v>0.88117283950617109</v>
       </c>
       <c r="G204" s="30"/>
       <c r="H204" s="30">
@@ -11000,7 +11036,7 @@
       </c>
       <c r="F205" s="15">
         <f t="shared" si="26"/>
-        <v>0.8918711656441729</v>
+        <v>0.89120370370370194</v>
       </c>
       <c r="G205" s="30"/>
       <c r="H205" s="30">
@@ -11029,7 +11065,7 @@
       </c>
       <c r="F206" s="15">
         <f t="shared" si="26"/>
-        <v>0.89417177914110546</v>
+        <v>0.89351851851851671</v>
       </c>
       <c r="G206" s="30"/>
       <c r="H206" s="30">
@@ -11058,7 +11094,7 @@
       </c>
       <c r="F207" s="15">
         <f t="shared" si="26"/>
-        <v>0.90720858895705636</v>
+        <v>0.906635802469134</v>
       </c>
       <c r="G207" s="30"/>
       <c r="H207" s="30">
@@ -11087,7 +11123,7 @@
       </c>
       <c r="F208" s="15">
         <f t="shared" si="26"/>
-        <v>0.90950920245398892</v>
+        <v>0.90895061728394877</v>
       </c>
       <c r="G208" s="30"/>
       <c r="H208" s="30">
@@ -11116,7 +11152,7 @@
       </c>
       <c r="F209" s="15">
         <f t="shared" si="26"/>
-        <v>0.91564417177914226</v>
+        <v>0.91512345679012164</v>
       </c>
       <c r="G209" s="30"/>
       <c r="H209" s="30">
@@ -11145,7 +11181,7 @@
       </c>
       <c r="F210" s="15">
         <f t="shared" si="26"/>
-        <v>0.91794478527607481</v>
+        <v>0.91743827160493641</v>
       </c>
       <c r="G210" s="30"/>
       <c r="H210" s="30">
@@ -11173,7 +11209,7 @@
       <c r="E211" s="27"/>
       <c r="F211" s="29">
         <f t="shared" si="26"/>
-        <v>0.91794478527607481</v>
+        <v>0.91743827160493641</v>
       </c>
       <c r="G211" s="41" t="str">
         <f>IF(COUNTA(G212:G214)=COUNTA(B212:B214), "COMPLETE", "")</f>
@@ -11205,7 +11241,7 @@
       </c>
       <c r="F212" s="15">
         <f t="shared" si="26"/>
-        <v>0.91871165644171904</v>
+        <v>0.91820987654320796</v>
       </c>
       <c r="G212" s="30"/>
       <c r="H212" s="30">
@@ -11234,7 +11270,7 @@
       </c>
       <c r="F213" s="15">
         <f t="shared" si="26"/>
-        <v>0.92791411042944905</v>
+        <v>0.92746913580246726</v>
       </c>
       <c r="G213" s="30"/>
       <c r="H213" s="30">
@@ -11263,7 +11299,7 @@
       </c>
       <c r="F214" s="15">
         <f t="shared" si="26"/>
-        <v>0.9302147239263816</v>
+        <v>0.92978395061728203</v>
       </c>
       <c r="G214" s="30"/>
       <c r="H214" s="30">
@@ -11292,7 +11328,7 @@
       </c>
       <c r="F215" s="15">
         <f t="shared" si="26"/>
-        <v>0.93558282208589083</v>
+        <v>0.93518518518518323</v>
       </c>
       <c r="G215" s="30"/>
       <c r="H215" s="30">
@@ -11321,7 +11357,7 @@
       </c>
       <c r="F216" s="15">
         <f t="shared" si="26"/>
-        <v>0.93788343558282339</v>
+        <v>0.937499999999998</v>
       </c>
       <c r="G216" s="30"/>
       <c r="H216" s="30">
@@ -11349,7 +11385,7 @@
       <c r="E217" s="27"/>
       <c r="F217" s="29">
         <f t="shared" si="26"/>
-        <v>0.93788343558282339</v>
+        <v>0.937499999999998</v>
       </c>
       <c r="G217" s="41" t="str">
         <f>IF(COUNTA(G218:G220)=COUNTA(B218:B220), "COMPLETE", "")</f>
@@ -11381,7 +11417,7 @@
       </c>
       <c r="F218" s="15">
         <f t="shared" si="26"/>
-        <v>0.94478527607362095</v>
+        <v>0.94444444444444242</v>
       </c>
       <c r="G218" s="30"/>
       <c r="H218" s="30">
@@ -11410,7 +11446,7 @@
       </c>
       <c r="F219" s="15">
         <f t="shared" si="26"/>
-        <v>0.94708588957055351</v>
+        <v>0.94675925925925719</v>
       </c>
       <c r="G219" s="30"/>
       <c r="H219" s="30">
@@ -11439,7 +11475,7 @@
       </c>
       <c r="F220" s="15">
         <f t="shared" si="26"/>
-        <v>0.94938650306748606</v>
+        <v>0.94907407407407196</v>
       </c>
       <c r="G220" s="30"/>
       <c r="H220" s="30">
@@ -11468,7 +11504,7 @@
       </c>
       <c r="F221" s="15">
         <f t="shared" si="26"/>
-        <v>0.95782208588957196</v>
+        <v>0.9575617283950596</v>
       </c>
       <c r="G221" s="30"/>
       <c r="H221" s="30">
@@ -11497,7 +11533,7 @@
       </c>
       <c r="F222" s="15">
         <f t="shared" si="26"/>
-        <v>0.96012269938650452</v>
+        <v>0.95987654320987437</v>
       </c>
       <c r="G222" s="30"/>
       <c r="H222" s="30">
@@ -11526,7 +11562,7 @@
       </c>
       <c r="F223" s="15">
         <f t="shared" si="26"/>
-        <v>0.96088957055214874</v>
+        <v>0.96064814814814592</v>
       </c>
       <c r="G223" s="30"/>
       <c r="H223" s="30">
@@ -11534,11 +11570,11 @@
       </c>
       <c r="I223" s="9">
         <f t="shared" si="27"/>
-        <v>573</v>
+        <v>565</v>
       </c>
       <c r="J223" s="38">
         <f t="shared" si="28"/>
-        <v>9.5500000000000007</v>
+        <v>9.4166666666666661</v>
       </c>
     </row>
     <row r="224" spans="1:10" ht="21" thickBot="1">
@@ -11554,7 +11590,7 @@
       <c r="E224" s="27"/>
       <c r="F224" s="29">
         <f t="shared" si="26"/>
-        <v>0.96088957055214874</v>
+        <v>0.96064814814814592</v>
       </c>
       <c r="G224" s="41" t="str">
         <f>IF(COUNTA(G225:G225)=COUNTA(B225:B225), "COMPLETE", "")</f>
@@ -11585,7 +11621,7 @@
       </c>
       <c r="F225" s="15">
         <f t="shared" si="26"/>
-        <v>0.96165644171779296</v>
+        <v>0.96141975308641747</v>
       </c>
       <c r="G225" s="30"/>
       <c r="H225" s="30">
@@ -11613,7 +11649,7 @@
       <c r="E226" s="27"/>
       <c r="F226" s="29">
         <f t="shared" si="26"/>
-        <v>0.96165644171779296</v>
+        <v>0.96141975308641747</v>
       </c>
       <c r="G226" s="41" t="str">
         <f>IF(COUNTA(G227:G229)=COUNTA(B227:B229), "COMPLETE", "")</f>
@@ -11645,7 +11681,7 @@
       </c>
       <c r="F227" s="15">
         <f t="shared" si="26"/>
-        <v>0.96395705521472552</v>
+        <v>0.96373456790123224</v>
       </c>
       <c r="G227" s="30"/>
       <c r="H227" s="30">
@@ -11674,7 +11710,7 @@
       </c>
       <c r="F228" s="15">
         <f t="shared" si="26"/>
-        <v>0.96625766871165808</v>
+        <v>0.96604938271604701</v>
       </c>
       <c r="G228" s="30"/>
       <c r="H228" s="30">
@@ -11703,7 +11739,7 @@
       </c>
       <c r="F229" s="15">
         <f t="shared" si="26"/>
-        <v>0.96855828220859064</v>
+        <v>0.96836419753086178</v>
       </c>
       <c r="G229" s="30"/>
       <c r="H229" s="30">
@@ -11732,7 +11768,7 @@
       </c>
       <c r="F230" s="15">
         <f t="shared" si="26"/>
-        <v>0.97085889570552319</v>
+        <v>0.97067901234567655</v>
       </c>
       <c r="G230" s="30"/>
       <c r="H230" s="30">
@@ -11761,7 +11797,7 @@
       </c>
       <c r="F231" s="15">
         <f t="shared" si="26"/>
-        <v>0.97315950920245575</v>
+        <v>0.97299382716049132</v>
       </c>
       <c r="G231" s="30"/>
       <c r="H231" s="30">
@@ -11790,7 +11826,7 @@
       </c>
       <c r="F232" s="15">
         <f t="shared" si="26"/>
-        <v>0.97546012269938831</v>
+        <v>0.97530864197530609</v>
       </c>
       <c r="G232" s="30"/>
       <c r="H232" s="30">
@@ -11819,7 +11855,7 @@
       </c>
       <c r="F233" s="15">
         <f t="shared" si="26"/>
-        <v>0.97776073619632087</v>
+        <v>0.97762345679012086</v>
       </c>
       <c r="G233" s="30"/>
       <c r="H233" s="30">
@@ -11848,7 +11884,7 @@
       </c>
       <c r="F234" s="15">
         <f t="shared" si="26"/>
-        <v>0.98006134969325343</v>
+        <v>0.97993827160493563</v>
       </c>
       <c r="G234" s="30"/>
       <c r="H234" s="30">
@@ -11877,7 +11913,7 @@
       </c>
       <c r="F235" s="15">
         <f t="shared" si="26"/>
-        <v>0.98236196319018598</v>
+        <v>0.9822530864197504</v>
       </c>
       <c r="G235" s="30"/>
       <c r="H235" s="30">
@@ -11906,7 +11942,7 @@
       </c>
       <c r="F236" s="15">
         <f t="shared" si="26"/>
-        <v>0.98466257668711854</v>
+        <v>0.98456790123456517</v>
       </c>
       <c r="G236" s="30"/>
       <c r="H236" s="30">
@@ -11935,7 +11971,7 @@
       </c>
       <c r="F237" s="15">
         <f t="shared" si="26"/>
-        <v>0.9869631901840511</v>
+        <v>0.98688271604937994</v>
       </c>
       <c r="G237" s="30"/>
       <c r="H237" s="30">
@@ -11964,7 +12000,7 @@
       </c>
       <c r="F238" s="15">
         <f t="shared" si="26"/>
-        <v>0.98926380368098366</v>
+        <v>0.98919753086419471</v>
       </c>
       <c r="G238" s="30"/>
       <c r="H238" s="30">
@@ -11993,7 +12029,7 @@
       </c>
       <c r="F239" s="15">
         <f t="shared" si="26"/>
-        <v>0.99156441717791621</v>
+        <v>0.99151234567900948</v>
       </c>
       <c r="G239" s="30"/>
       <c r="H239" s="30">
@@ -12022,7 +12058,7 @@
       </c>
       <c r="F240" s="15">
         <f t="shared" si="26"/>
-        <v>0.99386503067484877</v>
+        <v>0.99382716049382425</v>
       </c>
       <c r="G240" s="30"/>
       <c r="H240" s="30">
@@ -12051,7 +12087,7 @@
       </c>
       <c r="F241" s="15">
         <f t="shared" si="26"/>
-        <v>0.99616564417178133</v>
+        <v>0.99614197530863902</v>
       </c>
       <c r="G241" s="30"/>
       <c r="H241" s="30">
@@ -12080,7 +12116,7 @@
       </c>
       <c r="F242" s="15">
         <f t="shared" si="26"/>
-        <v>0.99846625766871389</v>
+        <v>0.99845679012345379</v>
       </c>
       <c r="G242" s="30"/>
       <c r="H242" s="30">
@@ -12109,7 +12145,7 @@
       </c>
       <c r="F243" s="15">
         <f t="shared" si="26"/>
-        <v>1.0000000000000022</v>
+        <v>0.999999999999997</v>
       </c>
       <c r="G243" s="30"/>
       <c r="H243" s="30">
@@ -12130,7 +12166,7 @@
       </c>
       <c r="C245" s="40">
         <f>SUM(C4:C244)</f>
-        <v>1304</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="246" spans="2:10" ht="15.75" thickTop="1">
@@ -12139,7 +12175,7 @@
       </c>
       <c r="C246" s="12">
         <f>+C245/60</f>
-        <v>21.733333333333334</v>
+        <v>21.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Section 12: Audio completed
</commit_message>
<xml_diff>
--- a/Unity Certification Course (Udemy) - Video Listing.xlsx
+++ b/Unity Certification Course (Udemy) - Video Listing.xlsx
@@ -4807,8 +4807,8 @@
   <dimension ref="A1:K246"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G160" sqref="G160"/>
+      <pane ySplit="3" topLeftCell="A166" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G172" sqref="G172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -4836,7 +4836,7 @@
       </c>
       <c r="F1" s="34">
         <f>SUMIF(G4:G244, "&gt;0", C4:C244)</f>
-        <v>886</v>
+        <v>965</v>
       </c>
       <c r="G1" s="35">
         <f>+C245</f>
@@ -4844,7 +4844,7 @@
       </c>
       <c r="H1" s="36">
         <f>+F1/G1</f>
-        <v>0.68364197530864201</v>
+        <v>0.7445987654320988</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -9695,7 +9695,7 @@
       </c>
       <c r="G159" s="41" t="str">
         <f>IF(COUNTA(G160:G162)=COUNTA(B160:B162), "COMPLETE", "")</f>
-        <v/>
+        <v>COMPLETE</v>
       </c>
       <c r="I159" s="9" t="str">
         <f t="shared" si="19"/>
@@ -9756,7 +9756,9 @@
         <f t="shared" si="18"/>
         <v>0.69058641975308555</v>
       </c>
-      <c r="G161" s="30"/>
+      <c r="G161" s="30">
+        <v>42796</v>
+      </c>
       <c r="H161" s="30">
         <v>42796</v>
       </c>
@@ -9785,7 +9787,9 @@
         <f t="shared" si="18"/>
         <v>0.69290123456790031</v>
       </c>
-      <c r="G162" s="30"/>
+      <c r="G162" s="30">
+        <v>42796</v>
+      </c>
       <c r="H162" s="30">
         <v>42796</v>
       </c>
@@ -9814,7 +9818,9 @@
         <f t="shared" si="18"/>
         <v>0.7006172839506164</v>
       </c>
-      <c r="G163" s="30"/>
+      <c r="G163" s="30">
+        <v>42796</v>
+      </c>
       <c r="H163" s="30">
         <v>42796</v>
       </c>
@@ -9843,7 +9849,9 @@
         <f t="shared" si="18"/>
         <v>0.70293209876543117</v>
       </c>
-      <c r="G164" s="30"/>
+      <c r="G164" s="30">
+        <v>42796</v>
+      </c>
       <c r="H164" s="30">
         <v>42796</v>
       </c>
@@ -9872,7 +9880,9 @@
         <f t="shared" si="18"/>
         <v>0.70987654320987559</v>
       </c>
-      <c r="G165" s="30"/>
+      <c r="G165" s="30">
+        <v>42796</v>
+      </c>
       <c r="H165" s="30">
         <v>42796</v>
       </c>
@@ -9901,7 +9911,9 @@
         <f t="shared" si="18"/>
         <v>0.71219135802469036</v>
       </c>
-      <c r="G166" s="30"/>
+      <c r="G166" s="30">
+        <v>42796</v>
+      </c>
       <c r="H166" s="30">
         <v>42796</v>
       </c>
@@ -9930,7 +9942,9 @@
         <f t="shared" si="18"/>
         <v>0.72145061728394966</v>
       </c>
-      <c r="G167" s="30"/>
+      <c r="G167" s="30">
+        <v>42796</v>
+      </c>
       <c r="H167" s="30">
         <v>42796</v>
       </c>
@@ -9959,7 +9973,9 @@
         <f t="shared" si="18"/>
         <v>0.72376543209876443</v>
       </c>
-      <c r="G168" s="30"/>
+      <c r="G168" s="30">
+        <v>42796</v>
+      </c>
       <c r="H168" s="30">
         <v>42796</v>
       </c>
@@ -9988,7 +10004,9 @@
         <f t="shared" si="18"/>
         <v>0.73225308641975206</v>
       </c>
-      <c r="G169" s="30"/>
+      <c r="G169" s="30">
+        <v>42796</v>
+      </c>
       <c r="H169" s="30">
         <v>42796</v>
       </c>
@@ -10017,7 +10035,9 @@
         <f t="shared" si="18"/>
         <v>0.73456790123456683</v>
       </c>
-      <c r="G170" s="30"/>
+      <c r="G170" s="30">
+        <v>42796</v>
+      </c>
       <c r="H170" s="30">
         <v>42796</v>
       </c>
@@ -10046,7 +10066,9 @@
         <f t="shared" si="18"/>
         <v>0.74228395061728292</v>
       </c>
-      <c r="G171" s="30"/>
+      <c r="G171" s="30">
+        <v>42796</v>
+      </c>
       <c r="H171" s="30">
         <v>42796</v>
       </c>
@@ -10075,7 +10097,9 @@
         <f t="shared" si="18"/>
         <v>0.74459876543209769</v>
       </c>
-      <c r="G172" s="30"/>
+      <c r="G172" s="30">
+        <v>42796</v>
+      </c>
       <c r="H172" s="30">
         <v>42796</v>
       </c>
@@ -11363,13 +11387,13 @@
       <c r="H216" s="30">
         <v>42796</v>
       </c>
-      <c r="I216" s="9" t="str">
+      <c r="I216" s="9">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-      <c r="J216" s="38" t="str">
+        <v>535</v>
+      </c>
+      <c r="J216" s="38">
         <f t="shared" si="28"/>
-        <v/>
+        <v>8.9166666666666661</v>
       </c>
     </row>
     <row r="217" spans="1:10" ht="21" thickBot="1">
@@ -11421,7 +11445,7 @@
       </c>
       <c r="G218" s="30"/>
       <c r="H218" s="30">
-        <v>42796</v>
+        <v>42797</v>
       </c>
       <c r="I218" s="9" t="str">
         <f t="shared" si="27"/>
@@ -11450,7 +11474,7 @@
       </c>
       <c r="G219" s="30"/>
       <c r="H219" s="30">
-        <v>42796</v>
+        <v>42797</v>
       </c>
       <c r="I219" s="9" t="str">
         <f t="shared" si="27"/>
@@ -11479,7 +11503,7 @@
       </c>
       <c r="G220" s="30"/>
       <c r="H220" s="30">
-        <v>42796</v>
+        <v>42797</v>
       </c>
       <c r="I220" s="9" t="str">
         <f t="shared" si="27"/>
@@ -11508,7 +11532,7 @@
       </c>
       <c r="G221" s="30"/>
       <c r="H221" s="30">
-        <v>42796</v>
+        <v>42797</v>
       </c>
       <c r="I221" s="9" t="str">
         <f t="shared" si="27"/>
@@ -11537,7 +11561,7 @@
       </c>
       <c r="G222" s="30"/>
       <c r="H222" s="30">
-        <v>42796</v>
+        <v>42797</v>
       </c>
       <c r="I222" s="9" t="str">
         <f t="shared" si="27"/>
@@ -11566,15 +11590,15 @@
       </c>
       <c r="G223" s="30"/>
       <c r="H223" s="30">
-        <v>42796</v>
-      </c>
-      <c r="I223" s="9">
+        <v>42797</v>
+      </c>
+      <c r="I223" s="9" t="str">
         <f t="shared" si="27"/>
-        <v>565</v>
-      </c>
-      <c r="J223" s="38">
+        <v/>
+      </c>
+      <c r="J223" s="38" t="str">
         <f t="shared" si="28"/>
-        <v>9.4166666666666661</v>
+        <v/>
       </c>
     </row>
     <row r="224" spans="1:10" ht="21" thickBot="1">
@@ -12153,11 +12177,11 @@
       </c>
       <c r="I243" s="9">
         <f t="shared" si="27"/>
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="J243" s="38">
         <f t="shared" si="28"/>
-        <v>0.85</v>
+        <v>1.35</v>
       </c>
     </row>
     <row r="245" spans="2:10" ht="15.75" thickBot="1">

</xml_diff>

<commit_message>
Section 13: Animations completed
</commit_message>
<xml_diff>
--- a/Unity Certification Course (Udemy) - Video Listing.xlsx
+++ b/Unity Certification Course (Udemy) - Video Listing.xlsx
@@ -2625,7 +2625,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1189" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1191" uniqueCount="367">
   <si>
     <t>VIDEO NAME</t>
   </si>
@@ -3941,6 +3941,12 @@
   </si>
   <si>
     <t>skipped-no time</t>
+  </si>
+  <si>
+    <t>animations weren't working since he used a different avatar from the original</t>
+  </si>
+  <si>
+    <t>watched videos and took quizzes but didn’t follow along in unity</t>
   </si>
 </sst>
 </file>
@@ -4807,8 +4813,8 @@
   <dimension ref="A1:K246"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A166" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G172" sqref="G172"/>
+      <pane ySplit="3" topLeftCell="A171" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K190" sqref="K190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -4836,7 +4842,7 @@
       </c>
       <c r="F1" s="34">
         <f>SUMIF(G4:G244, "&gt;0", C4:C244)</f>
-        <v>965</v>
+        <v>1090</v>
       </c>
       <c r="G1" s="35">
         <f>+C245</f>
@@ -4844,7 +4850,7 @@
       </c>
       <c r="H1" s="36">
         <f>+F1/G1</f>
-        <v>0.7445987654320988</v>
+        <v>0.84104938271604934</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -10129,7 +10135,7 @@
       </c>
       <c r="G173" s="41" t="str">
         <f>IF(COUNTA(G174:G176)=COUNTA(B174:B176), "COMPLETE", "")</f>
-        <v/>
+        <v>COMPLETE</v>
       </c>
       <c r="I173" s="9" t="str">
         <f t="shared" si="19"/>
@@ -10159,7 +10165,9 @@
         <f t="shared" si="18"/>
         <v>0.74537037037036924</v>
       </c>
-      <c r="G174" s="30"/>
+      <c r="G174" s="30">
+        <v>42796</v>
+      </c>
       <c r="H174" s="30">
         <v>42796</v>
       </c>
@@ -10188,7 +10196,9 @@
         <f t="shared" si="18"/>
         <v>0.75231481481481366</v>
       </c>
-      <c r="G175" s="30"/>
+      <c r="G175" s="30">
+        <v>42796</v>
+      </c>
       <c r="H175" s="30">
         <v>42796</v>
       </c>
@@ -10217,7 +10227,9 @@
         <f t="shared" si="18"/>
         <v>0.75462962962962843</v>
       </c>
-      <c r="G176" s="30"/>
+      <c r="G176" s="30">
+        <v>42796</v>
+      </c>
       <c r="H176" s="30">
         <v>42796</v>
       </c>
@@ -10230,7 +10242,7 @@
         <v/>
       </c>
     </row>
-    <row r="177" spans="2:10" outlineLevel="1">
+    <row r="177" spans="2:11" outlineLevel="1">
       <c r="B177" s="18" t="s">
         <v>216</v>
       </c>
@@ -10246,7 +10258,9 @@
         <f t="shared" si="18"/>
         <v>0.76003086419752963</v>
       </c>
-      <c r="G177" s="30"/>
+      <c r="G177" s="30">
+        <v>42796</v>
+      </c>
       <c r="H177" s="30">
         <v>42796</v>
       </c>
@@ -10259,7 +10273,7 @@
         <v/>
       </c>
     </row>
-    <row r="178" spans="2:10" outlineLevel="1">
+    <row r="178" spans="2:11" outlineLevel="1">
       <c r="B178" s="18" t="s">
         <v>217</v>
       </c>
@@ -10275,7 +10289,9 @@
         <f t="shared" si="18"/>
         <v>0.7623456790123444</v>
       </c>
-      <c r="G178" s="30"/>
+      <c r="G178" s="30">
+        <v>42796</v>
+      </c>
       <c r="H178" s="30">
         <v>42796</v>
       </c>
@@ -10288,7 +10304,7 @@
         <v/>
       </c>
     </row>
-    <row r="179" spans="2:10" outlineLevel="1">
+    <row r="179" spans="2:11" outlineLevel="1">
       <c r="B179" s="18" t="s">
         <v>218</v>
       </c>
@@ -10304,7 +10320,9 @@
         <f t="shared" si="18"/>
         <v>0.76929012345678882</v>
       </c>
-      <c r="G179" s="30"/>
+      <c r="G179" s="30">
+        <v>42796</v>
+      </c>
       <c r="H179" s="30">
         <v>42796</v>
       </c>
@@ -10317,7 +10335,7 @@
         <v/>
       </c>
     </row>
-    <row r="180" spans="2:10" outlineLevel="1">
+    <row r="180" spans="2:11" outlineLevel="1">
       <c r="B180" s="18" t="s">
         <v>219</v>
       </c>
@@ -10333,7 +10351,9 @@
         <f t="shared" si="18"/>
         <v>0.77160493827160359</v>
       </c>
-      <c r="G180" s="30"/>
+      <c r="G180" s="30">
+        <v>42796</v>
+      </c>
       <c r="H180" s="30">
         <v>42796</v>
       </c>
@@ -10346,7 +10366,7 @@
         <v/>
       </c>
     </row>
-    <row r="181" spans="2:10" outlineLevel="1">
+    <row r="181" spans="2:11" outlineLevel="1">
       <c r="B181" s="18" t="s">
         <v>220</v>
       </c>
@@ -10362,7 +10382,9 @@
         <f t="shared" si="18"/>
         <v>0.78009259259259123</v>
       </c>
-      <c r="G181" s="30"/>
+      <c r="G181" s="30">
+        <v>42796</v>
+      </c>
       <c r="H181" s="30">
         <v>42796</v>
       </c>
@@ -10375,7 +10397,7 @@
         <v/>
       </c>
     </row>
-    <row r="182" spans="2:10" outlineLevel="1">
+    <row r="182" spans="2:11" outlineLevel="1">
       <c r="B182" s="18" t="s">
         <v>221</v>
       </c>
@@ -10391,7 +10413,9 @@
         <f t="shared" si="18"/>
         <v>0.782407407407406</v>
       </c>
-      <c r="G182" s="30"/>
+      <c r="G182" s="30">
+        <v>42796</v>
+      </c>
       <c r="H182" s="30">
         <v>42796</v>
       </c>
@@ -10404,7 +10428,7 @@
         <v/>
       </c>
     </row>
-    <row r="183" spans="2:10" outlineLevel="1">
+    <row r="183" spans="2:11" outlineLevel="1">
       <c r="B183" s="18" t="s">
         <v>222</v>
       </c>
@@ -10420,7 +10444,9 @@
         <f t="shared" si="18"/>
         <v>0.79012345679012208</v>
       </c>
-      <c r="G183" s="30"/>
+      <c r="G183" s="30">
+        <v>42796</v>
+      </c>
       <c r="H183" s="30">
         <v>42796</v>
       </c>
@@ -10433,7 +10459,7 @@
         <v/>
       </c>
     </row>
-    <row r="184" spans="2:10" outlineLevel="1">
+    <row r="184" spans="2:11" outlineLevel="1">
       <c r="B184" s="18" t="s">
         <v>223</v>
       </c>
@@ -10449,7 +10475,9 @@
         <f t="shared" si="18"/>
         <v>0.79243827160493685</v>
       </c>
-      <c r="G184" s="30"/>
+      <c r="G184" s="30">
+        <v>42796</v>
+      </c>
       <c r="H184" s="30">
         <v>42796</v>
       </c>
@@ -10462,7 +10490,7 @@
         <v/>
       </c>
     </row>
-    <row r="185" spans="2:10" outlineLevel="1">
+    <row r="185" spans="2:11" outlineLevel="1">
       <c r="B185" s="18" t="s">
         <v>224</v>
       </c>
@@ -10478,7 +10506,9 @@
         <f t="shared" si="18"/>
         <v>0.80015432098765293</v>
       </c>
-      <c r="G185" s="30"/>
+      <c r="G185" s="30">
+        <v>42796</v>
+      </c>
       <c r="H185" s="30">
         <v>42796</v>
       </c>
@@ -10491,7 +10521,7 @@
         <v/>
       </c>
     </row>
-    <row r="186" spans="2:10" outlineLevel="1">
+    <row r="186" spans="2:11" outlineLevel="1">
       <c r="B186" s="18" t="s">
         <v>225</v>
       </c>
@@ -10507,7 +10537,9 @@
         <f t="shared" si="18"/>
         <v>0.8024691358024677</v>
       </c>
-      <c r="G186" s="30"/>
+      <c r="G186" s="30">
+        <v>42796</v>
+      </c>
       <c r="H186" s="30">
         <v>42796</v>
       </c>
@@ -10520,7 +10552,7 @@
         <v/>
       </c>
     </row>
-    <row r="187" spans="2:10" outlineLevel="1">
+    <row r="187" spans="2:11" outlineLevel="1">
       <c r="B187" s="18" t="s">
         <v>226</v>
       </c>
@@ -10536,7 +10568,9 @@
         <f t="shared" si="18"/>
         <v>0.80941358024691212</v>
       </c>
-      <c r="G187" s="30"/>
+      <c r="G187" s="30">
+        <v>42796</v>
+      </c>
       <c r="H187" s="30">
         <v>42796</v>
       </c>
@@ -10549,7 +10583,7 @@
         <v/>
       </c>
     </row>
-    <row r="188" spans="2:10" outlineLevel="1">
+    <row r="188" spans="2:11" outlineLevel="1">
       <c r="B188" s="18" t="s">
         <v>228</v>
       </c>
@@ -10565,7 +10599,9 @@
         <f t="shared" si="18"/>
         <v>0.82098765432098619</v>
       </c>
-      <c r="G188" s="30"/>
+      <c r="G188" s="30">
+        <v>42796</v>
+      </c>
       <c r="H188" s="30">
         <v>42796</v>
       </c>
@@ -10577,8 +10613,11 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-    </row>
-    <row r="189" spans="2:10" outlineLevel="1">
+      <c r="K188" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="189" spans="2:11" outlineLevel="1">
       <c r="B189" s="18" t="s">
         <v>229</v>
       </c>
@@ -10594,7 +10633,9 @@
         <f t="shared" si="18"/>
         <v>0.82330246913580096</v>
       </c>
-      <c r="G189" s="30"/>
+      <c r="G189" s="30">
+        <v>42796</v>
+      </c>
       <c r="H189" s="30">
         <v>42796</v>
       </c>
@@ -10606,8 +10647,11 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-    </row>
-    <row r="190" spans="2:10" outlineLevel="1">
+      <c r="K189" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="190" spans="2:11" outlineLevel="1">
       <c r="B190" s="18" t="s">
         <v>230</v>
       </c>
@@ -10623,7 +10667,9 @@
         <f t="shared" si="18"/>
         <v>0.83101851851851705</v>
       </c>
-      <c r="G190" s="30"/>
+      <c r="G190" s="30">
+        <v>42796</v>
+      </c>
       <c r="H190" s="30">
         <v>42796</v>
       </c>
@@ -10636,7 +10682,7 @@
         <v/>
       </c>
     </row>
-    <row r="191" spans="2:10" outlineLevel="1">
+    <row r="191" spans="2:11" outlineLevel="1">
       <c r="B191" s="18" t="s">
         <v>231</v>
       </c>
@@ -10652,7 +10698,9 @@
         <f t="shared" si="18"/>
         <v>0.83873456790123313</v>
       </c>
-      <c r="G191" s="30"/>
+      <c r="G191" s="30">
+        <v>42796</v>
+      </c>
       <c r="H191" s="30">
         <v>42796</v>
       </c>
@@ -10665,7 +10713,7 @@
         <v/>
       </c>
     </row>
-    <row r="192" spans="2:10" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="192" spans="2:11" ht="15.75" outlineLevel="1" thickBot="1">
       <c r="B192" s="18" t="s">
         <v>232</v>
       </c>
@@ -10681,7 +10729,9 @@
         <f t="shared" si="18"/>
         <v>0.8410493827160479</v>
       </c>
-      <c r="G192" s="30"/>
+      <c r="G192" s="30">
+        <v>42796</v>
+      </c>
       <c r="H192" s="30">
         <v>42796</v>
       </c>

</xml_diff>